<commit_message>
First version of the notebook section analysing FR and BE flat glass ind
</commit_message>
<xml_diff>
--- a/RawData/BE_RawData_VPython.xlsx
+++ b/RawData/BE_RawData_VPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\01_MFA_GlassIndustry\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC929BED-3D5E-4ADA-A25D-13B01948F047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C816E028-7B6F-49E7-9D90-EDB00E27013E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2340" windowWidth="19650" windowHeight="13860" firstSheet="1" activeTab="2" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="19650" windowHeight="13860" firstSheet="1" activeTab="2" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="stock" sheetId="17" r:id="rId1"/>

</xml_diff>

<commit_message>
Update of the notebook
</commit_message>
<xml_diff>
--- a/RawData/BE_RawData_VPython.xlsx
+++ b/RawData/BE_RawData_VPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\01_MFA_GlassIndustry\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA01E2E-57FD-4D47-A2F6-E569B2C1FE67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD863548-2EC2-44F1-BE77-8063B08D4D91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14715" yWindow="600" windowWidth="13125" windowHeight="15600" activeTab="4" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="1560" yWindow="600" windowWidth="13125" windowHeight="15600" activeTab="2" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="stock" sheetId="17" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="workforce" sheetId="12" r:id="rId6"/>
     <sheet name="FlatGlassInd_GlassInd" sheetId="9" r:id="rId7"/>
     <sheet name="RawMat_GlassInd_ABS" sheetId="8" r:id="rId8"/>
+    <sheet name="Population" sheetId="18" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -98,20 +99,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{6CB673EF-88CC-4E56-B1B1-C6E3AF0F71A3}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>OECD Data:
-https://data.oecd.org/pop/population.htm</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -149,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{CB10E512-9D92-4056-8D71-70FED6AEAF5A}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{FFF54F8C-42A9-47BE-BA11-9E812209664C}">
       <text>
         <r>
           <rPr>
@@ -159,7 +146,7 @@
             <family val="2"/>
           </rPr>
           <t>Calculus:
-The average glass thickness is estimated at around 9mm (2x4.5mm). See import and export data.</t>
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
         </r>
       </text>
     </comment>
@@ -217,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{B0549D22-40AF-4A9B-BC10-59F1A1DA741A}">
+    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{60B3FC3B-6055-4E4D-A231-0144E09060ED}">
       <text>
         <r>
           <rPr>
@@ -249,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{3AB7B9F4-1590-4E25-963A-3EEBB02E5941}">
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{E0DC0D82-D9DF-4BD7-A33A-0B50C35C698C}">
       <text>
         <r>
           <rPr>
@@ -281,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{8586E7D9-7F4A-4B48-972D-768919F368A7}">
+    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{B57BEA95-24D2-439E-BC94-D0202114BFEE}">
       <text>
         <r>
           <rPr>
@@ -313,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{75E5B087-15A0-4DB8-B8D8-856FF537EA0C}">
+    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{A59076F1-9E80-4441-8ED6-27E14722081D}">
       <text>
         <r>
           <rPr>
@@ -345,7 +332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D31" authorId="0" shapeId="0" xr:uid="{376886D1-6D5A-467E-9033-63DFF7BA93B0}">
+    <comment ref="D31" authorId="0" shapeId="0" xr:uid="{B620C8B3-D3D8-4F2E-88AC-49DF22C49163}">
       <text>
         <r>
           <rPr>
@@ -377,7 +364,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D32" authorId="0" shapeId="0" xr:uid="{5B921C9C-51EC-4917-9542-EE039474F33F}">
+    <comment ref="D32" authorId="0" shapeId="0" xr:uid="{7E6E91CE-5369-400E-84C8-87ED4166867E}">
       <text>
         <r>
           <rPr>
@@ -409,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D33" authorId="0" shapeId="0" xr:uid="{2EA2EA32-C939-41E3-9248-F6CEBE552185}">
+    <comment ref="D33" authorId="0" shapeId="0" xr:uid="{2D1186D9-881A-4F20-ADD8-CAB038072AAF}">
       <text>
         <r>
           <rPr>
@@ -441,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D34" authorId="0" shapeId="0" xr:uid="{52EC176A-4EC2-4307-8540-903D7511A2D4}">
+    <comment ref="D34" authorId="0" shapeId="0" xr:uid="{BDD39EC5-4C5E-4627-87B4-F83CB68E978D}">
       <text>
         <r>
           <rPr>
@@ -473,7 +460,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D35" authorId="0" shapeId="0" xr:uid="{0B98A300-9C08-477B-870C-A793F16760D7}">
+    <comment ref="D35" authorId="0" shapeId="0" xr:uid="{7346AC3A-B774-4FA8-9EBF-CE05F08EDFFE}">
       <text>
         <r>
           <rPr>
@@ -505,7 +492,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D36" authorId="0" shapeId="0" xr:uid="{95089EA7-7EBC-40A9-83AE-E66B33A7AD1A}">
+    <comment ref="D36" authorId="0" shapeId="0" xr:uid="{0E5ECCE1-5919-440F-A307-EE158D9FFF1C}">
       <text>
         <r>
           <rPr>
@@ -537,7 +524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="0" shapeId="0" xr:uid="{DF169E54-D977-4967-AD90-4D9B83D1B805}">
+    <comment ref="D37" authorId="0" shapeId="0" xr:uid="{04708709-9149-4AFB-87D7-A0DC6741F7FF}">
       <text>
         <r>
           <rPr>
@@ -569,7 +556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D38" authorId="0" shapeId="0" xr:uid="{C765E89B-6216-4860-855E-249CCB8A9E07}">
+    <comment ref="D38" authorId="0" shapeId="0" xr:uid="{3A282B50-09F3-4DC7-A499-5C5D00AEBFD8}">
       <text>
         <r>
           <rPr>
@@ -890,6 +877,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D53" authorId="0" shapeId="0" xr:uid="{6A92BE97-88FC-4CBB-B413-32D583A1F26B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B54" authorId="0" shapeId="0" xr:uid="{70DC3473-3447-4719-A1C0-D766A356D209}">
       <text>
         <r>
@@ -928,6 +929,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D54" authorId="0" shapeId="0" xr:uid="{89B94B09-4861-415E-8D8A-28B885190E83}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B55" authorId="0" shapeId="0" xr:uid="{25B8BFD1-FF8E-4695-8D3B-1F04E0873F8E}">
       <text>
         <r>
@@ -966,6 +981,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D55" authorId="0" shapeId="0" xr:uid="{715DB3FF-CBCE-47CD-A5B2-0CD675635A46}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B56" authorId="0" shapeId="0" xr:uid="{52F33A99-0D0B-4259-A80A-327EB7C19980}">
       <text>
         <r>
@@ -1004,6 +1033,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D56" authorId="0" shapeId="0" xr:uid="{846263C8-56D9-4393-B76F-9A928C23206C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B57" authorId="0" shapeId="0" xr:uid="{EED5E0C0-7039-4EBE-BEB7-731F4AB2D310}">
       <text>
         <r>
@@ -1042,6 +1085,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D57" authorId="0" shapeId="0" xr:uid="{BC86A0BE-7408-48E0-82BF-1E3CAA79D938}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B58" authorId="0" shapeId="0" xr:uid="{CB926990-D23D-40E6-A836-F3281928C622}">
       <text>
         <r>
@@ -1080,6 +1137,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D58" authorId="0" shapeId="0" xr:uid="{16080463-D40F-4F27-ACCA-FE286755C62E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B59" authorId="0" shapeId="0" xr:uid="{21748B7F-E41B-4370-85B5-FD2F0867FD43}">
       <text>
         <r>
@@ -1118,6 +1189,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D59" authorId="0" shapeId="0" xr:uid="{10BBC027-87B2-455D-AA4A-AD6760E6C1B7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B60" authorId="0" shapeId="0" xr:uid="{1464D249-C5A4-4870-8379-8C910C5FE3F7}">
       <text>
         <r>
@@ -1156,6 +1241,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D60" authorId="0" shapeId="0" xr:uid="{9A908036-2EA6-4224-A7B0-618BD55B22D6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B61" authorId="0" shapeId="0" xr:uid="{692A6916-772E-44DF-93C7-154E663D6B1D}">
       <text>
         <r>
@@ -1194,6 +1293,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D61" authorId="0" shapeId="0" xr:uid="{8019F4D1-CBCB-436E-AE65-388D66D48CC8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B62" authorId="0" shapeId="0" xr:uid="{A427882F-7797-4C83-9895-E1E70694B621}">
       <text>
         <r>
@@ -1232,6 +1345,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D62" authorId="0" shapeId="0" xr:uid="{AD00789E-24A2-4D4E-A56F-9878A4E01297}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B63" authorId="0" shapeId="0" xr:uid="{6019CF96-E4D4-4629-9B21-41F7B13F7B2D}">
       <text>
         <r>
@@ -1270,6 +1397,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D63" authorId="0" shapeId="0" xr:uid="{9001778D-D759-4E8B-BABE-B035C57C369F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B64" authorId="0" shapeId="0" xr:uid="{4B691808-64DE-4924-8E47-8CD5B4CC7882}">
       <text>
         <r>
@@ -1308,6 +1449,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D64" authorId="0" shapeId="0" xr:uid="{67AA3941-F7CA-43FA-9FB3-5255635E4178}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B65" authorId="0" shapeId="0" xr:uid="{FA00D844-B0AE-4966-9F18-BFBA78DC5A62}">
       <text>
         <r>
@@ -1346,6 +1501,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D65" authorId="0" shapeId="0" xr:uid="{807209AC-AED6-4500-8472-8777BC975CD6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B66" authorId="0" shapeId="0" xr:uid="{17454C45-7D9B-4EDD-8DBD-CD55B2F7B504}">
       <text>
         <r>
@@ -1384,6 +1553,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D66" authorId="0" shapeId="0" xr:uid="{4DAD81AD-7C93-413A-B8B7-40A0E8082195}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B67" authorId="0" shapeId="0" xr:uid="{05FD7DBA-81F6-4F23-B05F-C0076288518C}">
       <text>
         <r>
@@ -1422,6 +1605,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D67" authorId="0" shapeId="0" xr:uid="{D4BC2686-428A-4DF0-AE46-1D97F886885D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B68" authorId="0" shapeId="0" xr:uid="{C5AFDD2F-1913-40D4-B64F-8130C27890FC}">
       <text>
         <r>
@@ -1460,6 +1657,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D68" authorId="0" shapeId="0" xr:uid="{633C8BF9-74C6-4B80-B62E-A776BB70F9B7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B69" authorId="0" shapeId="0" xr:uid="{1DE707F9-BA17-469A-B287-9FA7BCE6C68D}">
       <text>
         <r>
@@ -1498,6 +1709,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D69" authorId="0" shapeId="0" xr:uid="{B425D0E3-C24A-4DA6-A957-E805ED32E0DC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C70" authorId="0" shapeId="0" xr:uid="{07FEBA3F-E56B-4F52-9259-160F498D974F}">
       <text>
         <r>
@@ -1523,6 +1748,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D70" authorId="0" shapeId="0" xr:uid="{87343770-E23F-494D-8192-C68B314BBD6E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C72" authorId="0" shapeId="0" xr:uid="{3424DAA8-F20D-40BB-A352-F67F4359BB28}">
       <text>
         <r>
@@ -1548,6 +1787,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D72" authorId="0" shapeId="0" xr:uid="{EB56DE9E-C15D-4F46-A9CD-7AAA263DD66F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C73" authorId="0" shapeId="0" xr:uid="{FFA7925B-2D83-4554-B348-1952BA9F2C5C}">
       <text>
         <r>
@@ -1573,6 +1826,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D73" authorId="0" shapeId="0" xr:uid="{ED37C69B-56F5-406A-A826-4175E81CD614}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C74" authorId="0" shapeId="0" xr:uid="{6DF2A1C8-5094-42B5-9407-778F607797C1}">
       <text>
         <r>
@@ -1598,6 +1865,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D74" authorId="0" shapeId="0" xr:uid="{9D55D874-1F2E-4728-B689-5C4A6224ED55}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C75" authorId="0" shapeId="0" xr:uid="{DF8387AD-0A51-4B49-A79D-71F86211F715}">
       <text>
         <r>
@@ -1623,6 +1904,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D75" authorId="0" shapeId="0" xr:uid="{D349DE63-84AB-480E-A446-357989BE3B82}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C76" authorId="0" shapeId="0" xr:uid="{E64FB881-E1E5-4712-9ABE-8C10751806EB}">
       <text>
         <r>
@@ -1645,6 +1940,20 @@
           <t xml:space="preserve">
 PRODCOM Database, Eurostat.
 Code: 23121330 - Multiple-walled insulating units of glass</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D76" authorId="0" shapeId="0" xr:uid="{862C43D0-02DD-4A37-B58A-478A6F1202A3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculus:
+The average glass thickness is estimated at around 10mm (2x5mm). See import and export data.</t>
         </r>
       </text>
     </comment>
@@ -1829,6 +2138,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{929BAED1-A62F-4FF8-AE58-2DA3C0FE5EA5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>L'industrie du verre en 1969, Rapport annuel, Fédération de l'industrie du verre, 1970</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B21" authorId="0" shapeId="0" xr:uid="{67FAEDF3-3681-4F76-AD42-0A15DFB5230E}">
       <text>
         <r>
@@ -6493,8 +6815,46 @@
 </comments>
 </file>
 
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>jean</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{D03E3816-3F82-47F1-A999-231153AAE251}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>OECD Data:
+https://data.oecd.org/pop/population.htm</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{A8064E29-81F2-45FE-8AD8-04497206EDD5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>La population de la Belgique, 1974, Société Belge de Démographie, Brussels : C.I.C.R.E.D.
+http://www.cicred.org/Eng/Publications/pdf/c-c4.pdf</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>glazing, '000 m²</t>
   </si>
@@ -6565,8 +6925,7 @@
     <t>VAB/person/year, "000 F</t>
   </si>
   <si>
-    <t>BE, 
-"000 persons</t>
+    <t>Population, x1000</t>
   </si>
 </sst>
 </file>
@@ -6579,7 +6938,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6622,6 +6981,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -6690,7 +7055,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -6822,6 +7187,14 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7693,606 +8066,446 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEEDA53-7E46-4237-BFF2-D54E4EED559A}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
     <sheetView zoomScale="88" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H58" sqref="H58"/>
+      <selection pane="bottomRight" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="16384" width="13.5703125" style="6"/>
+    <col min="3" max="16384" width="13.5703125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>1945</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2"/>
-    </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>1946</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3"/>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>1947</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4"/>
-    </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>1948</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5"/>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>1949</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6"/>
-    </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>1950</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7"/>
-    </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>1951</v>
       </c>
       <c r="B8" s="8"/>
-      <c r="C8"/>
-    </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>1952</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9"/>
-    </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>1953</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10"/>
-    </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>1954</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11"/>
-    </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>1955</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12"/>
-    </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>1956</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13"/>
-    </row>
-    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>1957</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14"/>
-    </row>
-    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>1958</v>
       </c>
       <c r="B15" s="8"/>
-      <c r="C15"/>
-    </row>
-    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>1959</v>
       </c>
       <c r="B16" s="8"/>
-      <c r="C16"/>
-    </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>1960</v>
       </c>
       <c r="B17" s="8"/>
-      <c r="C17" s="8">
-        <v>9153</v>
-      </c>
-      <c r="D17" s="39"/>
-    </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="39"/>
+    </row>
+    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>1961</v>
       </c>
       <c r="B18" s="8"/>
-      <c r="C18" s="8">
-        <v>9184</v>
-      </c>
-      <c r="D18" s="39"/>
-    </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="39"/>
+    </row>
+    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>1962</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="8">
-        <v>9221</v>
-      </c>
-      <c r="D19" s="39"/>
-    </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="39"/>
+    </row>
+    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>1963</v>
       </c>
       <c r="B20" s="8"/>
-      <c r="C20" s="8">
-        <v>9290</v>
-      </c>
-      <c r="D20" s="39"/>
-    </row>
-    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="39"/>
+    </row>
+    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>1964</v>
       </c>
       <c r="B21" s="8"/>
-      <c r="C21" s="8">
-        <v>9378</v>
-      </c>
-      <c r="D21" s="39"/>
-    </row>
-    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="39"/>
+    </row>
+    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>1965</v>
       </c>
       <c r="B22" s="8"/>
-      <c r="C22" s="8">
-        <v>9464</v>
-      </c>
-      <c r="D22" s="39"/>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="39"/>
+    </row>
+    <row r="23" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
         <v>1966</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="8">
-        <v>9528</v>
-      </c>
-      <c r="D23" s="39"/>
-    </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="39"/>
+    </row>
+    <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>1967</v>
       </c>
       <c r="B24" s="8"/>
-      <c r="C24" s="8">
-        <v>9581</v>
-      </c>
-      <c r="D24" s="39"/>
-    </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="39"/>
+    </row>
+    <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>1968</v>
       </c>
       <c r="B25" s="8"/>
-      <c r="C25" s="8">
-        <v>9619</v>
-      </c>
-      <c r="D25" s="39"/>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="39"/>
+    </row>
+    <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <v>1969</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="8">
-        <v>9646</v>
-      </c>
-      <c r="D26" s="39"/>
-    </row>
-    <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="39"/>
+    </row>
+    <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
         <v>1970</v>
       </c>
       <c r="B27" s="8"/>
-      <c r="C27" s="8">
-        <v>9656</v>
-      </c>
-      <c r="D27" s="39"/>
-    </row>
-    <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="39"/>
+    </row>
+    <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>1971</v>
       </c>
       <c r="B28" s="8"/>
-      <c r="C28" s="8">
-        <v>9673</v>
-      </c>
-      <c r="D28" s="39"/>
-    </row>
-    <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="39"/>
+    </row>
+    <row r="29" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>1972</v>
       </c>
       <c r="B29" s="8"/>
-      <c r="C29" s="8">
-        <v>9711</v>
-      </c>
-      <c r="D29" s="39"/>
-    </row>
-    <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="39"/>
+    </row>
+    <row r="30" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>1973</v>
       </c>
       <c r="B30" s="8"/>
-      <c r="C30" s="8">
-        <v>9742</v>
-      </c>
-      <c r="D30" s="39"/>
-    </row>
-    <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="39"/>
+    </row>
+    <row r="31" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>1974</v>
       </c>
       <c r="B31" s="8"/>
-      <c r="C31" s="8">
-        <v>9772</v>
-      </c>
-      <c r="D31" s="39"/>
-    </row>
-    <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="39"/>
+    </row>
+    <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>1975</v>
       </c>
-      <c r="C32" s="8">
-        <v>9801</v>
-      </c>
-      <c r="D32" s="39"/>
-    </row>
-    <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="39"/>
+    </row>
+    <row r="33" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>1976</v>
       </c>
-      <c r="C33" s="8">
-        <v>9818</v>
-      </c>
-      <c r="D33" s="39"/>
-    </row>
-    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="39"/>
+    </row>
+    <row r="34" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>1977</v>
       </c>
-      <c r="C34" s="8">
-        <v>9830</v>
-      </c>
-      <c r="D34" s="39"/>
-    </row>
-    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="39"/>
+    </row>
+    <row r="35" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
         <v>1978</v>
       </c>
-      <c r="C35" s="8">
-        <v>9840</v>
-      </c>
-      <c r="D35" s="39"/>
-    </row>
-    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="39"/>
+    </row>
+    <row r="36" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>1979</v>
       </c>
       <c r="B36" s="8"/>
-      <c r="C36" s="8">
-        <v>9848</v>
-      </c>
-      <c r="D36" s="39"/>
-    </row>
-    <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="39"/>
+    </row>
+    <row r="37" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
         <v>1980</v>
       </c>
       <c r="B37" s="8"/>
-      <c r="C37" s="8">
-        <v>9859</v>
-      </c>
-      <c r="D37" s="39"/>
-    </row>
-    <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="39"/>
+    </row>
+    <row r="38" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>1981</v>
       </c>
       <c r="B38" s="8"/>
-      <c r="C38" s="8">
-        <v>9859</v>
-      </c>
-      <c r="D38" s="39"/>
-    </row>
-    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="39"/>
+    </row>
+    <row r="39" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
         <v>1982</v>
       </c>
       <c r="B39" s="8"/>
-      <c r="C39" s="8">
-        <v>9856</v>
-      </c>
-      <c r="D39" s="39"/>
-    </row>
-    <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="39"/>
+    </row>
+    <row r="40" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
         <v>1983</v>
       </c>
       <c r="B40" s="8"/>
-      <c r="C40" s="8">
-        <v>9856</v>
-      </c>
-      <c r="D40" s="39"/>
-    </row>
-    <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="39"/>
+    </row>
+    <row r="41" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
         <v>1984</v>
       </c>
       <c r="B41" s="8"/>
-      <c r="C41" s="8">
-        <v>9855</v>
-      </c>
-      <c r="D41" s="39"/>
-    </row>
-    <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="39"/>
+    </row>
+    <row r="42" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
         <v>1985</v>
       </c>
       <c r="B42" s="8"/>
-      <c r="C42" s="8">
-        <v>9858</v>
-      </c>
-      <c r="D42" s="39"/>
-    </row>
-    <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="39"/>
+    </row>
+    <row r="43" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="14">
         <v>1986</v>
       </c>
       <c r="B43" s="8"/>
-      <c r="C43" s="8">
-        <v>9862</v>
-      </c>
-      <c r="D43" s="39"/>
-    </row>
-    <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="39"/>
+    </row>
+    <row r="44" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14">
         <v>1987</v>
       </c>
       <c r="B44" s="8"/>
-      <c r="C44" s="8">
-        <v>9870</v>
-      </c>
-      <c r="D44" s="39"/>
-    </row>
-    <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="39"/>
+    </row>
+    <row r="45" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
         <v>1988</v>
       </c>
       <c r="B45" s="8"/>
-      <c r="C45" s="8">
-        <v>9902</v>
-      </c>
-      <c r="D45" s="39"/>
-    </row>
-    <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="39"/>
+    </row>
+    <row r="46" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
         <v>1989</v>
       </c>
       <c r="B46" s="8"/>
-      <c r="C46" s="8">
-        <v>9938</v>
-      </c>
-      <c r="D46" s="39"/>
-    </row>
-    <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="39"/>
+    </row>
+    <row r="47" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14">
         <v>1990</v>
       </c>
       <c r="B47" s="8"/>
-      <c r="C47" s="8">
-        <v>9967</v>
-      </c>
-      <c r="D47" s="39"/>
-    </row>
-    <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="39"/>
+    </row>
+    <row r="48" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
         <v>1991</v>
       </c>
       <c r="B48" s="8"/>
-      <c r="C48" s="8">
-        <v>10004</v>
-      </c>
-      <c r="D48" s="39"/>
-    </row>
-    <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="39"/>
+    </row>
+    <row r="49" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14">
         <v>1992</v>
       </c>
       <c r="B49" s="8"/>
-      <c r="C49" s="8">
-        <v>10045</v>
-      </c>
-      <c r="D49" s="39"/>
-    </row>
-    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="39"/>
+    </row>
+    <row r="50" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14">
         <v>1993</v>
       </c>
       <c r="B50" s="8"/>
-      <c r="C50" s="8">
-        <v>10084</v>
-      </c>
-      <c r="D50" s="39"/>
-    </row>
-    <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="39"/>
+    </row>
+    <row r="51" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14">
         <v>1994</v>
       </c>
       <c r="B51" s="8"/>
-      <c r="C51" s="8">
-        <v>10116</v>
-      </c>
-      <c r="D51" s="39"/>
-    </row>
-    <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="39"/>
+    </row>
+    <row r="52" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14">
         <v>1995</v>
       </c>
       <c r="B52" s="8"/>
-      <c r="C52" s="8">
-        <v>10137</v>
-      </c>
-      <c r="D52" s="39"/>
-    </row>
-    <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="39"/>
+    </row>
+    <row r="53" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14">
         <v>1996</v>
       </c>
       <c r="B53" s="8"/>
-      <c r="C53" s="8">
-        <v>10157</v>
-      </c>
-      <c r="D53" s="39"/>
-    </row>
-    <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="39"/>
+    </row>
+    <row r="54" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14">
         <v>1997</v>
       </c>
       <c r="B54" s="8"/>
-      <c r="C54" s="8">
-        <v>10181</v>
-      </c>
-      <c r="D54" s="39"/>
-    </row>
-    <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="39"/>
+    </row>
+    <row r="55" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14">
         <v>1998</v>
       </c>
       <c r="B55" s="8"/>
-      <c r="C55" s="8">
-        <v>10203</v>
-      </c>
-      <c r="D55" s="39"/>
-    </row>
-    <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="39"/>
+    </row>
+    <row r="56" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14">
         <v>1999</v>
       </c>
       <c r="B56" s="8"/>
-      <c r="C56" s="8">
-        <v>10226</v>
-      </c>
-      <c r="D56" s="39"/>
-    </row>
-    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="39"/>
+    </row>
+    <row r="57" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14">
         <v>2000</v>
       </c>
       <c r="B57" s="8"/>
-      <c r="C57" s="8">
-        <v>10251</v>
-      </c>
-      <c r="D57" s="39"/>
-    </row>
-    <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="39"/>
+    </row>
+    <row r="58" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14">
         <v>2001</v>
       </c>
       <c r="B58" s="8"/>
-      <c r="C58" s="8">
-        <v>10287</v>
-      </c>
-      <c r="D58" s="39"/>
-    </row>
-    <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="39"/>
+    </row>
+    <row r="59" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14">
         <v>2002</v>
       </c>
       <c r="B59" s="8"/>
-      <c r="C59" s="8">
-        <v>10333</v>
-      </c>
-      <c r="D59" s="39"/>
-    </row>
-    <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="39"/>
+    </row>
+    <row r="60" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14">
         <v>2003</v>
       </c>
       <c r="B60" s="8"/>
-      <c r="C60" s="8">
-        <v>10376</v>
-      </c>
-      <c r="D60" s="39"/>
-    </row>
-    <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="39"/>
+    </row>
+    <row r="61" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14">
         <v>2004</v>
       </c>
       <c r="B61" s="8"/>
-      <c r="C61" s="8">
-        <v>10421</v>
-      </c>
-      <c r="D61" s="39"/>
-    </row>
-    <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="39"/>
+    </row>
+    <row r="62" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14">
         <v>2005</v>
       </c>
       <c r="B62" s="8"/>
-      <c r="C62" s="8">
-        <v>10479</v>
-      </c>
-      <c r="D62" s="39"/>
-    </row>
-    <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="39"/>
+    </row>
+    <row r="63" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14">
         <v>2006</v>
       </c>
       <c r="B63" s="8"/>
-      <c r="C63" s="8">
-        <v>10548</v>
-      </c>
-      <c r="D63" s="39"/>
-    </row>
-    <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="39"/>
+    </row>
+    <row r="64" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14">
         <v>2007</v>
       </c>
@@ -8300,12 +8513,9 @@
         <f>2500*(1.2*1.2)</f>
         <v>3600</v>
       </c>
-      <c r="C64" s="8">
-        <v>10626</v>
-      </c>
-      <c r="D64" s="39"/>
-    </row>
-    <row r="65" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="39"/>
+    </row>
+    <row r="65" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14">
         <v>2008</v>
       </c>
@@ -8313,12 +8523,9 @@
         <f>2500*(1.2*1.2)</f>
         <v>3600</v>
       </c>
-      <c r="C65" s="8">
-        <v>10710</v>
-      </c>
-      <c r="D65" s="39"/>
-    </row>
-    <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="39"/>
+    </row>
+    <row r="66" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14">
         <v>2009</v>
       </c>
@@ -8326,12 +8533,9 @@
         <f>5450*(1.2*1.2)</f>
         <v>7848</v>
       </c>
-      <c r="C66" s="8">
-        <v>10796</v>
-      </c>
-      <c r="D66" s="39"/>
-    </row>
-    <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="39"/>
+    </row>
+    <row r="67" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14">
         <v>2010</v>
       </c>
@@ -8339,12 +8543,9 @@
         <f>2450*(1.2*1.2)</f>
         <v>3528</v>
       </c>
-      <c r="C67" s="8">
-        <v>10896</v>
-      </c>
-      <c r="D67" s="39"/>
-    </row>
-    <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="39"/>
+    </row>
+    <row r="68" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14">
         <v>2011</v>
       </c>
@@ -8352,12 +8553,9 @@
         <f>2470*(1.2*1.2)</f>
         <v>3556.7999999999997</v>
       </c>
-      <c r="C68" s="8">
-        <v>10994</v>
-      </c>
-      <c r="D68" s="39"/>
-    </row>
-    <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C68" s="39"/>
+    </row>
+    <row r="69" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14">
         <v>2012</v>
       </c>
@@ -8365,90 +8563,67 @@
         <f>2430*(1.2*1.2)</f>
         <v>3499.2</v>
       </c>
-      <c r="C69" s="8">
-        <v>11068</v>
-      </c>
-      <c r="D69" s="39"/>
-    </row>
-    <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="39"/>
+    </row>
+    <row r="70" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="14">
         <v>2013</v>
       </c>
       <c r="B70" s="8"/>
-      <c r="C70" s="8">
-        <v>11125</v>
-      </c>
-      <c r="D70" s="39"/>
-    </row>
-    <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="39"/>
+    </row>
+    <row r="71" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="14">
         <v>2014</v>
       </c>
       <c r="B71" s="8"/>
-      <c r="C71" s="8">
-        <v>11180</v>
-      </c>
-      <c r="D71" s="39"/>
-    </row>
-    <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C71" s="39"/>
+    </row>
+    <row r="72" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="14">
         <v>2015</v>
       </c>
       <c r="B72" s="8"/>
-      <c r="C72" s="8">
-        <v>11238</v>
-      </c>
-      <c r="D72" s="39"/>
-    </row>
-    <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="39"/>
+    </row>
+    <row r="73" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="14">
         <v>2016</v>
       </c>
       <c r="B73" s="8"/>
-      <c r="C73" s="8">
-        <v>11295</v>
-      </c>
-      <c r="D73" s="39"/>
-    </row>
-    <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="39"/>
+    </row>
+    <row r="74" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="14">
         <v>2017</v>
       </c>
       <c r="B74" s="8"/>
-      <c r="C74" s="8">
-        <v>11349</v>
-      </c>
-      <c r="D74" s="39"/>
-    </row>
-    <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="39"/>
+    </row>
+    <row r="75" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="14">
         <v>2018</v>
       </c>
-      <c r="C75" s="8">
-        <v>11404</v>
-      </c>
-      <c r="D75" s="39"/>
-    </row>
-    <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="39"/>
+    </row>
+    <row r="76" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="14">
         <v>2019</v>
       </c>
-      <c r="C76"/>
-    </row>
-    <row r="77" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="14">
         <v>2020</v>
       </c>
-      <c r="C77"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
       <c r="B79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="13"/>
       <c r="B80" s="8"/>
     </row>
@@ -8495,11 +8670,11 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8545,7 +8720,8 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="17">
+        <f>C4*0.0091*2.5</f>
         <v>0</v>
       </c>
     </row>
@@ -8568,6 +8744,14 @@
       <c r="B7" s="9">
         <v>206.25</v>
       </c>
+      <c r="C7" s="45">
+        <f>0.0015*C27</f>
+        <v>4.0513333333333339</v>
+      </c>
+      <c r="D7" s="8">
+        <f>C7*2.5*0.009</f>
+        <v>9.1155E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -8723,8 +8907,8 @@
         <v>2700.8888888888891</v>
       </c>
       <c r="D27" s="37">
-        <f>C27*11*2.5/1000</f>
-        <v>74.274444444444455</v>
+        <f t="shared" ref="D27:D38" si="0">C27*0.0091*2.5</f>
+        <v>61.445222222222228</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8739,8 +8923,8 @@
         <v>2646.8888888888891</v>
       </c>
       <c r="D28" s="37">
-        <f t="shared" ref="D28:D39" si="0">C28*10*2.5/1000</f>
-        <v>66.172222222222217</v>
+        <f t="shared" si="0"/>
+        <v>60.216722222222231</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8756,7 +8940,7 @@
       </c>
       <c r="D29" s="37">
         <f t="shared" si="0"/>
-        <v>66.847222222222214</v>
+        <v>60.830972222222229</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8772,7 +8956,7 @@
       </c>
       <c r="D30" s="37">
         <f t="shared" si="0"/>
-        <v>69.547222222222217</v>
+        <v>63.287972222222237</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8788,7 +8972,7 @@
       </c>
       <c r="D31" s="37">
         <f t="shared" si="0"/>
-        <v>75.847222222222214</v>
+        <v>69.020972222222227</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8804,7 +8988,7 @@
       </c>
       <c r="D32" s="37">
         <f t="shared" si="0"/>
-        <v>80.909722222222214</v>
+        <v>73.627847222222229</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8820,7 +9004,7 @@
       </c>
       <c r="D33" s="37">
         <f t="shared" si="0"/>
-        <v>87.547222222222217</v>
+        <v>79.667972222222232</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8836,7 +9020,7 @@
       </c>
       <c r="D34" s="37">
         <f t="shared" si="0"/>
-        <v>93.397222222222226</v>
+        <v>84.991472222222228</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8852,7 +9036,7 @@
       </c>
       <c r="D35" s="37">
         <f t="shared" si="0"/>
-        <v>93.847222222222214</v>
+        <v>85.400972222222236</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8868,7 +9052,7 @@
       </c>
       <c r="D36" s="37">
         <f t="shared" si="0"/>
-        <v>93.847222222222214</v>
+        <v>85.400972222222236</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8884,7 +9068,7 @@
       </c>
       <c r="D37" s="37">
         <f t="shared" si="0"/>
-        <v>108.47222222222221</v>
+        <v>98.709722222222226</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8900,7 +9084,7 @@
       </c>
       <c r="D38" s="37">
         <f t="shared" si="0"/>
-        <v>99.472222222222214</v>
+        <v>90.519722222222242</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8915,8 +9099,8 @@
         <v>3798.8888888888891</v>
       </c>
       <c r="D39" s="37">
-        <f t="shared" si="0"/>
-        <v>94.972222222222214</v>
+        <f>C39*0.0091*2.5</f>
+        <v>86.424722222222229</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9033,8 +9217,8 @@
         <v>4607.9660000000003</v>
       </c>
       <c r="D52" s="37">
-        <f>C52*10*2.5/1000</f>
-        <v>115.19915</v>
+        <f>C52*0.009*2.5</f>
+        <v>103.67923500000001</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9048,8 +9232,8 @@
         <v>4074.3609999999999</v>
       </c>
       <c r="D53" s="37">
-        <f t="shared" ref="D53:D75" si="1">C53*9*2.5/1000</f>
-        <v>91.673122499999991</v>
+        <f t="shared" ref="D53:D70" si="1">C53*0.009*2.5</f>
+        <v>91.673122499999977</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9124,7 +9308,7 @@
       </c>
       <c r="D58" s="37">
         <f t="shared" si="1"/>
-        <v>122.16782249999999</v>
+        <v>122.16782249999997</v>
       </c>
     </row>
     <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9154,7 +9338,7 @@
       </c>
       <c r="D60" s="37">
         <f t="shared" si="1"/>
-        <v>109.18077749999999</v>
+        <v>109.1807775</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9169,7 +9353,7 @@
       </c>
       <c r="D61" s="37">
         <f t="shared" si="1"/>
-        <v>112.40689500000001</v>
+        <v>112.40689499999999</v>
       </c>
     </row>
     <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9199,7 +9383,7 @@
       </c>
       <c r="D63" s="37">
         <f t="shared" si="1"/>
-        <v>121.39703999999999</v>
+        <v>121.39703999999998</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9214,7 +9398,7 @@
       </c>
       <c r="D64" s="37">
         <f t="shared" si="1"/>
-        <v>124.40108249999999</v>
+        <v>124.40108249999997</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9229,7 +9413,7 @@
       </c>
       <c r="D65" s="37">
         <f t="shared" si="1"/>
-        <v>116.46132750000001</v>
+        <v>116.4613275</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9259,7 +9443,7 @@
       </c>
       <c r="D67" s="37">
         <f t="shared" si="1"/>
-        <v>100.98346500000001</v>
+        <v>100.983465</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9301,7 +9485,7 @@
       </c>
       <c r="D70" s="37">
         <f t="shared" si="1"/>
-        <v>91.352430000000012</v>
+        <v>91.352429999999998</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9319,8 +9503,8 @@
         <v>3889.6</v>
       </c>
       <c r="D72" s="37">
-        <f t="shared" si="1"/>
-        <v>87.516000000000005</v>
+        <f t="shared" ref="D72:D76" si="2">C72*0.009*2.5</f>
+        <v>87.515999999999991</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9332,8 +9516,8 @@
         <v>3946.616</v>
       </c>
       <c r="D73" s="37">
-        <f t="shared" si="1"/>
-        <v>88.798860000000005</v>
+        <f t="shared" si="2"/>
+        <v>88.798859999999991</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9345,8 +9529,8 @@
         <v>4192.6400000000003</v>
       </c>
       <c r="D74" s="37">
-        <f t="shared" si="1"/>
-        <v>94.334400000000002</v>
+        <f t="shared" si="2"/>
+        <v>94.334399999999988</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9358,8 +9542,8 @@
         <v>4124.6139999999996</v>
       </c>
       <c r="D75" s="37">
-        <f t="shared" si="1"/>
-        <v>92.803815</v>
+        <f t="shared" si="2"/>
+        <v>92.803814999999986</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9371,8 +9555,8 @@
         <v>4349.4560000000001</v>
       </c>
       <c r="D76" s="37">
-        <f>C76*10*2.5/1000</f>
-        <v>108.73639999999999</v>
+        <f t="shared" si="2"/>
+        <v>97.862759999999994</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9425,13 +9609,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FB653F-4255-4899-B7D6-3BA7509BAA32}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView zoomScale="72" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9646,7 +9830,9 @@
       <c r="G15" s="8">
         <v>0.02</v>
       </c>
-      <c r="H15" s="8"/>
+      <c r="H15" s="8">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
@@ -9683,7 +9869,9 @@
       <c r="G17" s="37">
         <v>0</v>
       </c>
-      <c r="H17" s="37"/>
+      <c r="H17" s="37">
+        <v>0</v>
+      </c>
       <c r="I17" s="23"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -9709,7 +9897,9 @@
       <c r="G18" s="37">
         <v>0</v>
       </c>
-      <c r="H18" s="37"/>
+      <c r="H18" s="37">
+        <v>0</v>
+      </c>
       <c r="I18" s="23"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -9735,7 +9925,9 @@
       <c r="G19" s="37">
         <v>0</v>
       </c>
-      <c r="H19" s="37"/>
+      <c r="H19" s="37">
+        <v>0</v>
+      </c>
       <c r="I19" s="23"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -9761,7 +9953,9 @@
       <c r="G20" s="37">
         <v>0</v>
       </c>
-      <c r="H20" s="37"/>
+      <c r="H20" s="37">
+        <v>0</v>
+      </c>
       <c r="I20" s="23"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -9786,7 +9980,9 @@
       <c r="G21" s="37">
         <v>0</v>
       </c>
-      <c r="H21" s="37"/>
+      <c r="H21" s="37">
+        <v>0</v>
+      </c>
       <c r="I21" s="23"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -9811,7 +10007,9 @@
       <c r="G22" s="37">
         <v>0</v>
       </c>
-      <c r="H22" s="37"/>
+      <c r="H22" s="37">
+        <v>0</v>
+      </c>
       <c r="I22" s="23"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -9837,7 +10035,9 @@
       <c r="G23" s="37">
         <v>0</v>
       </c>
-      <c r="H23" s="37"/>
+      <c r="H23" s="37">
+        <v>0</v>
+      </c>
       <c r="I23" s="23"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -9863,7 +10063,9 @@
       <c r="G24" s="37">
         <v>0</v>
       </c>
-      <c r="H24" s="37"/>
+      <c r="H24" s="37">
+        <v>0</v>
+      </c>
       <c r="I24" s="23"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -9889,7 +10091,9 @@
       <c r="G25" s="37">
         <v>0</v>
       </c>
-      <c r="H25" s="37"/>
+      <c r="H25" s="37">
+        <v>0</v>
+      </c>
       <c r="I25" s="23"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -9915,7 +10119,9 @@
       <c r="G26" s="37">
         <v>0</v>
       </c>
-      <c r="H26" s="37"/>
+      <c r="H26" s="37">
+        <v>0</v>
+      </c>
       <c r="I26" s="23"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -9941,7 +10147,9 @@
       <c r="G27" s="37">
         <v>0</v>
       </c>
-      <c r="H27" s="37"/>
+      <c r="H27" s="37">
+        <v>0</v>
+      </c>
       <c r="I27" s="23"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -9949,7 +10157,7 @@
         <v>1971</v>
       </c>
       <c r="B28" s="37">
-        <f>SUM(C28:G28)</f>
+        <f t="shared" ref="B28:B38" si="0">SUM(C28:G28)</f>
         <v>35</v>
       </c>
       <c r="C28" s="37">
@@ -9967,7 +10175,9 @@
       <c r="G28" s="37">
         <v>0</v>
       </c>
-      <c r="H28" s="37"/>
+      <c r="H28" s="37">
+        <v>0</v>
+      </c>
       <c r="I28" s="23"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -9975,7 +10185,7 @@
         <v>1972</v>
       </c>
       <c r="B29" s="37">
-        <f>SUM(C29:G29)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="C29" s="37">
@@ -9993,7 +10203,9 @@
       <c r="G29" s="37">
         <v>0</v>
       </c>
-      <c r="H29" s="37"/>
+      <c r="H29" s="37">
+        <v>0</v>
+      </c>
       <c r="I29" s="23"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -10001,7 +10213,7 @@
         <v>1973</v>
       </c>
       <c r="B30" s="37">
-        <f>SUM(C30:G30)</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C30" s="37">
@@ -10019,7 +10231,9 @@
       <c r="G30" s="37">
         <v>0</v>
       </c>
-      <c r="H30" s="37"/>
+      <c r="H30" s="37">
+        <v>0</v>
+      </c>
       <c r="I30" s="23"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -10027,7 +10241,7 @@
         <v>1974</v>
       </c>
       <c r="B31" s="37">
-        <f>SUM(C31:G31)</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="C31" s="37">
@@ -10045,7 +10259,9 @@
       <c r="G31" s="37">
         <v>0</v>
       </c>
-      <c r="H31" s="37"/>
+      <c r="H31" s="37">
+        <v>0</v>
+      </c>
       <c r="I31" s="23"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -10053,7 +10269,7 @@
         <v>1975</v>
       </c>
       <c r="B32" s="37">
-        <f>SUM(C32:G32)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="C32" s="37">
@@ -10072,7 +10288,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="37">
-        <f>G32/2.5/0.009</f>
+        <f t="shared" ref="H32:H50" si="1">G32/2.5/0.009</f>
         <v>44.44444444444445</v>
       </c>
       <c r="I32" s="23"/>
@@ -10082,7 +10298,7 @@
         <v>1976</v>
       </c>
       <c r="B33" s="37">
-        <f>SUM(C33:G33)</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="C33" s="37">
@@ -10101,7 +10317,7 @@
         <v>2</v>
       </c>
       <c r="H33" s="37">
-        <f>G33/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>88.8888888888889</v>
       </c>
       <c r="I33" s="23"/>
@@ -10111,7 +10327,7 @@
         <v>1977</v>
       </c>
       <c r="B34" s="37">
-        <f>SUM(C34:G34)</f>
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="C34" s="37">
@@ -10130,7 +10346,7 @@
         <v>3</v>
       </c>
       <c r="H34" s="37">
-        <f>G34/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>133.33333333333334</v>
       </c>
       <c r="I34" s="23"/>
@@ -10140,7 +10356,7 @@
         <v>1978</v>
       </c>
       <c r="B35" s="37">
-        <f>SUM(C35:G35)</f>
+        <f t="shared" si="0"/>
         <v>88</v>
       </c>
       <c r="C35" s="37">
@@ -10159,7 +10375,7 @@
         <v>5</v>
       </c>
       <c r="H35" s="37">
-        <f>G35/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>222.22222222222223</v>
       </c>
       <c r="I35" s="23"/>
@@ -10169,7 +10385,7 @@
         <v>1979</v>
       </c>
       <c r="B36" s="37">
-        <f>SUM(C36:G36)</f>
+        <f t="shared" si="0"/>
         <v>108</v>
       </c>
       <c r="C36" s="37">
@@ -10188,7 +10404,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="37">
-        <f>G36/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>266.66666666666669</v>
       </c>
       <c r="I36" s="23"/>
@@ -10198,7 +10414,7 @@
         <v>1980</v>
       </c>
       <c r="B37" s="37">
-        <f>SUM(C37:G37)</f>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="C37" s="37">
@@ -10217,7 +10433,7 @@
         <v>9</v>
       </c>
       <c r="H37" s="37">
-        <f>G37/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>400.00000000000006</v>
       </c>
       <c r="I37" s="23"/>
@@ -10227,7 +10443,7 @@
         <v>1981</v>
       </c>
       <c r="B38" s="37">
-        <f>SUM(C38:G38)</f>
+        <f t="shared" si="0"/>
         <v>123</v>
       </c>
       <c r="C38" s="37">
@@ -10246,7 +10462,7 @@
         <v>8</v>
       </c>
       <c r="H38" s="37">
-        <f>G38/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>355.5555555555556</v>
       </c>
       <c r="I38" s="23"/>
@@ -10275,7 +10491,7 @@
         <v>7</v>
       </c>
       <c r="H39" s="37">
-        <f>G39/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>311.11111111111114</v>
       </c>
       <c r="I39" s="23"/>
@@ -10304,7 +10520,7 @@
         <v>6</v>
       </c>
       <c r="H40" s="37">
-        <f>G40/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>266.66666666666669</v>
       </c>
       <c r="I40" s="23"/>
@@ -10333,7 +10549,7 @@
         <v>5</v>
       </c>
       <c r="H41" s="37">
-        <f>G41/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>222.22222222222223</v>
       </c>
       <c r="I41" s="23"/>
@@ -10362,7 +10578,7 @@
         <v>5</v>
       </c>
       <c r="H42" s="37">
-        <f>G42/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>222.22222222222223</v>
       </c>
       <c r="I42" s="23"/>
@@ -10391,7 +10607,7 @@
         <v>6</v>
       </c>
       <c r="H43" s="37">
-        <f>G43/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>266.66666666666669</v>
       </c>
       <c r="I43" s="23"/>
@@ -10401,7 +10617,7 @@
         <v>1987</v>
       </c>
       <c r="B44" s="37">
-        <f>SUM(C44:G44)</f>
+        <f t="shared" ref="B44:B50" si="2">SUM(C44:G44)</f>
         <v>191</v>
       </c>
       <c r="C44" s="37">
@@ -10420,7 +10636,7 @@
         <v>6</v>
       </c>
       <c r="H44" s="37">
-        <f>G44/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>266.66666666666669</v>
       </c>
       <c r="I44" s="23"/>
@@ -10430,7 +10646,7 @@
         <v>1988</v>
       </c>
       <c r="B45" s="37">
-        <f>SUM(C45:G45)</f>
+        <f t="shared" si="2"/>
         <v>194</v>
       </c>
       <c r="C45" s="37">
@@ -10449,7 +10665,7 @@
         <v>6</v>
       </c>
       <c r="H45" s="37">
-        <f>G45/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>266.66666666666669</v>
       </c>
       <c r="I45" s="23"/>
@@ -10459,7 +10675,7 @@
         <v>1989</v>
       </c>
       <c r="B46" s="37">
-        <f>SUM(C46:G46)</f>
+        <f t="shared" si="2"/>
         <v>198</v>
       </c>
       <c r="C46" s="37">
@@ -10478,7 +10694,7 @@
         <v>7</v>
       </c>
       <c r="H46" s="37">
-        <f>G46/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>311.11111111111114</v>
       </c>
       <c r="I46" s="23"/>
@@ -10488,7 +10704,7 @@
         <v>1990</v>
       </c>
       <c r="B47" s="37">
-        <f>SUM(C47:G47)</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="C47" s="37">
@@ -10507,7 +10723,7 @@
         <v>8</v>
       </c>
       <c r="H47" s="37">
-        <f>G47/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>355.5555555555556</v>
       </c>
       <c r="I47" s="23"/>
@@ -10517,7 +10733,7 @@
         <v>1991</v>
       </c>
       <c r="B48" s="37">
-        <f>SUM(C48:G48)</f>
+        <f t="shared" si="2"/>
         <v>202</v>
       </c>
       <c r="C48" s="37">
@@ -10536,17 +10752,17 @@
         <v>11</v>
       </c>
       <c r="H48" s="37">
-        <f>G48/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>488.88888888888897</v>
       </c>
       <c r="I48" s="23"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="20">
         <v>1992</v>
       </c>
       <c r="B49" s="37">
-        <f>SUM(C49:G49)</f>
+        <f t="shared" si="2"/>
         <v>221</v>
       </c>
       <c r="C49" s="37">
@@ -10565,17 +10781,17 @@
         <v>10</v>
       </c>
       <c r="H49" s="37">
-        <f>G49/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>444.44444444444446</v>
       </c>
       <c r="I49" s="23"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="20">
         <v>1993</v>
       </c>
       <c r="B50" s="37">
-        <f>SUM(C50:G50)</f>
+        <f t="shared" si="2"/>
         <v>155</v>
       </c>
       <c r="C50" s="37">
@@ -10594,12 +10810,12 @@
         <v>6</v>
       </c>
       <c r="H50" s="37">
-        <f>G50/2.5/0.009</f>
+        <f t="shared" si="1"/>
         <v>266.66666666666669</v>
       </c>
       <c r="I50" s="23"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="20">
         <v>1994</v>
       </c>
@@ -10611,7 +10827,7 @@
       <c r="G51" s="38"/>
       <c r="H51" s="38"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="20">
         <v>1995</v>
       </c>
@@ -10621,14 +10837,14 @@
       <c r="E52" s="38"/>
       <c r="F52" s="38"/>
       <c r="G52" s="37">
-        <f>H52*(9.2)*2.5/1000</f>
+        <f t="shared" ref="G52:G60" si="3">H52*(9.2)*2.5/1000</f>
         <v>9.2086019999999991</v>
       </c>
       <c r="H52" s="8">
         <v>400.37400000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="20">
         <v>1996</v>
       </c>
@@ -10640,14 +10856,14 @@
       <c r="E53" s="38"/>
       <c r="F53" s="38"/>
       <c r="G53" s="37">
-        <f>H53*(9.2)*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>9.979538999999999</v>
       </c>
       <c r="H53" s="8">
         <v>433.89299999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="20">
         <v>1997</v>
       </c>
@@ -10659,14 +10875,14 @@
       <c r="E54" s="37"/>
       <c r="F54" s="37"/>
       <c r="G54" s="37">
-        <f>H54*(9.2)*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>10.487448000000001</v>
       </c>
       <c r="H54" s="8">
         <v>455.976</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="20">
         <v>1998</v>
       </c>
@@ -10677,14 +10893,14 @@
       <c r="E55" s="38"/>
       <c r="F55" s="38"/>
       <c r="G55" s="37">
-        <f>H55*(9.2)*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>10.868373999999999</v>
       </c>
       <c r="H55" s="8">
         <v>472.53800000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
         <v>1999</v>
       </c>
@@ -10695,14 +10911,14 @@
       <c r="E56" s="38"/>
       <c r="F56" s="38"/>
       <c r="G56" s="37">
-        <f>H56*(9.2)*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>8.9088199999999986</v>
       </c>
       <c r="H56" s="8">
         <v>387.34</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="20">
         <v>2000</v>
       </c>
@@ -10714,21 +10930,15 @@
       <c r="E57" s="38"/>
       <c r="F57" s="38"/>
       <c r="G57" s="37">
-        <f>H57*(9.2)*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>10.196681999999999</v>
       </c>
       <c r="H57" s="8">
         <v>443.334</v>
       </c>
-      <c r="I57" s="40">
-        <v>400374</v>
-      </c>
-      <c r="J57" s="19">
-        <f t="shared" ref="J57:J81" si="0">I57/1000</f>
-        <v>400.37400000000002</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I57" s="40"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="20">
         <v>2001</v>
       </c>
@@ -10740,21 +10950,15 @@
       <c r="E58" s="38"/>
       <c r="F58" s="38"/>
       <c r="G58" s="37">
-        <f>H58*(9.2)*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>11.294195999999999</v>
       </c>
       <c r="H58" s="8">
         <v>491.05200000000002</v>
       </c>
-      <c r="I58" s="40">
-        <v>433893</v>
-      </c>
-      <c r="J58" s="19">
-        <f t="shared" si="0"/>
-        <v>433.89299999999997</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I58" s="40"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="20">
         <v>2002</v>
       </c>
@@ -10766,21 +10970,15 @@
       <c r="E59" s="38"/>
       <c r="F59" s="38"/>
       <c r="G59" s="37">
-        <f>H59*(9.2)*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>10.998323999999997</v>
       </c>
       <c r="H59" s="8">
         <v>478.18799999999999</v>
       </c>
-      <c r="I59" s="40">
-        <v>455976</v>
-      </c>
-      <c r="J59" s="19">
-        <f t="shared" si="0"/>
-        <v>455.976</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I59" s="40"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="20">
         <v>2003</v>
       </c>
@@ -10792,21 +10990,15 @@
       <c r="E60" s="38"/>
       <c r="F60" s="38"/>
       <c r="G60" s="37">
-        <f>H60*(9.2)*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>11.341921000000001</v>
       </c>
       <c r="H60" s="8">
         <v>493.12700000000001</v>
       </c>
-      <c r="I60" s="40">
-        <v>472538</v>
-      </c>
-      <c r="J60" s="19">
-        <f t="shared" si="0"/>
-        <v>472.53800000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I60" s="40"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="20">
         <v>2004</v>
       </c>
@@ -10823,15 +11015,9 @@
       <c r="H61" s="8">
         <v>449.02499999999998</v>
       </c>
-      <c r="I61" s="40">
-        <v>387340</v>
-      </c>
-      <c r="J61" s="19">
-        <f t="shared" si="0"/>
-        <v>387.34</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I61" s="40"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="20">
         <v>2005</v>
       </c>
@@ -10848,15 +11034,9 @@
       <c r="H62" s="8">
         <v>699.721</v>
       </c>
-      <c r="I62" s="40">
-        <v>443334</v>
-      </c>
-      <c r="J62" s="19">
-        <f t="shared" si="0"/>
-        <v>443.334</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I62" s="40"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="20">
         <v>2006</v>
       </c>
@@ -10868,21 +11048,15 @@
       <c r="E63" s="38"/>
       <c r="F63" s="38"/>
       <c r="G63" s="37">
-        <f>H63*(9.2)*2.5/1000</f>
+        <f t="shared" ref="G63:G76" si="4">H63*(9.2)*2.5/1000</f>
         <v>11.492777999999998</v>
       </c>
       <c r="H63" s="8">
         <v>499.68599999999998</v>
       </c>
-      <c r="I63" s="40">
-        <v>491052</v>
-      </c>
-      <c r="J63" s="19">
-        <f t="shared" si="0"/>
-        <v>491.05200000000002</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I63" s="40"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="20">
         <v>2007</v>
       </c>
@@ -10894,21 +11068,15 @@
       <c r="E64" s="38"/>
       <c r="F64" s="38"/>
       <c r="G64" s="37">
-        <f>H64*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>13.133505999999999</v>
       </c>
       <c r="H64" s="8">
         <v>571.02200000000005</v>
       </c>
-      <c r="I64" s="40">
-        <v>478188</v>
-      </c>
-      <c r="J64" s="19">
-        <f t="shared" si="0"/>
-        <v>478.18799999999999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I64" s="40"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="20">
         <v>2008</v>
       </c>
@@ -10920,21 +11088,15 @@
       <c r="E65" s="37"/>
       <c r="F65" s="37"/>
       <c r="G65" s="37">
-        <f>H65*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>13.790339999999999</v>
       </c>
       <c r="H65" s="8">
         <v>599.58000000000004</v>
       </c>
-      <c r="I65" s="40">
-        <v>493127</v>
-      </c>
-      <c r="J65" s="19">
-        <f t="shared" si="0"/>
-        <v>493.12700000000001</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I65" s="40"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="20">
         <v>2009</v>
       </c>
@@ -10946,21 +11108,15 @@
       <c r="E66" s="37"/>
       <c r="F66" s="37"/>
       <c r="G66" s="37">
-        <f>H66*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>12.927333999999998</v>
       </c>
       <c r="H66" s="8">
         <v>562.05799999999999</v>
       </c>
-      <c r="I66" s="40">
-        <v>449025</v>
-      </c>
-      <c r="J66" s="19">
-        <f t="shared" si="0"/>
-        <v>449.02499999999998</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I66" s="40"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="20">
         <v>2010</v>
       </c>
@@ -10971,21 +11127,15 @@
       <c r="E67" s="37"/>
       <c r="F67" s="37"/>
       <c r="G67" s="37">
-        <f>H67*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>11.184739</v>
       </c>
       <c r="H67" s="8">
         <v>486.29300000000001</v>
       </c>
-      <c r="I67" s="40">
-        <v>699721</v>
-      </c>
-      <c r="J67" s="19">
-        <f t="shared" si="0"/>
-        <v>699.721</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I67" s="40"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="20">
         <v>2011</v>
       </c>
@@ -10996,21 +11146,15 @@
       <c r="E68" s="37"/>
       <c r="F68" s="37"/>
       <c r="G68" s="37">
-        <f>H68*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>12.343110999999999</v>
       </c>
       <c r="H68" s="8">
         <v>536.65700000000004</v>
       </c>
-      <c r="I68" s="40">
-        <v>499686</v>
-      </c>
-      <c r="J68" s="19">
-        <f t="shared" si="0"/>
-        <v>499.68599999999998</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I68" s="40"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="20">
         <v>2012</v>
       </c>
@@ -11021,21 +11165,15 @@
       <c r="E69" s="37"/>
       <c r="F69" s="37"/>
       <c r="G69" s="37">
-        <f>H69*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>13.599508999999998</v>
       </c>
       <c r="H69" s="8">
         <v>591.28300000000002</v>
       </c>
-      <c r="I69" s="40">
-        <v>571022</v>
-      </c>
-      <c r="J69" s="19">
-        <f t="shared" si="0"/>
-        <v>571.02200000000005</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I69" s="40"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="20">
         <v>2013</v>
       </c>
@@ -11046,21 +11184,15 @@
       <c r="E70" s="37"/>
       <c r="F70" s="37"/>
       <c r="G70" s="37">
-        <f>H70*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>11.751458999999999</v>
       </c>
       <c r="H70" s="8">
         <v>510.93299999999999</v>
       </c>
-      <c r="I70" s="40">
-        <v>599580</v>
-      </c>
-      <c r="J70" s="19">
-        <f t="shared" si="0"/>
-        <v>599.58000000000004</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I70" s="40"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="20">
         <v>2014</v>
       </c>
@@ -11071,21 +11203,15 @@
       <c r="E71" s="37"/>
       <c r="F71" s="37"/>
       <c r="G71" s="37">
-        <f>H71*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>12.467908999999997</v>
       </c>
       <c r="H71" s="8">
         <v>542.08299999999997</v>
       </c>
-      <c r="I71" s="40">
-        <v>562058</v>
-      </c>
-      <c r="J71" s="19">
-        <f t="shared" si="0"/>
-        <v>562.05799999999999</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I71" s="40"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="20">
         <v>2015</v>
       </c>
@@ -11096,21 +11222,15 @@
       <c r="E72" s="37"/>
       <c r="F72" s="37"/>
       <c r="G72" s="37">
-        <f>H72*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>10.045572</v>
       </c>
       <c r="H72" s="8">
         <v>436.76400000000001</v>
       </c>
-      <c r="I72" s="40">
-        <v>486293</v>
-      </c>
-      <c r="J72" s="19">
-        <f t="shared" si="0"/>
-        <v>486.29300000000001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I72" s="40"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="20">
         <v>2016</v>
       </c>
@@ -11121,21 +11241,15 @@
       <c r="E73" s="37"/>
       <c r="F73" s="37"/>
       <c r="G73" s="37">
-        <f>H73*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>9.8299009999999978</v>
       </c>
       <c r="H73" s="8">
         <v>427.387</v>
       </c>
-      <c r="I73" s="40">
-        <v>536657</v>
-      </c>
-      <c r="J73" s="19">
-        <f t="shared" si="0"/>
-        <v>536.65700000000004</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I73" s="40"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="20">
         <v>2017</v>
       </c>
@@ -11147,21 +11261,15 @@
       <c r="E74" s="37"/>
       <c r="F74" s="37"/>
       <c r="G74" s="37">
-        <f>H74*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>10.351357</v>
       </c>
       <c r="H74" s="8">
         <v>450.05900000000003</v>
       </c>
-      <c r="I74" s="40">
-        <v>591283</v>
-      </c>
-      <c r="J74" s="19">
-        <f t="shared" si="0"/>
-        <v>591.28300000000002</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I74" s="40"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="20">
         <v>2018</v>
       </c>
@@ -11173,21 +11281,15 @@
       <c r="E75" s="37"/>
       <c r="F75" s="37"/>
       <c r="G75" s="37">
-        <f>H75*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>8.2984229999999997</v>
       </c>
       <c r="H75" s="8">
         <v>360.80099999999999</v>
       </c>
-      <c r="I75" s="40">
-        <v>510933</v>
-      </c>
-      <c r="J75" s="19">
-        <f t="shared" si="0"/>
-        <v>510.93299999999999</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I75" s="40"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="20">
         <v>2019</v>
       </c>
@@ -11199,67 +11301,31 @@
       <c r="E76" s="37"/>
       <c r="F76" s="37"/>
       <c r="G76" s="37">
-        <f>H76*(9.2)*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>14.018108999999997</v>
       </c>
       <c r="H76" s="8">
         <v>609.48299999999995</v>
       </c>
-      <c r="I76" s="40">
-        <v>542083</v>
-      </c>
-      <c r="J76" s="19">
-        <f t="shared" si="0"/>
-        <v>542.08299999999997</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I76" s="40"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="20">
         <v>2020</v>
       </c>
-      <c r="I77" s="40">
-        <v>436764</v>
-      </c>
-      <c r="J77" s="19">
-        <f t="shared" si="0"/>
-        <v>436.76400000000001</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I78" s="40">
-        <v>427387</v>
-      </c>
-      <c r="J78" s="19">
-        <f t="shared" si="0"/>
-        <v>427.387</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I79" s="40">
-        <v>450059</v>
-      </c>
-      <c r="J79" s="19">
-        <f t="shared" si="0"/>
-        <v>450.05900000000003</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I80" s="40">
-        <v>360801</v>
-      </c>
-      <c r="J80" s="19">
-        <f t="shared" si="0"/>
-        <v>360.80099999999999</v>
-      </c>
-    </row>
-    <row r="81" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I81" s="40">
-        <v>609483</v>
-      </c>
-      <c r="J81" s="19">
-        <f t="shared" si="0"/>
-        <v>609.48299999999995</v>
-      </c>
+      <c r="I77" s="40"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I78" s="40"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I79" s="40"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I80" s="40"/>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I81" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11273,11 +11339,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11643,7 +11709,7 @@
         <v>13.080000000000002</v>
       </c>
       <c r="H17" s="37">
-        <f>G17/2.5/0.009</f>
+        <f t="shared" ref="H17:H50" si="0">G17/2.5/0.009</f>
         <v>581.33333333333348</v>
       </c>
       <c r="I17" s="11"/>
@@ -11673,7 +11739,7 @@
         <v>17</v>
       </c>
       <c r="H18" s="37">
-        <f>G18/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>755.55555555555554</v>
       </c>
       <c r="I18" s="11"/>
@@ -11703,7 +11769,7 @@
         <v>20</v>
       </c>
       <c r="H19" s="37">
-        <f>G19/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>888.88888888888891</v>
       </c>
       <c r="I19" s="11"/>
@@ -11733,7 +11799,7 @@
         <v>21</v>
       </c>
       <c r="H20" s="37">
-        <f>G20/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>933.33333333333348</v>
       </c>
       <c r="I20" s="11"/>
@@ -11763,7 +11829,7 @@
         <v>25</v>
       </c>
       <c r="H21" s="37">
-        <f>G21/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1111.1111111111111</v>
       </c>
       <c r="I21" s="11"/>
@@ -11793,7 +11859,7 @@
         <v>34</v>
       </c>
       <c r="H22" s="37">
-        <f>G22/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1511.1111111111111</v>
       </c>
       <c r="I22" s="11"/>
@@ -11823,7 +11889,7 @@
         <v>32</v>
       </c>
       <c r="H23" s="37">
-        <f>G23/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1422.2222222222224</v>
       </c>
       <c r="I23" s="11"/>
@@ -11853,7 +11919,7 @@
         <v>36</v>
       </c>
       <c r="H24" s="37">
-        <f>G24/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1600.0000000000002</v>
       </c>
       <c r="I24" s="11"/>
@@ -11883,7 +11949,7 @@
         <v>37</v>
       </c>
       <c r="H25" s="37">
-        <f>G25/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1644.4444444444446</v>
       </c>
       <c r="I25" s="11"/>
@@ -11913,7 +11979,7 @@
         <v>42</v>
       </c>
       <c r="H26" s="37">
-        <f>G26/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1866.666666666667</v>
       </c>
       <c r="I26" s="11"/>
@@ -11943,7 +12009,7 @@
         <v>47</v>
       </c>
       <c r="H27" s="37">
-        <f>G27/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>2088.8888888888891</v>
       </c>
       <c r="I27" s="11"/>
@@ -11954,7 +12020,7 @@
         <v>1971</v>
       </c>
       <c r="B28" s="4">
-        <f>SUM(C28:G28)</f>
+        <f t="shared" ref="B28:B38" si="1">SUM(C28:G28)</f>
         <v>498</v>
       </c>
       <c r="C28" s="8">
@@ -11973,7 +12039,7 @@
         <v>45</v>
       </c>
       <c r="H28" s="37">
-        <f>G28/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>2000.0000000000002</v>
       </c>
       <c r="I28" s="11"/>
@@ -11984,7 +12050,7 @@
         <v>1972</v>
       </c>
       <c r="B29" s="4">
-        <f>SUM(C29:G29)</f>
+        <f t="shared" si="1"/>
         <v>569</v>
       </c>
       <c r="C29" s="8">
@@ -12003,7 +12069,7 @@
         <v>44</v>
       </c>
       <c r="H29" s="37">
-        <f>G29/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1955.5555555555559</v>
       </c>
       <c r="I29" s="11"/>
@@ -12014,7 +12080,7 @@
         <v>1973</v>
       </c>
       <c r="B30" s="4">
-        <f>SUM(C30:G30)</f>
+        <f t="shared" si="1"/>
         <v>565</v>
       </c>
       <c r="C30" s="8">
@@ -12033,7 +12099,7 @@
         <v>40</v>
       </c>
       <c r="H30" s="37">
-        <f>G30/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1777.7777777777778</v>
       </c>
       <c r="I30" s="11"/>
@@ -12044,7 +12110,7 @@
         <v>1974</v>
       </c>
       <c r="B31" s="4">
-        <f>SUM(C31:G31)</f>
+        <f t="shared" si="1"/>
         <v>515</v>
       </c>
       <c r="C31" s="8">
@@ -12063,7 +12129,7 @@
         <v>34</v>
       </c>
       <c r="H31" s="37">
-        <f>G31/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1511.1111111111111</v>
       </c>
       <c r="I31" s="11"/>
@@ -12074,7 +12140,7 @@
         <v>1975</v>
       </c>
       <c r="B32" s="4">
-        <f>SUM(C32:G32)</f>
+        <f t="shared" si="1"/>
         <v>358</v>
       </c>
       <c r="C32" s="8">
@@ -12093,7 +12159,7 @@
         <v>34</v>
       </c>
       <c r="H32" s="37">
-        <f>G32/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1511.1111111111111</v>
       </c>
       <c r="I32" s="11"/>
@@ -12104,7 +12170,7 @@
         <v>1976</v>
       </c>
       <c r="B33" s="4">
-        <f>SUM(C33:G33)</f>
+        <f t="shared" si="1"/>
         <v>505</v>
       </c>
       <c r="C33" s="8">
@@ -12123,7 +12189,7 @@
         <v>32</v>
       </c>
       <c r="H33" s="37">
-        <f>G33/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1422.2222222222224</v>
       </c>
       <c r="I33" s="11"/>
@@ -12134,7 +12200,7 @@
         <v>1977</v>
       </c>
       <c r="B34" s="4">
-        <f>SUM(C34:G34)</f>
+        <f t="shared" si="1"/>
         <v>548</v>
       </c>
       <c r="C34" s="8">
@@ -12153,7 +12219,7 @@
         <v>26</v>
       </c>
       <c r="H34" s="37">
-        <f>G34/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1155.5555555555557</v>
       </c>
       <c r="I34" s="11"/>
@@ -12164,7 +12230,7 @@
         <v>1978</v>
       </c>
       <c r="B35" s="4">
-        <f>SUM(C35:G35)</f>
+        <f t="shared" si="1"/>
         <v>633</v>
       </c>
       <c r="C35" s="8">
@@ -12183,7 +12249,7 @@
         <v>33</v>
       </c>
       <c r="H35" s="37">
-        <f>G35/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1466.6666666666667</v>
       </c>
       <c r="I35" s="11"/>
@@ -12194,7 +12260,7 @@
         <v>1979</v>
       </c>
       <c r="B36" s="4">
-        <f>SUM(C36:G36)</f>
+        <f t="shared" si="1"/>
         <v>646</v>
       </c>
       <c r="C36" s="8">
@@ -12213,7 +12279,7 @@
         <v>41</v>
       </c>
       <c r="H36" s="37">
-        <f>G36/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1822.2222222222222</v>
       </c>
       <c r="I36" s="11"/>
@@ -12224,7 +12290,7 @@
         <v>1980</v>
       </c>
       <c r="B37" s="4">
-        <f>SUM(C37:G37)</f>
+        <f t="shared" si="1"/>
         <v>657</v>
       </c>
       <c r="C37" s="8">
@@ -12243,7 +12309,7 @@
         <v>54</v>
       </c>
       <c r="H37" s="37">
-        <f>G37/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>2400.0000000000005</v>
       </c>
       <c r="I37" s="11"/>
@@ -12254,7 +12320,7 @@
         <v>1981</v>
       </c>
       <c r="B38" s="4">
-        <f>SUM(C38:G38)</f>
+        <f t="shared" si="1"/>
         <v>586</v>
       </c>
       <c r="C38" s="8">
@@ -12273,7 +12339,7 @@
         <v>39</v>
       </c>
       <c r="H38" s="37">
-        <f>G38/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1733.3333333333335</v>
       </c>
       <c r="I38" s="11"/>
@@ -12303,7 +12369,7 @@
         <v>29</v>
       </c>
       <c r="H39" s="37">
-        <f>G39/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1288.8888888888889</v>
       </c>
       <c r="I39" s="11"/>
@@ -12333,7 +12399,7 @@
         <v>25</v>
       </c>
       <c r="H40" s="37">
-        <f>G40/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1111.1111111111111</v>
       </c>
       <c r="I40" s="11"/>
@@ -12363,7 +12429,7 @@
         <v>24</v>
       </c>
       <c r="H41" s="37">
-        <f>G41/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1066.6666666666667</v>
       </c>
       <c r="I41" s="11"/>
@@ -12393,7 +12459,7 @@
         <v>27</v>
       </c>
       <c r="H42" s="37">
-        <f>G42/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1200.0000000000002</v>
       </c>
       <c r="I42" s="11"/>
@@ -12423,7 +12489,7 @@
         <v>28</v>
       </c>
       <c r="H43" s="37">
-        <f>G43/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1244.4444444444446</v>
       </c>
       <c r="I43" s="11"/>
@@ -12434,7 +12500,7 @@
         <v>1987</v>
       </c>
       <c r="B44" s="4">
-        <f>SUM(C44:G44)</f>
+        <f t="shared" ref="B44:B50" si="2">SUM(C44:G44)</f>
         <v>876</v>
       </c>
       <c r="C44" s="8">
@@ -12453,7 +12519,7 @@
         <v>32</v>
       </c>
       <c r="H44" s="37">
-        <f>G44/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1422.2222222222224</v>
       </c>
       <c r="I44" s="11"/>
@@ -12464,7 +12530,7 @@
         <v>1988</v>
       </c>
       <c r="B45" s="4">
-        <f>SUM(C45:G45)</f>
+        <f t="shared" si="2"/>
         <v>888</v>
       </c>
       <c r="C45" s="8">
@@ -12483,7 +12549,7 @@
         <v>37</v>
       </c>
       <c r="H45" s="37">
-        <f>G45/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1644.4444444444446</v>
       </c>
       <c r="I45" s="11"/>
@@ -12494,7 +12560,7 @@
         <v>1989</v>
       </c>
       <c r="B46" s="4">
-        <f>SUM(C46:G46)</f>
+        <f t="shared" si="2"/>
         <v>1076</v>
       </c>
       <c r="C46" s="8">
@@ -12513,7 +12579,7 @@
         <v>32</v>
       </c>
       <c r="H46" s="37">
-        <f>G46/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1422.2222222222224</v>
       </c>
       <c r="I46" s="11"/>
@@ -12524,7 +12590,7 @@
         <v>1990</v>
       </c>
       <c r="B47" s="4">
-        <f>SUM(C47:G47)</f>
+        <f t="shared" si="2"/>
         <v>1091</v>
       </c>
       <c r="C47" s="8">
@@ -12543,7 +12609,7 @@
         <v>30</v>
       </c>
       <c r="H47" s="37">
-        <f>G47/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1333.3333333333335</v>
       </c>
       <c r="I47" s="11"/>
@@ -12554,7 +12620,7 @@
         <v>1991</v>
       </c>
       <c r="B48" s="4">
-        <f>SUM(C48:G48)</f>
+        <f t="shared" si="2"/>
         <v>957</v>
       </c>
       <c r="C48" s="8">
@@ -12573,7 +12639,7 @@
         <v>28</v>
       </c>
       <c r="H48" s="37">
-        <f>G48/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1244.4444444444446</v>
       </c>
       <c r="I48" s="11"/>
@@ -12584,7 +12650,7 @@
         <v>1992</v>
       </c>
       <c r="B49" s="4">
-        <f>SUM(C49:G49)</f>
+        <f t="shared" si="2"/>
         <v>981</v>
       </c>
       <c r="C49" s="8">
@@ -12603,7 +12669,7 @@
         <v>26</v>
       </c>
       <c r="H49" s="37">
-        <f>G49/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1155.5555555555557</v>
       </c>
       <c r="I49" s="11"/>
@@ -12614,7 +12680,7 @@
         <v>1993</v>
       </c>
       <c r="B50" s="4">
-        <f>SUM(C50:G50)</f>
+        <f t="shared" si="2"/>
         <v>1065</v>
       </c>
       <c r="C50" s="8">
@@ -12633,7 +12699,7 @@
         <v>27</v>
       </c>
       <c r="H50" s="37">
-        <f>G50/2.5/0.009</f>
+        <f t="shared" si="0"/>
         <v>1200.0000000000002</v>
       </c>
       <c r="I50" s="11"/>
@@ -12662,7 +12728,7 @@
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="8">
-        <f>H52*11*2.5/1000</f>
+        <f t="shared" ref="G52:G60" si="3">H52*11*2.5/1000</f>
         <v>31.953322500000002</v>
       </c>
       <c r="H52" s="8">
@@ -12683,7 +12749,7 @@
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="8">
-        <f>H53*11*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>28.438575</v>
       </c>
       <c r="H53" s="8">
@@ -12704,7 +12770,7 @@
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
       <c r="G54" s="8">
-        <f>H54*11*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>32.004307499999996</v>
       </c>
       <c r="H54" s="8">
@@ -12725,7 +12791,7 @@
       <c r="E55" s="10"/>
       <c r="F55" s="10"/>
       <c r="G55" s="8">
-        <f>H55*11*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>36.909702500000002</v>
       </c>
       <c r="H55" s="8">
@@ -12746,7 +12812,7 @@
       <c r="E56" s="10"/>
       <c r="F56" s="10"/>
       <c r="G56" s="8">
-        <f>H56*11*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>41.368497500000004</v>
       </c>
       <c r="H56" s="8">
@@ -12767,7 +12833,7 @@
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
       <c r="G57" s="8">
-        <f>H57*11*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>45.356987500000002</v>
       </c>
       <c r="H57" s="8">
@@ -12788,7 +12854,7 @@
       <c r="E58" s="8"/>
       <c r="F58" s="10"/>
       <c r="G58" s="8">
-        <f>H58*11*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>47.589767500000001</v>
       </c>
       <c r="H58" s="8">
@@ -12809,7 +12875,7 @@
       <c r="E59" s="8"/>
       <c r="F59" s="10"/>
       <c r="G59" s="8">
-        <f>H59*11*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>42.730462500000002</v>
       </c>
       <c r="H59" s="8">
@@ -12830,7 +12896,7 @@
       <c r="E60" s="8"/>
       <c r="F60" s="10"/>
       <c r="G60" s="8">
-        <f>H60*11*2.5/1000</f>
+        <f t="shared" si="3"/>
         <v>35.249142500000005</v>
       </c>
       <c r="H60" s="8">
@@ -12891,7 +12957,7 @@
       <c r="E63" s="10"/>
       <c r="F63" s="10"/>
       <c r="G63" s="8">
-        <f>H63*11*2.5/1000</f>
+        <f t="shared" ref="G63:G75" si="4">H63*11*2.5/1000</f>
         <v>23.251745000000003</v>
       </c>
       <c r="H63" s="8">
@@ -12912,7 +12978,7 @@
       <c r="E64" s="10"/>
       <c r="F64" s="10"/>
       <c r="G64" s="8">
-        <f>H64*11*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>27.908347500000001</v>
       </c>
       <c r="H64" s="8">
@@ -12933,7 +12999,7 @@
       <c r="E65" s="10"/>
       <c r="F65" s="10"/>
       <c r="G65" s="8">
-        <f>H65*11*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>29.395684999999997</v>
       </c>
       <c r="H65" s="8">
@@ -12954,7 +13020,7 @@
       <c r="E66" s="10"/>
       <c r="F66" s="10"/>
       <c r="G66" s="8">
-        <f>H66*11*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>23.787912499999997</v>
       </c>
       <c r="H66" s="8">
@@ -12975,7 +13041,7 @@
       <c r="E67" s="8"/>
       <c r="F67" s="10"/>
       <c r="G67" s="8">
-        <f>H67*11*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>22.698307500000002</v>
       </c>
       <c r="H67" s="8">
@@ -12996,7 +13062,7 @@
       <c r="E68" s="8"/>
       <c r="F68" s="10"/>
       <c r="G68" s="8">
-        <f>H68*11*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>19.528629999999996</v>
       </c>
       <c r="H68" s="8">
@@ -13017,7 +13083,7 @@
       <c r="E69" s="8"/>
       <c r="F69" s="10"/>
       <c r="G69" s="8">
-        <f>H69*11*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>15.309442500000001</v>
       </c>
       <c r="H69" s="8">
@@ -13038,7 +13104,7 @@
       <c r="E70" s="8"/>
       <c r="F70" s="10"/>
       <c r="G70" s="8">
-        <f>H70*11*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>15.463222500000001</v>
       </c>
       <c r="H70" s="8">
@@ -13059,7 +13125,7 @@
       <c r="E71" s="8"/>
       <c r="F71" s="10"/>
       <c r="G71" s="8">
-        <f>H71*11*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>14.345732499999999</v>
       </c>
       <c r="H71" s="8">
@@ -13080,7 +13146,7 @@
       <c r="E72" s="8"/>
       <c r="F72" s="10"/>
       <c r="G72" s="8">
-        <f>H72*11*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>19.744972499999999</v>
       </c>
       <c r="H72" s="8">
@@ -13101,7 +13167,7 @@
       <c r="E73" s="8"/>
       <c r="F73" s="10"/>
       <c r="G73" s="8">
-        <f>H73*11*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>21.609857499999997</v>
       </c>
       <c r="H73" s="8">
@@ -13122,7 +13188,7 @@
       <c r="E74" s="8"/>
       <c r="F74" s="10"/>
       <c r="G74" s="8">
-        <f>H74*11*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>19.800934999999999</v>
       </c>
       <c r="H74" s="8">
@@ -13143,7 +13209,7 @@
       <c r="E75" s="8"/>
       <c r="F75" s="10"/>
       <c r="G75" s="8">
-        <f>H75*11*2.5/1000</f>
+        <f t="shared" si="4"/>
         <v>20.938197500000001</v>
       </c>
       <c r="H75" s="8">
@@ -16323,4 +16389,634 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20697ACE-82C7-45F0-9119-243699C7EDD6}">
+  <dimension ref="A1:C88"/>
+  <sheetViews>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>1947</v>
+      </c>
+      <c r="B4" s="8">
+        <v>8512</v>
+      </c>
+      <c r="C4" s="46"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>1960</v>
+      </c>
+      <c r="B17" s="8">
+        <v>9153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>1961</v>
+      </c>
+      <c r="B18" s="8">
+        <v>9184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>1962</v>
+      </c>
+      <c r="B19" s="8">
+        <v>9221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>1963</v>
+      </c>
+      <c r="B20" s="8">
+        <v>9290</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>1964</v>
+      </c>
+      <c r="B21" s="8">
+        <v>9378</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>1965</v>
+      </c>
+      <c r="B22" s="8">
+        <v>9464</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>1966</v>
+      </c>
+      <c r="B23" s="8">
+        <v>9528</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>1967</v>
+      </c>
+      <c r="B24" s="8">
+        <v>9581</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>1968</v>
+      </c>
+      <c r="B25" s="8">
+        <v>9619</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>1969</v>
+      </c>
+      <c r="B26" s="8">
+        <v>9646</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>1970</v>
+      </c>
+      <c r="B27" s="8">
+        <v>9656</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>1971</v>
+      </c>
+      <c r="B28" s="8">
+        <v>9673</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>1972</v>
+      </c>
+      <c r="B29" s="8">
+        <v>9711</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>1973</v>
+      </c>
+      <c r="B30" s="8">
+        <v>9742</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>1974</v>
+      </c>
+      <c r="B31" s="8">
+        <v>9772</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>1975</v>
+      </c>
+      <c r="B32" s="8">
+        <v>9801</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>1976</v>
+      </c>
+      <c r="B33" s="8">
+        <v>9818</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>1977</v>
+      </c>
+      <c r="B34" s="8">
+        <v>9830</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
+        <v>1978</v>
+      </c>
+      <c r="B35" s="8">
+        <v>9840</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>1979</v>
+      </c>
+      <c r="B36" s="8">
+        <v>9848</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>1980</v>
+      </c>
+      <c r="B37" s="8">
+        <v>9859</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="14">
+        <v>1981</v>
+      </c>
+      <c r="B38" s="8">
+        <v>9859</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="14">
+        <v>1982</v>
+      </c>
+      <c r="B39" s="8">
+        <v>9856</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
+        <v>1983</v>
+      </c>
+      <c r="B40" s="8">
+        <v>9856</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="14">
+        <v>1984</v>
+      </c>
+      <c r="B41" s="8">
+        <v>9855</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
+        <v>1985</v>
+      </c>
+      <c r="B42" s="8">
+        <v>9858</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="14">
+        <v>1986</v>
+      </c>
+      <c r="B43" s="8">
+        <v>9862</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="14">
+        <v>1987</v>
+      </c>
+      <c r="B44" s="8">
+        <v>9870</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
+        <v>1988</v>
+      </c>
+      <c r="B45" s="8">
+        <v>9902</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
+        <v>1989</v>
+      </c>
+      <c r="B46" s="8">
+        <v>9938</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
+        <v>1990</v>
+      </c>
+      <c r="B47" s="8">
+        <v>9967</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="14">
+        <v>1991</v>
+      </c>
+      <c r="B48" s="8">
+        <v>10004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="14">
+        <v>1992</v>
+      </c>
+      <c r="B49" s="8">
+        <v>10045</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="14">
+        <v>1993</v>
+      </c>
+      <c r="B50" s="8">
+        <v>10084</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="14">
+        <v>1994</v>
+      </c>
+      <c r="B51" s="8">
+        <v>10116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="14">
+        <v>1995</v>
+      </c>
+      <c r="B52" s="8">
+        <v>10137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="14">
+        <v>1996</v>
+      </c>
+      <c r="B53" s="8">
+        <v>10157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="14">
+        <v>1997</v>
+      </c>
+      <c r="B54" s="8">
+        <v>10181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="14">
+        <v>1998</v>
+      </c>
+      <c r="B55" s="8">
+        <v>10203</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="14">
+        <v>1999</v>
+      </c>
+      <c r="B56" s="8">
+        <v>10226</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="14">
+        <v>2000</v>
+      </c>
+      <c r="B57" s="8">
+        <v>10251</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="14">
+        <v>2001</v>
+      </c>
+      <c r="B58" s="8">
+        <v>10287</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="14">
+        <v>2002</v>
+      </c>
+      <c r="B59" s="8">
+        <v>10333</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="14">
+        <v>2003</v>
+      </c>
+      <c r="B60" s="8">
+        <v>10376</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="14">
+        <v>2004</v>
+      </c>
+      <c r="B61" s="8">
+        <v>10421</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="14">
+        <v>2005</v>
+      </c>
+      <c r="B62" s="8">
+        <v>10479</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="14">
+        <v>2006</v>
+      </c>
+      <c r="B63" s="8">
+        <v>10548</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="14">
+        <v>2007</v>
+      </c>
+      <c r="B64" s="8">
+        <v>10626</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="14">
+        <v>2008</v>
+      </c>
+      <c r="B65" s="8">
+        <v>10710</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="14">
+        <v>2009</v>
+      </c>
+      <c r="B66" s="8">
+        <v>10796</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="14">
+        <v>2010</v>
+      </c>
+      <c r="B67" s="8">
+        <v>10896</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="14">
+        <v>2011</v>
+      </c>
+      <c r="B68" s="8">
+        <v>10994</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="14">
+        <v>2012</v>
+      </c>
+      <c r="B69" s="8">
+        <v>11068</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="14">
+        <v>2013</v>
+      </c>
+      <c r="B70" s="8">
+        <v>11125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="14">
+        <v>2014</v>
+      </c>
+      <c r="B71" s="8">
+        <v>11180</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="14">
+        <v>2015</v>
+      </c>
+      <c r="B72" s="8">
+        <v>11238</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="14">
+        <v>2016</v>
+      </c>
+      <c r="B73" s="8">
+        <v>11295</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="14">
+        <v>2017</v>
+      </c>
+      <c r="B74" s="8">
+        <v>11349</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="14">
+        <v>2018</v>
+      </c>
+      <c r="B75" s="8">
+        <v>11404</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="14">
+        <v>2019</v>
+      </c>
+      <c r="B76" s="8">
+        <v>11481</v>
+      </c>
+      <c r="C76" s="48"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="14">
+        <v>2020</v>
+      </c>
+      <c r="B77" s="47">
+        <v>11493</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="13"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="13"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="13"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="13"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="13"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="13"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="13"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="13"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="13"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update notebook, with uncertainties but still EU + ODYM to do
</commit_message>
<xml_diff>
--- a/RawData/BE_RawData_VPython.xlsx
+++ b/RawData/BE_RawData_VPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\01_MFA_GlassIndustry\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD863548-2EC2-44F1-BE77-8063B08D4D91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50ED58E-133A-4BD9-A8D8-3FAB57E25531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="600" windowWidth="13125" windowHeight="15600" activeTab="2" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="stock" sheetId="17" r:id="rId1"/>
@@ -122,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{6C77227F-1643-4775-B843-631830CA24FD}">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{6C77227F-1643-4775-B843-631830CA24FD}">
       <text>
         <r>
           <rPr>
@@ -136,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{FFF54F8C-42A9-47BE-BA11-9E812209664C}">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{FFF54F8C-42A9-47BE-BA11-9E812209664C}">
       <text>
         <r>
           <rPr>
@@ -160,6 +160,19 @@
             <family val="2"/>
           </rPr>
           <t>"L'industrie du verre en Belgique", Verre, vol 1, n° 4, July-August, 1987, p. 432-9</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{96C299E4-2F85-40C0-9F3A-1BF5ACC63F3A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>100.000 insulating glass units intalled in Europe in the year 1955. We suppose an average window area of 1.5x1.5m². It represents 2% of the annual production of the year 1970. We generalise this ratio to France and Belgium.</t>
         </r>
       </text>
     </comment>
@@ -7055,7 +7068,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -7195,6 +7208,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -8670,11 +8686,11 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8711,19 +8727,19 @@
         <v>1946</v>
       </c>
       <c r="B3" s="9"/>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17">
+        <f>C3*0.009*2.5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1947</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="17">
-        <f>C4*0.0091*2.5</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -8744,14 +8760,6 @@
       <c r="B7" s="9">
         <v>206.25</v>
       </c>
-      <c r="C7" s="45">
-        <f>0.0015*C27</f>
-        <v>4.0513333333333339</v>
-      </c>
-      <c r="D7" s="8">
-        <f>C7*2.5*0.009</f>
-        <v>9.1155E-2</v>
-      </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -8782,6 +8790,14 @@
         <v>1955</v>
       </c>
       <c r="B12" s="9"/>
+      <c r="C12" s="45">
+        <f>0.02*C27</f>
+        <v>54.017777777777781</v>
+      </c>
+      <c r="D12" s="8">
+        <f>C12*0.009*2.5</f>
+        <v>1.2154</v>
+      </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -8907,8 +8923,8 @@
         <v>2700.8888888888891</v>
       </c>
       <c r="D27" s="37">
-        <f t="shared" ref="D27:D38" si="0">C27*0.0091*2.5</f>
-        <v>61.445222222222228</v>
+        <f>C27*0.009*2.5</f>
+        <v>60.769999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8923,8 +8939,8 @@
         <v>2646.8888888888891</v>
       </c>
       <c r="D28" s="37">
-        <f t="shared" si="0"/>
-        <v>60.216722222222231</v>
+        <f t="shared" ref="D28:D39" si="0">C28*0.009*2.5</f>
+        <v>59.555</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8940,7 +8956,7 @@
       </c>
       <c r="D29" s="37">
         <f t="shared" si="0"/>
-        <v>60.830972222222229</v>
+        <v>60.162500000000001</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8956,7 +8972,7 @@
       </c>
       <c r="D30" s="37">
         <f t="shared" si="0"/>
-        <v>63.287972222222237</v>
+        <v>62.592500000000001</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8972,7 +8988,7 @@
       </c>
       <c r="D31" s="37">
         <f t="shared" si="0"/>
-        <v>69.020972222222227</v>
+        <v>68.262500000000003</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8988,7 +9004,7 @@
       </c>
       <c r="D32" s="37">
         <f t="shared" si="0"/>
-        <v>73.627847222222229</v>
+        <v>72.818750000000009</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9004,7 +9020,7 @@
       </c>
       <c r="D33" s="37">
         <f t="shared" si="0"/>
-        <v>79.667972222222232</v>
+        <v>78.792500000000004</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9020,7 +9036,7 @@
       </c>
       <c r="D34" s="37">
         <f t="shared" si="0"/>
-        <v>84.991472222222228</v>
+        <v>84.05749999999999</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9036,7 +9052,7 @@
       </c>
       <c r="D35" s="37">
         <f t="shared" si="0"/>
-        <v>85.400972222222236</v>
+        <v>84.462499999999991</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9052,7 +9068,7 @@
       </c>
       <c r="D36" s="37">
         <f t="shared" si="0"/>
-        <v>85.400972222222236</v>
+        <v>84.462499999999991</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9068,7 +9084,7 @@
       </c>
       <c r="D37" s="37">
         <f t="shared" si="0"/>
-        <v>98.709722222222226</v>
+        <v>97.625</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9084,7 +9100,7 @@
       </c>
       <c r="D38" s="37">
         <f t="shared" si="0"/>
-        <v>90.519722222222242</v>
+        <v>89.525000000000006</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9099,8 +9115,8 @@
         <v>3798.8888888888891</v>
       </c>
       <c r="D39" s="37">
-        <f>C39*0.0091*2.5</f>
-        <v>86.424722222222229</v>
+        <f t="shared" si="0"/>
+        <v>85.474999999999994</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9615,7 +9631,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11339,11 +11355,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12699,8 +12715,8 @@
         <v>27</v>
       </c>
       <c r="H50" s="37">
-        <f t="shared" si="0"/>
-        <v>1200.0000000000002</v>
+        <f>G50/2.5/0.01</f>
+        <v>1080</v>
       </c>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
@@ -12902,7 +12918,6 @@
       <c r="H60" s="8">
         <v>1281.787</v>
       </c>
-      <c r="I60" s="39"/>
       <c r="J60" s="11"/>
     </row>
     <row r="61" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12922,7 +12937,10 @@
       <c r="H61" s="8">
         <v>1129.606</v>
       </c>
-      <c r="I61" s="39"/>
+      <c r="I61" s="49">
+        <f>G61/H61/2.5</f>
+        <v>1.2075006683746368E-2</v>
+      </c>
       <c r="J61" s="11"/>
     </row>
     <row r="62" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -12942,8 +12960,14 @@
       <c r="H62" s="8">
         <v>1132.49</v>
       </c>
-      <c r="I62" s="39"/>
-      <c r="J62" s="11"/>
+      <c r="I62" s="49">
+        <f>G62/H62/2.5</f>
+        <v>1.0914003655661418E-2</v>
+      </c>
+      <c r="J62" s="11">
+        <f>I62+I61</f>
+        <v>2.2989010339407784E-2</v>
+      </c>
     </row>
     <row r="63" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14">
@@ -12964,7 +12988,10 @@
         <v>845.51800000000003</v>
       </c>
       <c r="I63" s="39"/>
-      <c r="J63" s="11"/>
+      <c r="J63" s="49">
+        <f>J62/2</f>
+        <v>1.1494505169703892E-2</v>
+      </c>
     </row>
     <row r="64" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14">

</xml_diff>

<commit_message>
Update with ODYM in IGU MFA
</commit_message>
<xml_diff>
--- a/RawData/BE_RawData_VPython.xlsx
+++ b/RawData/BE_RawData_VPython.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\01_MFA_GlassIndustry\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50ED58E-133A-4BD9-A8D8-3FAB57E25531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EA3DFA-4754-4061-9692-BB89F2B515E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="1170" yWindow="600" windowWidth="13125" windowHeight="15600" firstSheet="2" activeTab="4" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="stock" sheetId="17" r:id="rId1"/>
@@ -4333,13 +4333,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Verre…, vol 1, N° 4, juillet-aout 1987
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>See also:
+Verre…, vol 1, N° 4, juillet-aout 1987
 "L'industrie du verre en Belgique" p. 432-9</t>
         </r>
       </text>
@@ -4576,13 +4576,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Verre…, vol 1, N° 4, juillet-aout 1987
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>See also:
+Verre…, vol 1, N° 4, juillet-aout 1987
 "L'industrie du verre en Belgique" p. 432-9</t>
         </r>
       </text>
@@ -4610,13 +4610,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Verre…, vol 1, N° 4, juillet-aout 1987
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>See also:
+Verre…, vol 1, N° 4, juillet-aout 1987
 "L'industrie du verre en Belgique" p. 432-9</t>
         </r>
       </text>
@@ -4644,13 +4644,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Verre…, vol 1, N° 4, juillet-aout 1987
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>See also:
+Verre…, vol 1, N° 4, juillet-aout 1987
 "L'industrie du verre en Belgique" p. 432-9</t>
         </r>
       </text>
@@ -4678,13 +4678,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Verre…, vol 1, N° 4, juillet-aout 1987
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>See also:
+Verre…, vol 1, N° 4, juillet-aout 1987
 "L'industrie du verre en Belgique" p. 432-9</t>
         </r>
       </text>
@@ -4712,13 +4712,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Verre…, vol 1, N° 4, juillet-aout 1987
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>See also:
+Verre…, vol 1, N° 4, juillet-aout 1987
 "L'industrie du verre en Belgique" p. 432-9</t>
         </r>
       </text>
@@ -7068,7 +7068,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -7209,6 +7209,10 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -8687,10 +8691,10 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8821,7 +8825,7 @@
       <c r="A16" s="2">
         <v>1959</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="51"/>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -9631,7 +9635,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H36" sqref="H36"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9867,8 +9871,8 @@
         <v>1960</v>
       </c>
       <c r="B17" s="37">
-        <f>SUM(C17:G17)</f>
-        <v>14</v>
+        <f>14+1</f>
+        <v>15</v>
       </c>
       <c r="C17" s="37">
         <v>11</v>
@@ -9895,8 +9899,8 @@
         <v>1961</v>
       </c>
       <c r="B18" s="37">
-        <f>SUM(C18:G18)</f>
-        <v>6</v>
+        <f>4+1</f>
+        <v>5</v>
       </c>
       <c r="C18" s="37">
         <v>3</v>
@@ -9923,7 +9927,7 @@
         <v>1962</v>
       </c>
       <c r="B19" s="37">
-        <f>SUM(C19:G19)</f>
+        <f>11+1</f>
         <v>12</v>
       </c>
       <c r="C19" s="37">
@@ -9951,7 +9955,7 @@
         <v>1963</v>
       </c>
       <c r="B20" s="37">
-        <f>SUM(C20:G20)</f>
+        <f>7+1</f>
         <v>8</v>
       </c>
       <c r="C20" s="37">
@@ -10033,8 +10037,8 @@
         <v>1966</v>
       </c>
       <c r="B23" s="37">
-        <f>SUM(C23:G23)</f>
-        <v>34</v>
+        <f>32+3</f>
+        <v>35</v>
       </c>
       <c r="C23" s="37">
         <v>14</v>
@@ -10061,8 +10065,8 @@
         <v>1967</v>
       </c>
       <c r="B24" s="37">
-        <f>SUM(C24:G24)</f>
-        <v>29</v>
+        <f>26+1</f>
+        <v>27</v>
       </c>
       <c r="C24" s="37">
         <v>19</v>
@@ -10089,8 +10093,8 @@
         <v>1968</v>
       </c>
       <c r="B25" s="37">
-        <f>SUM(C25:G25)</f>
-        <v>33</v>
+        <f>31+3</f>
+        <v>34</v>
       </c>
       <c r="C25" s="37">
         <v>18</v>
@@ -10117,8 +10121,8 @@
         <v>1969</v>
       </c>
       <c r="B26" s="37">
-        <f>SUM(C26:G26)</f>
-        <v>35</v>
+        <f>30+6</f>
+        <v>36</v>
       </c>
       <c r="C26" s="37">
         <v>11</v>
@@ -10173,8 +10177,8 @@
         <v>1971</v>
       </c>
       <c r="B28" s="37">
-        <f t="shared" ref="B28:B38" si="0">SUM(C28:G28)</f>
-        <v>35</v>
+        <f>29+9</f>
+        <v>38</v>
       </c>
       <c r="C28" s="37">
         <v>6</v>
@@ -10201,8 +10205,8 @@
         <v>1972</v>
       </c>
       <c r="B29" s="37">
-        <f t="shared" si="0"/>
-        <v>43</v>
+        <f>38+7</f>
+        <v>45</v>
       </c>
       <c r="C29" s="37">
         <v>13</v>
@@ -10229,8 +10233,8 @@
         <v>1973</v>
       </c>
       <c r="B30" s="37">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <f>50+9</f>
+        <v>59</v>
       </c>
       <c r="C30" s="37">
         <v>21</v>
@@ -10257,8 +10261,8 @@
         <v>1974</v>
       </c>
       <c r="B31" s="37">
-        <f t="shared" si="0"/>
-        <v>55</v>
+        <f>51+7</f>
+        <v>58</v>
       </c>
       <c r="C31" s="37">
         <v>25</v>
@@ -10285,8 +10289,8 @@
         <v>1975</v>
       </c>
       <c r="B32" s="37">
-        <f t="shared" si="0"/>
-        <v>52</v>
+        <f>46+7</f>
+        <v>53</v>
       </c>
       <c r="C32" s="37">
         <v>26</v>
@@ -10304,7 +10308,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="37">
-        <f t="shared" ref="H32:H50" si="1">G32/2.5/0.009</f>
+        <f t="shared" ref="H32:H50" si="0">G32/2.5/0.009</f>
         <v>44.44444444444445</v>
       </c>
       <c r="I32" s="23"/>
@@ -10314,8 +10318,8 @@
         <v>1976</v>
       </c>
       <c r="B33" s="37">
-        <f t="shared" si="0"/>
-        <v>82</v>
+        <f>75+10</f>
+        <v>85</v>
       </c>
       <c r="C33" s="37">
         <v>43</v>
@@ -10333,7 +10337,7 @@
         <v>2</v>
       </c>
       <c r="H33" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>88.8888888888889</v>
       </c>
       <c r="I33" s="23"/>
@@ -10343,8 +10347,8 @@
         <v>1977</v>
       </c>
       <c r="B34" s="37">
-        <f t="shared" si="0"/>
-        <v>94</v>
+        <f>84+14</f>
+        <v>98</v>
       </c>
       <c r="C34" s="37">
         <v>57</v>
@@ -10362,7 +10366,7 @@
         <v>3</v>
       </c>
       <c r="H34" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>133.33333333333334</v>
       </c>
       <c r="I34" s="23"/>
@@ -10372,8 +10376,8 @@
         <v>1978</v>
       </c>
       <c r="B35" s="37">
-        <f t="shared" si="0"/>
-        <v>88</v>
+        <f>77+14</f>
+        <v>91</v>
       </c>
       <c r="C35" s="37">
         <v>55</v>
@@ -10391,7 +10395,7 @@
         <v>5</v>
       </c>
       <c r="H35" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>222.22222222222223</v>
       </c>
       <c r="I35" s="23"/>
@@ -10401,8 +10405,8 @@
         <v>1979</v>
       </c>
       <c r="B36" s="37">
-        <f t="shared" si="0"/>
-        <v>108</v>
+        <f>94+16</f>
+        <v>110</v>
       </c>
       <c r="C36" s="37">
         <v>78</v>
@@ -10420,7 +10424,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>266.66666666666669</v>
       </c>
       <c r="I36" s="23"/>
@@ -10430,8 +10434,8 @@
         <v>1980</v>
       </c>
       <c r="B37" s="37">
-        <f t="shared" si="0"/>
-        <v>128</v>
+        <f>111+20</f>
+        <v>131</v>
       </c>
       <c r="C37" s="37">
         <v>97</v>
@@ -10449,7 +10453,7 @@
         <v>9</v>
       </c>
       <c r="H37" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>400.00000000000006</v>
       </c>
       <c r="I37" s="23"/>
@@ -10459,8 +10463,8 @@
         <v>1981</v>
       </c>
       <c r="B38" s="37">
-        <f t="shared" si="0"/>
-        <v>123</v>
+        <f>110+18</f>
+        <v>128</v>
       </c>
       <c r="C38" s="37">
         <v>98</v>
@@ -10478,7 +10482,7 @@
         <v>8</v>
       </c>
       <c r="H38" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>355.5555555555556</v>
       </c>
       <c r="I38" s="23"/>
@@ -10507,7 +10511,7 @@
         <v>7</v>
       </c>
       <c r="H39" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>311.11111111111114</v>
       </c>
       <c r="I39" s="23"/>
@@ -10536,7 +10540,7 @@
         <v>6</v>
       </c>
       <c r="H40" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>266.66666666666669</v>
       </c>
       <c r="I40" s="23"/>
@@ -10565,7 +10569,7 @@
         <v>5</v>
       </c>
       <c r="H41" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>222.22222222222223</v>
       </c>
       <c r="I41" s="23"/>
@@ -10594,7 +10598,7 @@
         <v>5</v>
       </c>
       <c r="H42" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>222.22222222222223</v>
       </c>
       <c r="I42" s="23"/>
@@ -10623,7 +10627,7 @@
         <v>6</v>
       </c>
       <c r="H43" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>266.66666666666669</v>
       </c>
       <c r="I43" s="23"/>
@@ -10633,8 +10637,8 @@
         <v>1987</v>
       </c>
       <c r="B44" s="37">
-        <f t="shared" ref="B44:B50" si="2">SUM(C44:G44)</f>
-        <v>191</v>
+        <f>166+30</f>
+        <v>196</v>
       </c>
       <c r="C44" s="37">
         <v>155</v>
@@ -10652,7 +10656,7 @@
         <v>6</v>
       </c>
       <c r="H44" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>266.66666666666669</v>
       </c>
       <c r="I44" s="23"/>
@@ -10662,8 +10666,8 @@
         <v>1988</v>
       </c>
       <c r="B45" s="37">
-        <f t="shared" si="2"/>
-        <v>194</v>
+        <f>156+44</f>
+        <v>200</v>
       </c>
       <c r="C45" s="37">
         <v>142</v>
@@ -10681,7 +10685,7 @@
         <v>6</v>
       </c>
       <c r="H45" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>266.66666666666669</v>
       </c>
       <c r="I45" s="23"/>
@@ -10691,8 +10695,8 @@
         <v>1989</v>
       </c>
       <c r="B46" s="37">
-        <f t="shared" si="2"/>
-        <v>198</v>
+        <f>155+49</f>
+        <v>204</v>
       </c>
       <c r="C46" s="37">
         <v>142</v>
@@ -10710,7 +10714,7 @@
         <v>7</v>
       </c>
       <c r="H46" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>311.11111111111114</v>
       </c>
       <c r="I46" s="23"/>
@@ -10720,8 +10724,8 @@
         <v>1990</v>
       </c>
       <c r="B47" s="37">
-        <f t="shared" si="2"/>
-        <v>180</v>
+        <f>142+45</f>
+        <v>187</v>
       </c>
       <c r="C47" s="37">
         <v>124</v>
@@ -10739,7 +10743,7 @@
         <v>8</v>
       </c>
       <c r="H47" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>355.5555555555556</v>
       </c>
       <c r="I47" s="23"/>
@@ -10749,8 +10753,8 @@
         <v>1991</v>
       </c>
       <c r="B48" s="37">
-        <f t="shared" si="2"/>
-        <v>202</v>
+        <f>163+46</f>
+        <v>209</v>
       </c>
       <c r="C48" s="37">
         <v>147</v>
@@ -10768,7 +10772,7 @@
         <v>11</v>
       </c>
       <c r="H48" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>488.88888888888897</v>
       </c>
       <c r="I48" s="23"/>
@@ -10778,8 +10782,8 @@
         <v>1992</v>
       </c>
       <c r="B49" s="37">
-        <f t="shared" si="2"/>
-        <v>221</v>
+        <f>182+48</f>
+        <v>230</v>
       </c>
       <c r="C49" s="37">
         <v>166</v>
@@ -10797,7 +10801,7 @@
         <v>10</v>
       </c>
       <c r="H49" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>444.44444444444446</v>
       </c>
       <c r="I49" s="23"/>
@@ -10807,8 +10811,8 @@
         <v>1993</v>
       </c>
       <c r="B50" s="37">
-        <f t="shared" si="2"/>
-        <v>155</v>
+        <f>124+38</f>
+        <v>162</v>
       </c>
       <c r="C50" s="37">
         <v>106</v>
@@ -10826,7 +10830,7 @@
         <v>6</v>
       </c>
       <c r="H50" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>266.66666666666669</v>
       </c>
       <c r="I50" s="23"/>
@@ -10853,7 +10857,7 @@
       <c r="E52" s="38"/>
       <c r="F52" s="38"/>
       <c r="G52" s="37">
-        <f t="shared" ref="G52:G60" si="3">H52*(9.2)*2.5/1000</f>
+        <f t="shared" ref="G52:G60" si="1">H52*(9.2)*2.5/1000</f>
         <v>9.2086019999999991</v>
       </c>
       <c r="H52" s="8">
@@ -10872,7 +10876,7 @@
       <c r="E53" s="38"/>
       <c r="F53" s="38"/>
       <c r="G53" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>9.979538999999999</v>
       </c>
       <c r="H53" s="8">
@@ -10891,7 +10895,7 @@
       <c r="E54" s="37"/>
       <c r="F54" s="37"/>
       <c r="G54" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>10.487448000000001</v>
       </c>
       <c r="H54" s="8">
@@ -10909,7 +10913,7 @@
       <c r="E55" s="38"/>
       <c r="F55" s="38"/>
       <c r="G55" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>10.868373999999999</v>
       </c>
       <c r="H55" s="8">
@@ -10927,7 +10931,7 @@
       <c r="E56" s="38"/>
       <c r="F56" s="38"/>
       <c r="G56" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>8.9088199999999986</v>
       </c>
       <c r="H56" s="8">
@@ -10946,7 +10950,7 @@
       <c r="E57" s="38"/>
       <c r="F57" s="38"/>
       <c r="G57" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>10.196681999999999</v>
       </c>
       <c r="H57" s="8">
@@ -10966,7 +10970,7 @@
       <c r="E58" s="38"/>
       <c r="F58" s="38"/>
       <c r="G58" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>11.294195999999999</v>
       </c>
       <c r="H58" s="8">
@@ -10986,7 +10990,7 @@
       <c r="E59" s="38"/>
       <c r="F59" s="38"/>
       <c r="G59" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>10.998323999999997</v>
       </c>
       <c r="H59" s="8">
@@ -11006,7 +11010,7 @@
       <c r="E60" s="38"/>
       <c r="F60" s="38"/>
       <c r="G60" s="37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>11.341921000000001</v>
       </c>
       <c r="H60" s="8">
@@ -11064,7 +11068,7 @@
       <c r="E63" s="38"/>
       <c r="F63" s="38"/>
       <c r="G63" s="37">
-        <f t="shared" ref="G63:G76" si="4">H63*(9.2)*2.5/1000</f>
+        <f t="shared" ref="G63:G76" si="2">H63*(9.2)*2.5/1000</f>
         <v>11.492777999999998</v>
       </c>
       <c r="H63" s="8">
@@ -11084,7 +11088,7 @@
       <c r="E64" s="38"/>
       <c r="F64" s="38"/>
       <c r="G64" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>13.133505999999999</v>
       </c>
       <c r="H64" s="8">
@@ -11104,7 +11108,7 @@
       <c r="E65" s="37"/>
       <c r="F65" s="37"/>
       <c r="G65" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>13.790339999999999</v>
       </c>
       <c r="H65" s="8">
@@ -11124,7 +11128,7 @@
       <c r="E66" s="37"/>
       <c r="F66" s="37"/>
       <c r="G66" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>12.927333999999998</v>
       </c>
       <c r="H66" s="8">
@@ -11143,7 +11147,7 @@
       <c r="E67" s="37"/>
       <c r="F67" s="37"/>
       <c r="G67" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>11.184739</v>
       </c>
       <c r="H67" s="8">
@@ -11162,7 +11166,7 @@
       <c r="E68" s="37"/>
       <c r="F68" s="37"/>
       <c r="G68" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>12.343110999999999</v>
       </c>
       <c r="H68" s="8">
@@ -11181,7 +11185,7 @@
       <c r="E69" s="37"/>
       <c r="F69" s="37"/>
       <c r="G69" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>13.599508999999998</v>
       </c>
       <c r="H69" s="8">
@@ -11200,7 +11204,7 @@
       <c r="E70" s="37"/>
       <c r="F70" s="37"/>
       <c r="G70" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>11.751458999999999</v>
       </c>
       <c r="H70" s="8">
@@ -11219,7 +11223,7 @@
       <c r="E71" s="37"/>
       <c r="F71" s="37"/>
       <c r="G71" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>12.467908999999997</v>
       </c>
       <c r="H71" s="8">
@@ -11238,7 +11242,7 @@
       <c r="E72" s="37"/>
       <c r="F72" s="37"/>
       <c r="G72" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>10.045572</v>
       </c>
       <c r="H72" s="8">
@@ -11257,7 +11261,7 @@
       <c r="E73" s="37"/>
       <c r="F73" s="37"/>
       <c r="G73" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9.8299009999999978</v>
       </c>
       <c r="H73" s="8">
@@ -11277,7 +11281,7 @@
       <c r="E74" s="37"/>
       <c r="F74" s="37"/>
       <c r="G74" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>10.351357</v>
       </c>
       <c r="H74" s="8">
@@ -11297,7 +11301,7 @@
       <c r="E75" s="37"/>
       <c r="F75" s="37"/>
       <c r="G75" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>8.2984229999999997</v>
       </c>
       <c r="H75" s="8">
@@ -11317,7 +11321,7 @@
       <c r="E76" s="37"/>
       <c r="F76" s="37"/>
       <c r="G76" s="37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>14.018108999999997</v>
       </c>
       <c r="H76" s="8">
@@ -11356,10 +11360,10 @@
   <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G52" sqref="G52"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11725,7 +11729,7 @@
         <v>13.080000000000002</v>
       </c>
       <c r="H17" s="37">
-        <f t="shared" ref="H17:H50" si="0">G17/2.5/0.009</f>
+        <f t="shared" ref="H17:H49" si="0">G17/2.5/0.009</f>
         <v>581.33333333333348</v>
       </c>
       <c r="I17" s="11"/>
@@ -11886,8 +11890,8 @@
         <v>1966</v>
       </c>
       <c r="B23" s="4">
-        <f>SUM(C23:G23)</f>
-        <v>376</v>
+        <f>328+66</f>
+        <v>394</v>
       </c>
       <c r="C23" s="8">
         <v>76</v>
@@ -11916,8 +11920,8 @@
         <v>1967</v>
       </c>
       <c r="B24" s="4">
-        <f>SUM(C24:G24)</f>
-        <v>370</v>
+        <f>315+72</f>
+        <v>387</v>
       </c>
       <c r="C24" s="8">
         <v>72</v>
@@ -11946,8 +11950,8 @@
         <v>1968</v>
       </c>
       <c r="B25" s="4">
-        <f>SUM(C25:G25)</f>
-        <v>413</v>
+        <f>354+76</f>
+        <v>430</v>
       </c>
       <c r="C25" s="8">
         <v>79</v>
@@ -11976,8 +11980,8 @@
         <v>1969</v>
       </c>
       <c r="B26" s="4">
-        <f>SUM(C26:G26)</f>
-        <v>432</v>
+        <f>369+82</f>
+        <v>451</v>
       </c>
       <c r="C26" s="8">
         <v>79</v>
@@ -12036,8 +12040,8 @@
         <v>1971</v>
       </c>
       <c r="B28" s="4">
-        <f t="shared" ref="B28:B38" si="1">SUM(C28:G28)</f>
-        <v>498</v>
+        <f>425+97</f>
+        <v>522</v>
       </c>
       <c r="C28" s="8">
         <v>161</v>
@@ -12066,8 +12070,8 @@
         <v>1972</v>
       </c>
       <c r="B29" s="4">
-        <f t="shared" si="1"/>
-        <v>569</v>
+        <f>498+101</f>
+        <v>599</v>
       </c>
       <c r="C29" s="8">
         <v>192</v>
@@ -12096,8 +12100,8 @@
         <v>1973</v>
       </c>
       <c r="B30" s="4">
-        <f t="shared" si="1"/>
-        <v>565</v>
+        <f>500+102</f>
+        <v>602</v>
       </c>
       <c r="C30" s="8">
         <v>176</v>
@@ -12126,8 +12130,8 @@
         <v>1974</v>
       </c>
       <c r="B31" s="4">
-        <f t="shared" si="1"/>
-        <v>515</v>
+        <f>457+90</f>
+        <v>547</v>
       </c>
       <c r="C31" s="8">
         <v>149</v>
@@ -12156,8 +12160,8 @@
         <v>1975</v>
       </c>
       <c r="B32" s="4">
-        <f t="shared" si="1"/>
-        <v>358</v>
+        <f>304+80</f>
+        <v>384</v>
       </c>
       <c r="C32" s="8">
         <v>134</v>
@@ -12186,8 +12190,8 @@
         <v>1976</v>
       </c>
       <c r="B33" s="4">
-        <f t="shared" si="1"/>
-        <v>505</v>
+        <f>447+89</f>
+        <v>536</v>
       </c>
       <c r="C33" s="8">
         <v>264</v>
@@ -12216,8 +12220,8 @@
         <v>1977</v>
       </c>
       <c r="B34" s="4">
-        <f t="shared" si="1"/>
-        <v>548</v>
+        <f>497+78</f>
+        <v>575</v>
       </c>
       <c r="C34" s="8">
         <v>347</v>
@@ -12246,8 +12250,8 @@
         <v>1978</v>
       </c>
       <c r="B35" s="4">
-        <f t="shared" si="1"/>
-        <v>633</v>
+        <f>572+89</f>
+        <v>661</v>
       </c>
       <c r="C35" s="8">
         <v>423</v>
@@ -12276,8 +12280,8 @@
         <v>1979</v>
       </c>
       <c r="B36" s="4">
-        <f t="shared" si="1"/>
-        <v>646</v>
+        <f>578+96</f>
+        <v>674</v>
       </c>
       <c r="C36" s="8">
         <v>449</v>
@@ -12306,8 +12310,8 @@
         <v>1980</v>
       </c>
       <c r="B37" s="4">
-        <f t="shared" si="1"/>
-        <v>657</v>
+        <f>576+113</f>
+        <v>689</v>
       </c>
       <c r="C37" s="8">
         <v>472</v>
@@ -12336,8 +12340,8 @@
         <v>1981</v>
       </c>
       <c r="B38" s="4">
-        <f t="shared" si="1"/>
-        <v>586</v>
+        <f>519+101</f>
+        <v>620</v>
       </c>
       <c r="C38" s="8">
         <v>419</v>
@@ -12366,8 +12370,8 @@
         <v>1982</v>
       </c>
       <c r="B39" s="4">
-        <f>600+108</f>
-        <v>708</v>
+        <f>601+108</f>
+        <v>709</v>
       </c>
       <c r="C39" s="8">
         <v>527</v>
@@ -12516,8 +12520,8 @@
         <v>1987</v>
       </c>
       <c r="B44" s="4">
-        <f t="shared" ref="B44:B50" si="2">SUM(C44:G44)</f>
-        <v>876</v>
+        <f>770+194</f>
+        <v>964</v>
       </c>
       <c r="C44" s="8">
         <v>675</v>
@@ -12546,8 +12550,8 @@
         <v>1988</v>
       </c>
       <c r="B45" s="4">
-        <f t="shared" si="2"/>
-        <v>888</v>
+        <f>757+229</f>
+        <v>986</v>
       </c>
       <c r="C45" s="8">
         <v>671</v>
@@ -12576,8 +12580,8 @@
         <v>1989</v>
       </c>
       <c r="B46" s="4">
-        <f t="shared" si="2"/>
-        <v>1076</v>
+        <f>934+252</f>
+        <v>1186</v>
       </c>
       <c r="C46" s="8">
         <v>850</v>
@@ -12606,8 +12610,8 @@
         <v>1990</v>
       </c>
       <c r="B47" s="4">
-        <f t="shared" si="2"/>
-        <v>1091</v>
+        <f>961+239</f>
+        <v>1200</v>
       </c>
       <c r="C47" s="8">
         <v>887</v>
@@ -12636,8 +12640,8 @@
         <v>1991</v>
       </c>
       <c r="B48" s="4">
-        <f t="shared" si="2"/>
-        <v>957</v>
+        <f>836+232</f>
+        <v>1068</v>
       </c>
       <c r="C48" s="8">
         <v>765</v>
@@ -12666,8 +12670,8 @@
         <v>1992</v>
       </c>
       <c r="B49" s="4">
-        <f t="shared" si="2"/>
-        <v>981</v>
+        <f>846+229</f>
+        <v>1075</v>
       </c>
       <c r="C49" s="8">
         <v>779</v>
@@ -12696,8 +12700,8 @@
         <v>1993</v>
       </c>
       <c r="B50" s="4">
-        <f t="shared" si="2"/>
-        <v>1065</v>
+        <f>928+265</f>
+        <v>1193</v>
       </c>
       <c r="C50" s="8">
         <v>866</v>
@@ -12744,7 +12748,7 @@
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="8">
-        <f t="shared" ref="G52:G60" si="3">H52*11*2.5/1000</f>
+        <f t="shared" ref="G52:G60" si="1">H52*11*2.5/1000</f>
         <v>31.953322500000002</v>
       </c>
       <c r="H52" s="8">
@@ -12765,7 +12769,7 @@
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>28.438575</v>
       </c>
       <c r="H53" s="8">
@@ -12786,7 +12790,7 @@
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
       <c r="G54" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>32.004307499999996</v>
       </c>
       <c r="H54" s="8">
@@ -12807,7 +12811,7 @@
       <c r="E55" s="10"/>
       <c r="F55" s="10"/>
       <c r="G55" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>36.909702500000002</v>
       </c>
       <c r="H55" s="8">
@@ -12828,7 +12832,7 @@
       <c r="E56" s="10"/>
       <c r="F56" s="10"/>
       <c r="G56" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>41.368497500000004</v>
       </c>
       <c r="H56" s="8">
@@ -12849,7 +12853,7 @@
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
       <c r="G57" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>45.356987500000002</v>
       </c>
       <c r="H57" s="8">
@@ -12870,7 +12874,7 @@
       <c r="E58" s="8"/>
       <c r="F58" s="10"/>
       <c r="G58" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>47.589767500000001</v>
       </c>
       <c r="H58" s="8">
@@ -12891,7 +12895,7 @@
       <c r="E59" s="8"/>
       <c r="F59" s="10"/>
       <c r="G59" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>42.730462500000002</v>
       </c>
       <c r="H59" s="8">
@@ -12912,7 +12916,7 @@
       <c r="E60" s="8"/>
       <c r="F60" s="10"/>
       <c r="G60" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>35.249142500000005</v>
       </c>
       <c r="H60" s="8">
@@ -12981,7 +12985,7 @@
       <c r="E63" s="10"/>
       <c r="F63" s="10"/>
       <c r="G63" s="8">
-        <f t="shared" ref="G63:G75" si="4">H63*11*2.5/1000</f>
+        <f t="shared" ref="G63:G75" si="2">H63*11*2.5/1000</f>
         <v>23.251745000000003</v>
       </c>
       <c r="H63" s="8">
@@ -13005,7 +13009,7 @@
       <c r="E64" s="10"/>
       <c r="F64" s="10"/>
       <c r="G64" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>27.908347500000001</v>
       </c>
       <c r="H64" s="8">
@@ -13026,7 +13030,7 @@
       <c r="E65" s="10"/>
       <c r="F65" s="10"/>
       <c r="G65" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>29.395684999999997</v>
       </c>
       <c r="H65" s="8">
@@ -13047,7 +13051,7 @@
       <c r="E66" s="10"/>
       <c r="F66" s="10"/>
       <c r="G66" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>23.787912499999997</v>
       </c>
       <c r="H66" s="8">
@@ -13068,7 +13072,7 @@
       <c r="E67" s="8"/>
       <c r="F67" s="10"/>
       <c r="G67" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>22.698307500000002</v>
       </c>
       <c r="H67" s="8">
@@ -13089,7 +13093,7 @@
       <c r="E68" s="8"/>
       <c r="F68" s="10"/>
       <c r="G68" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>19.528629999999996</v>
       </c>
       <c r="H68" s="8">
@@ -13110,7 +13114,7 @@
       <c r="E69" s="8"/>
       <c r="F69" s="10"/>
       <c r="G69" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>15.309442500000001</v>
       </c>
       <c r="H69" s="8">
@@ -13131,7 +13135,7 @@
       <c r="E70" s="8"/>
       <c r="F70" s="10"/>
       <c r="G70" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>15.463222500000001</v>
       </c>
       <c r="H70" s="8">
@@ -13152,7 +13156,7 @@
       <c r="E71" s="8"/>
       <c r="F71" s="10"/>
       <c r="G71" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>14.345732499999999</v>
       </c>
       <c r="H71" s="8">
@@ -13173,7 +13177,7 @@
       <c r="E72" s="8"/>
       <c r="F72" s="10"/>
       <c r="G72" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>19.744972499999999</v>
       </c>
       <c r="H72" s="8">
@@ -13194,7 +13198,7 @@
       <c r="E73" s="8"/>
       <c r="F73" s="10"/>
       <c r="G73" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>21.609857499999997</v>
       </c>
       <c r="H73" s="8">
@@ -13215,7 +13219,7 @@
       <c r="E74" s="8"/>
       <c r="F74" s="10"/>
       <c r="G74" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>19.800934999999999</v>
       </c>
       <c r="H74" s="8">
@@ -13236,7 +13240,7 @@
       <c r="E75" s="8"/>
       <c r="F75" s="10"/>
       <c r="G75" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>20.938197500000001</v>
       </c>
       <c r="H75" s="8">
@@ -16422,8 +16426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20697ACE-82C7-45F0-9119-243699C7EDD6}">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16489,6 +16493,8 @@
       <c r="A10" s="14">
         <v>1953</v>
       </c>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="14">

</xml_diff>

<commit_message>
update BE, FR and EU datasets
</commit_message>
<xml_diff>
--- a/RawData/BE_RawData_VPython.xlsx
+++ b/RawData/BE_RawData_VPython.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\01_MFA_GlassIndustry\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C49B05-2C8C-4ADF-8865-84D891FF7253}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD51EE50-8D73-483D-AA49-1F8A36AA2BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="600" windowWidth="18525" windowHeight="15600" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21165" windowHeight="15600" activeTab="4" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="19" r:id="rId1"/>
     <sheet name="prod" sheetId="15" r:id="rId2"/>
     <sheet name="import" sheetId="14" r:id="rId3"/>
     <sheet name="export" sheetId="13" r:id="rId4"/>
-    <sheet name="Population" sheetId="18" r:id="rId5"/>
+    <sheet name="Energy_Intensity" sheetId="20" r:id="rId5"/>
+    <sheet name="Population" sheetId="18" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1632,6 +1636,562 @@
     <author>jean</author>
   </authors>
   <commentList>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{DE537177-3911-4596-AA03-3835C6C01F34}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>French data: see paper for explanation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{D206FCDE-335E-4920-B453-B58C33114E10}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>French data: see paper for explanation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{087A89E6-A66E-4BBD-928F-6B194FF60FC9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{B95431E1-3982-4C0A-A5FC-D15F35146521}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{8F06FEB8-9546-43D5-A6DB-CB71AEB1562E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E17" authorId="0" shapeId="0" xr:uid="{16C0BCF4-9E11-4201-B1AD-CE952F0FE18B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{7D93CD46-417C-42CD-AA7F-E2E0E3FFF9C3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{FB51A112-1D64-42D4-AAC8-F93A979609F2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{7D4C727A-EF44-4896-A09A-34C1A4F1446B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{4DAF08F2-FD84-42B2-A21B-7997544440DF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B27" authorId="0" shapeId="0" xr:uid="{084B936F-8A54-40CA-B925-5A418DFA6A13}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C27" authorId="0" shapeId="0" xr:uid="{FB67D8DD-F384-4A7A-8E33-BBAB6E7B1FA2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{64D53901-A92E-4EF7-9298-F674D2B1E323}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E27" authorId="0" shapeId="0" xr:uid="{41C88D21-6E50-4400-88FD-6A659BAAA377}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{F8CD4DCA-40F2-444A-97D7-8E5F99E86DA8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C32" authorId="0" shapeId="0" xr:uid="{5CE94E9C-3353-47AF-B1BF-438981A7FA28}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D32" authorId="0" shapeId="0" xr:uid="{15CA4ED0-AAA5-41E8-863C-CC8C22209288}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E32" authorId="0" shapeId="0" xr:uid="{D4F16F58-A8AD-4E7A-8A1C-4392B4590CF3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{3B74881D-88EA-438D-9F4B-700EB315BF81}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{FAC8AD69-B36C-487B-9B20-08C90EBD0E7A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D37" authorId="0" shapeId="0" xr:uid="{FE5DC22D-35BC-4234-8748-8AE45E7B04DD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E37" authorId="0" shapeId="0" xr:uid="{F5AFFC68-91A1-4976-9B4C-7DDDD8EE626D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{F3C9A46D-459D-4945-9E1E-9E44D4DA868A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C42" authorId="0" shapeId="0" xr:uid="{62263B9B-EC07-4766-BBAE-9F55583F8221}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D42" authorId="0" shapeId="0" xr:uid="{CBF2758F-B604-47F3-99CB-2AC57A8845C2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E42" authorId="0" shapeId="0" xr:uid="{C9EA12CC-B7B4-49F7-B42F-C23FD1044097}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B45" authorId="0" shapeId="0" xr:uid="{FFE76674-C8D2-4BC0-950B-EA5AFA419A9B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C45" authorId="0" shapeId="0" xr:uid="{7E865A39-DF89-4CFC-A5C3-9A5B3D68AF59}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D45" authorId="0" shapeId="0" xr:uid="{64411045-B946-42B0-8634-06C7EC93E236}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Commission of the European Communities, 1984)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E45" authorId="0" shapeId="0" xr:uid="{6E5B2B96-FCB1-421D-95E1-B353EC696B4D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(VGI-FIV, 1994)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B52" authorId="0" shapeId="0" xr:uid="{0B4E96A6-257D-46AA-B963-1BCFD1A801CB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Dinesen et al., 1994),  (Tackels, 1993), (Weir, 1998) and (West et al., 2011)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C52" authorId="0" shapeId="0" xr:uid="{7136E34E-3013-4C38-B4CC-E74F51634316}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Dinesen et al., 1994),  (Tackels, 1993), (Weir, 1998) and (West et al., 2011)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D52" authorId="0" shapeId="0" xr:uid="{95FC4FDA-BCDB-4B3F-9AB2-019AD98439BE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Dinesen et al., 1994),  (Tackels, 1993), (Weir, 1998) and (West et al., 2011)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E52" authorId="0" shapeId="0" xr:uid="{030C8104-8D81-457A-8579-D99098794C7D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Dinesen et al., 1994),  (Tackels, 1993), (Weir, 1998) and (West et al., 2011)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B67" authorId="0" shapeId="0" xr:uid="{039AE180-EEB0-45F6-8286-8E09B58A6FB9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(PE International, 2011) and (Schmitz et al., 2011)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C67" authorId="0" shapeId="0" xr:uid="{AC3A829B-397D-4859-8314-4B77983921AE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(PE International, 2011) and (Schmitz et al., 2011)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D67" authorId="0" shapeId="0" xr:uid="{192AF2BA-4794-40C3-B48E-49ACD4238D11}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(PE International, 2011) and (Schmitz et al., 2011)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E67" authorId="0" shapeId="0" xr:uid="{1A69A1E0-0A3C-44CA-A254-6792F6F1258F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(PE International, 2011) and (Schmitz et al., 2011)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B76" authorId="0" shapeId="0" xr:uid="{72D8DD52-12F8-4B6A-BFD4-072FF9464C9C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(PE International, 2011) and (Schmitz et al., 2011)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C76" authorId="0" shapeId="0" xr:uid="{F54D31B0-3DFA-4F01-B982-E766429A0EDF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(PE International, 2011) and (Schmitz et al., 2011)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D76" authorId="0" shapeId="0" xr:uid="{9491EF51-462C-4170-A6D8-36A9213F51AC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(PE International, 2011) and (Schmitz et al., 2011)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E76" authorId="0" shapeId="0" xr:uid="{2600A99E-340E-4B8F-9612-33F71417A296}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(PE International, 2011) and (Schmitz et al., 2011)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>jean</author>
+  </authors>
+  <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{D03E3816-3F82-47F1-A999-231153AAE251}">
       <text>
         <r>
@@ -1665,7 +2225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>year</t>
   </si>
@@ -1720,17 +2280,36 @@
   <si>
     <t>(VGI-FIV, 1966)</t>
   </si>
+  <si>
+    <t>fuel oil, GJ/t</t>
+  </si>
+  <si>
+    <t>electricity, GJ/t</t>
+  </si>
+  <si>
+    <t>natural gas, GJ/t</t>
+  </si>
+  <si>
+    <t>Total, GJ/t</t>
+  </si>
+  <si>
+    <t>(VGI-FIV, 2001)</t>
+  </si>
+  <si>
+    <t>Fédération de l'industrie du verre (VGI-FIV), 2001. La réduction des émissions de gaz à effet de serre.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1803,6 +2382,26 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1871,7 +2470,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1978,6 +2577,42 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1996,6 +2631,73 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="References"/>
+      <sheetName val="prod"/>
+      <sheetName val="import"/>
+      <sheetName val="export"/>
+      <sheetName val="Population"/>
+      <sheetName val="MatEnergy_WindowGlass"/>
+      <sheetName val="MatEnergy_PlateGlass"/>
+      <sheetName val="RawMat_Intensity"/>
+      <sheetName val="Energy_Intensity"/>
+      <sheetName val="emissions"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="7">
+          <cell r="G7">
+            <v>0.25630252100840334</v>
+          </cell>
+          <cell r="I7">
+            <v>0.40493697478991592</v>
+          </cell>
+          <cell r="K7">
+            <v>0.33876050420168063</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5">
+        <row r="7">
+          <cell r="L7">
+            <v>26.691839999999999</v>
+          </cell>
+          <cell r="N7">
+            <v>0.36000000000000004</v>
+          </cell>
+          <cell r="O7">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6">
+        <row r="7">
+          <cell r="L7">
+            <v>43.411199999999994</v>
+          </cell>
+          <cell r="N7">
+            <v>1.8</v>
+          </cell>
+          <cell r="O7">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2295,10 +2997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025F8ED2-37F9-40BE-8E6A-7FBA957A3175}">
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="118.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,50 +3035,77 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="37" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="39"/>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C9" s="38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="39"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="38"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="38"/>
+      <c r="D12" s="39"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="39"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="38"/>
+      <c r="D14" s="39"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C15" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D15" s="39" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="38"/>
+      <c r="D16" s="39"/>
+    </row>
+    <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="39"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" xr:uid="{B84DBD6C-579B-48BC-96D1-AA795C116670}"/>
+    <hyperlink ref="D15" r:id="rId1" xr:uid="{B84DBD6C-579B-48BC-96D1-AA795C116670}"/>
     <hyperlink ref="D7" r:id="rId2" xr:uid="{BABC48D3-1AA2-44C3-9FD9-1ACF96779787}"/>
-    <hyperlink ref="D9" r:id="rId3" xr:uid="{9095B0BE-927F-4EF3-8BC6-7EABCBE59D13}"/>
+    <hyperlink ref="D11" r:id="rId3" xr:uid="{9095B0BE-927F-4EF3-8BC6-7EABCBE59D13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
@@ -2389,7 +3118,7 @@
   <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F58" sqref="F58"/>
@@ -4541,6 +5270,919 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7426F8F2-947A-4C47-BA81-FD7398DE30D5}">
+  <dimension ref="A1:AL88"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.140625" style="45" customWidth="1"/>
+    <col min="5" max="16384" width="10.7109375" style="45"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="43">
+        <v>1945</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="43">
+        <v>1946</v>
+      </c>
+      <c r="B3" s="44"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="43">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="43">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="43">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="43">
+        <v>1950</v>
+      </c>
+      <c r="B7" s="44">
+        <f>([1]prod!$G7*[1]MatEnergy_PlateGlass!L7)+(([1]prod!$I7+[1]prod!$K7)*[1]MatEnergy_WindowGlass!L7)</f>
+        <v>30.977054117647054</v>
+      </c>
+      <c r="C7" s="44">
+        <f>([1]prod!$G7*[1]MatEnergy_PlateGlass!N7)+(([1]prod!$I7+[1]prod!$K7)*[1]MatEnergy_WindowGlass!N7)</f>
+        <v>0.72907563025210087</v>
+      </c>
+      <c r="D7" s="44">
+        <f>([1]prod!$G7*[1]MatEnergy_PlateGlass!O7)+(([1]prod!$I7+[1]prod!$K7)*[1]MatEnergy_WindowGlass!O7)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="44">
+        <f>SUM(B7:D7)</f>
+        <v>31.706129747899155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="43">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="43">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="43">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="43">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="43">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="43">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="43">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="43">
+        <v>1958</v>
+      </c>
+      <c r="B15" s="46"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="43">
+        <v>1959</v>
+      </c>
+      <c r="B16" s="46"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="43">
+        <v>1960</v>
+      </c>
+      <c r="B17" s="47">
+        <f>0.8*E17</f>
+        <v>16.8</v>
+      </c>
+      <c r="C17" s="47">
+        <f>0.047*E17</f>
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="D17" s="47">
+        <f>0.125*E17</f>
+        <v>2.625</v>
+      </c>
+      <c r="E17" s="50">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="43">
+        <v>1961</v>
+      </c>
+      <c r="E18" s="50"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="43">
+        <v>1962</v>
+      </c>
+      <c r="E19" s="50"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="43">
+        <v>1963</v>
+      </c>
+      <c r="B20" s="46"/>
+      <c r="E20" s="50"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="43">
+        <v>1964</v>
+      </c>
+      <c r="E21" s="50"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="43">
+        <v>1965</v>
+      </c>
+      <c r="B22" s="47">
+        <f>0.79*E22</f>
+        <v>16.6295</v>
+      </c>
+      <c r="C22" s="47">
+        <f>0.055*E22</f>
+        <v>1.1577500000000001</v>
+      </c>
+      <c r="D22" s="47">
+        <f>0.12*E22</f>
+        <v>2.5259999999999998</v>
+      </c>
+      <c r="E22" s="50">
+        <v>21.05</v>
+      </c>
+      <c r="J22" s="51"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="43">
+        <v>1966</v>
+      </c>
+      <c r="E23" s="50"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="43">
+        <v>1967</v>
+      </c>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="50"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="43">
+        <v>1968</v>
+      </c>
+      <c r="B25" s="46"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="50"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="43">
+        <v>1969</v>
+      </c>
+      <c r="E26" s="50"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="43">
+        <v>1970</v>
+      </c>
+      <c r="B27" s="46">
+        <f>0.79*E27</f>
+        <v>15.721</v>
+      </c>
+      <c r="C27" s="46">
+        <f>0.04*E27</f>
+        <v>0.79599999999999993</v>
+      </c>
+      <c r="D27" s="46">
+        <f>0.17*E27</f>
+        <v>3.383</v>
+      </c>
+      <c r="E27" s="50">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="43">
+        <v>1971</v>
+      </c>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="50"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="43">
+        <v>1972</v>
+      </c>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="50"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="43">
+        <v>1973</v>
+      </c>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="50"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="43">
+        <v>1974</v>
+      </c>
+      <c r="E31" s="50"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="43">
+        <v>1975</v>
+      </c>
+      <c r="B32" s="46">
+        <f>0.77*E32</f>
+        <v>13.636700000000001</v>
+      </c>
+      <c r="C32" s="46">
+        <f>0.04*E32</f>
+        <v>0.70840000000000003</v>
+      </c>
+      <c r="D32" s="46">
+        <f>0.18*E32</f>
+        <v>3.1878000000000002</v>
+      </c>
+      <c r="E32" s="50">
+        <v>17.71</v>
+      </c>
+      <c r="J32" s="51"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="43">
+        <v>1976</v>
+      </c>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="50"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="43">
+        <v>1977</v>
+      </c>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="50"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="43">
+        <v>1978</v>
+      </c>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="50"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="43">
+        <v>1979</v>
+      </c>
+      <c r="E36" s="50"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="43">
+        <v>1980</v>
+      </c>
+      <c r="B37" s="46">
+        <f>0.68*E37</f>
+        <v>10.376800000000001</v>
+      </c>
+      <c r="C37" s="46">
+        <f>0.04*E37</f>
+        <v>0.61040000000000005</v>
+      </c>
+      <c r="D37" s="46">
+        <f>0.3*E37</f>
+        <v>4.5779999999999994</v>
+      </c>
+      <c r="E37" s="50">
+        <v>15.26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="43">
+        <v>1981</v>
+      </c>
+      <c r="E38" s="50"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="43">
+        <v>1982</v>
+      </c>
+      <c r="E39" s="50"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="43">
+        <v>1983</v>
+      </c>
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="50"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="43">
+        <v>1984</v>
+      </c>
+      <c r="E41" s="50"/>
+      <c r="J41" s="51"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="43">
+        <v>1985</v>
+      </c>
+      <c r="B42" s="46">
+        <f>0.65*E42</f>
+        <v>8.918000000000001</v>
+      </c>
+      <c r="C42" s="46">
+        <f>0.04*E42</f>
+        <v>0.54880000000000007</v>
+      </c>
+      <c r="D42" s="46">
+        <f>0.3*E42</f>
+        <v>4.1159999999999997</v>
+      </c>
+      <c r="E42" s="50">
+        <v>13.72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="43">
+        <v>1986</v>
+      </c>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="50"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="43">
+        <v>1987</v>
+      </c>
+      <c r="B44" s="46"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="50"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="43">
+        <v>1988</v>
+      </c>
+      <c r="B45" s="46">
+        <f>0.65*E45</f>
+        <v>8.1640000000000015</v>
+      </c>
+      <c r="C45" s="46">
+        <f>0.04*E45</f>
+        <v>0.50240000000000007</v>
+      </c>
+      <c r="D45" s="46">
+        <f>0.3*E45</f>
+        <v>3.7679999999999998</v>
+      </c>
+      <c r="E45" s="50">
+        <v>12.56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="43">
+        <v>1989</v>
+      </c>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="46"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="43">
+        <v>1990</v>
+      </c>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="46"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="43">
+        <v>1991</v>
+      </c>
+      <c r="B48" s="46"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="46"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="43">
+        <v>1992</v>
+      </c>
+      <c r="B49" s="46"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="43">
+        <v>1993</v>
+      </c>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="43">
+        <v>1994</v>
+      </c>
+      <c r="B51" s="44"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="43">
+        <v>1995</v>
+      </c>
+      <c r="B52" s="46">
+        <v>5.01</v>
+      </c>
+      <c r="C52" s="46">
+        <v>1.48</v>
+      </c>
+      <c r="D52" s="46">
+        <v>4.8</v>
+      </c>
+      <c r="E52" s="46">
+        <v>11.3</v>
+      </c>
+      <c r="F52" s="46"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="43">
+        <v>1996</v>
+      </c>
+      <c r="B53" s="46"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="43">
+        <v>1997</v>
+      </c>
+      <c r="B54" s="46"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="43">
+        <v>1998</v>
+      </c>
+      <c r="B55" s="46"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="46"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="46"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="43">
+        <v>1999</v>
+      </c>
+      <c r="B56" s="46"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="43">
+        <v>2000</v>
+      </c>
+      <c r="F57" s="46"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="43">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="43">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="43">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="43">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="43">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="43">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="43">
+        <v>2007</v>
+      </c>
+      <c r="B64" s="46"/>
+      <c r="C64" s="46"/>
+      <c r="D64" s="46"/>
+      <c r="E64" s="46"/>
+    </row>
+    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A65" s="43">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A66" s="43">
+        <v>2009</v>
+      </c>
+      <c r="B66" s="46"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="47"/>
+    </row>
+    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A67" s="43">
+        <v>2010</v>
+      </c>
+      <c r="B67" s="46">
+        <v>2.1</v>
+      </c>
+      <c r="C67" s="46">
+        <v>0.9</v>
+      </c>
+      <c r="D67" s="46">
+        <v>6.1</v>
+      </c>
+      <c r="E67" s="44">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A68" s="43">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A69" s="43">
+        <v>2012</v>
+      </c>
+      <c r="B69" s="46"/>
+      <c r="C69" s="46"/>
+      <c r="D69" s="46"/>
+    </row>
+    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A70" s="43">
+        <v>2013</v>
+      </c>
+      <c r="B70" s="46"/>
+      <c r="C70" s="46"/>
+      <c r="D70" s="46"/>
+    </row>
+    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A71" s="43">
+        <v>2014</v>
+      </c>
+      <c r="B71" s="46"/>
+      <c r="C71" s="46"/>
+      <c r="D71" s="46"/>
+    </row>
+    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A72" s="43">
+        <v>2015</v>
+      </c>
+      <c r="B72" s="46"/>
+      <c r="C72" s="46"/>
+      <c r="D72" s="46"/>
+    </row>
+    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A73" s="43">
+        <v>2016</v>
+      </c>
+      <c r="B73" s="46"/>
+      <c r="C73" s="46"/>
+      <c r="D73" s="46"/>
+    </row>
+    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A74" s="43">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="75" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A75" s="43">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="76" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A76" s="43">
+        <v>2019</v>
+      </c>
+      <c r="B76" s="46">
+        <v>2.1</v>
+      </c>
+      <c r="C76" s="46">
+        <v>0.9</v>
+      </c>
+      <c r="D76" s="46">
+        <v>6.1</v>
+      </c>
+      <c r="E76" s="44">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A77" s="43">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="78" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="48"/>
+      <c r="B78" s="45"/>
+      <c r="C78" s="45"/>
+      <c r="D78" s="45"/>
+      <c r="E78" s="45"/>
+      <c r="F78" s="45"/>
+      <c r="G78" s="45"/>
+      <c r="H78" s="45"/>
+      <c r="I78" s="45"/>
+      <c r="J78" s="45"/>
+      <c r="K78" s="45"/>
+      <c r="L78" s="45"/>
+      <c r="M78" s="45"/>
+      <c r="N78" s="45"/>
+      <c r="O78" s="45"/>
+      <c r="P78" s="45"/>
+      <c r="Q78" s="45"/>
+      <c r="R78" s="45"/>
+      <c r="S78" s="45"/>
+      <c r="T78" s="45"/>
+      <c r="U78" s="45"/>
+      <c r="V78" s="45"/>
+      <c r="W78" s="45"/>
+      <c r="X78" s="45"/>
+      <c r="Y78" s="45"/>
+      <c r="Z78" s="45"/>
+      <c r="AA78" s="45"/>
+      <c r="AB78" s="45"/>
+      <c r="AC78" s="45"/>
+      <c r="AD78" s="45"/>
+      <c r="AE78" s="45"/>
+      <c r="AF78" s="45"/>
+      <c r="AG78" s="45"/>
+      <c r="AH78" s="45"/>
+      <c r="AI78" s="45"/>
+      <c r="AJ78" s="45"/>
+      <c r="AK78" s="45"/>
+      <c r="AL78" s="45"/>
+    </row>
+    <row r="79" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="48"/>
+      <c r="B79" s="45"/>
+      <c r="C79" s="45"/>
+      <c r="D79" s="45"/>
+      <c r="E79" s="45"/>
+      <c r="F79" s="45"/>
+      <c r="G79" s="45"/>
+      <c r="H79" s="45"/>
+      <c r="I79" s="45"/>
+      <c r="J79" s="45"/>
+      <c r="K79" s="45"/>
+      <c r="L79" s="45"/>
+      <c r="M79" s="45"/>
+      <c r="N79" s="45"/>
+      <c r="O79" s="45"/>
+      <c r="P79" s="45"/>
+      <c r="Q79" s="45"/>
+      <c r="R79" s="45"/>
+      <c r="S79" s="45"/>
+      <c r="T79" s="45"/>
+      <c r="U79" s="45"/>
+      <c r="V79" s="45"/>
+      <c r="W79" s="45"/>
+      <c r="X79" s="45"/>
+      <c r="Y79" s="45"/>
+      <c r="Z79" s="45"/>
+      <c r="AA79" s="45"/>
+      <c r="AB79" s="45"/>
+      <c r="AC79" s="45"/>
+      <c r="AD79" s="45"/>
+      <c r="AE79" s="45"/>
+      <c r="AF79" s="45"/>
+      <c r="AG79" s="45"/>
+      <c r="AH79" s="45"/>
+      <c r="AI79" s="45"/>
+      <c r="AJ79" s="45"/>
+      <c r="AK79" s="45"/>
+      <c r="AL79" s="45"/>
+    </row>
+    <row r="80" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="48"/>
+      <c r="B80" s="45"/>
+      <c r="C80" s="45"/>
+      <c r="D80" s="45"/>
+      <c r="E80" s="45"/>
+      <c r="F80" s="45"/>
+      <c r="G80" s="45"/>
+      <c r="H80" s="45"/>
+      <c r="I80" s="45"/>
+      <c r="J80" s="45"/>
+      <c r="K80" s="45"/>
+      <c r="L80" s="45"/>
+      <c r="M80" s="45"/>
+      <c r="N80" s="45"/>
+      <c r="O80" s="45"/>
+      <c r="P80" s="45"/>
+      <c r="Q80" s="45"/>
+      <c r="R80" s="45"/>
+      <c r="S80" s="45"/>
+      <c r="T80" s="45"/>
+      <c r="U80" s="45"/>
+      <c r="V80" s="45"/>
+      <c r="W80" s="45"/>
+      <c r="X80" s="45"/>
+      <c r="Y80" s="45"/>
+      <c r="Z80" s="45"/>
+      <c r="AA80" s="45"/>
+      <c r="AB80" s="45"/>
+      <c r="AC80" s="45"/>
+      <c r="AD80" s="45"/>
+      <c r="AE80" s="45"/>
+      <c r="AF80" s="45"/>
+      <c r="AG80" s="45"/>
+      <c r="AH80" s="45"/>
+      <c r="AI80" s="45"/>
+      <c r="AJ80" s="45"/>
+      <c r="AK80" s="45"/>
+      <c r="AL80" s="45"/>
+    </row>
+    <row r="87" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="48"/>
+      <c r="B87" s="45"/>
+      <c r="C87" s="45"/>
+      <c r="D87" s="45"/>
+      <c r="E87" s="45"/>
+      <c r="F87" s="45"/>
+      <c r="G87" s="45"/>
+      <c r="H87" s="45"/>
+      <c r="I87" s="45"/>
+      <c r="J87" s="45"/>
+      <c r="K87" s="45"/>
+      <c r="L87" s="45"/>
+      <c r="M87" s="45"/>
+      <c r="N87" s="45"/>
+      <c r="O87" s="45"/>
+      <c r="P87" s="45"/>
+      <c r="Q87" s="45"/>
+      <c r="R87" s="45"/>
+      <c r="S87" s="45"/>
+      <c r="T87" s="45"/>
+      <c r="U87" s="45"/>
+      <c r="V87" s="45"/>
+      <c r="W87" s="45"/>
+      <c r="X87" s="45"/>
+      <c r="Y87" s="45"/>
+      <c r="Z87" s="45"/>
+      <c r="AA87" s="45"/>
+      <c r="AB87" s="45"/>
+      <c r="AC87" s="45"/>
+      <c r="AD87" s="45"/>
+      <c r="AE87" s="45"/>
+      <c r="AF87" s="45"/>
+      <c r="AG87" s="45"/>
+      <c r="AH87" s="45"/>
+      <c r="AI87" s="45"/>
+      <c r="AJ87" s="45"/>
+      <c r="AK87" s="45"/>
+      <c r="AL87" s="45"/>
+    </row>
+    <row r="88" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="48"/>
+      <c r="B88" s="45"/>
+      <c r="C88" s="45"/>
+      <c r="D88" s="45"/>
+      <c r="E88" s="45"/>
+      <c r="F88" s="45"/>
+      <c r="G88" s="45"/>
+      <c r="H88" s="45"/>
+      <c r="I88" s="45"/>
+      <c r="J88" s="45"/>
+      <c r="K88" s="45"/>
+      <c r="L88" s="45"/>
+      <c r="M88" s="45"/>
+      <c r="N88" s="45"/>
+      <c r="O88" s="45"/>
+      <c r="P88" s="45"/>
+      <c r="Q88" s="45"/>
+      <c r="R88" s="45"/>
+      <c r="S88" s="45"/>
+      <c r="T88" s="45"/>
+      <c r="U88" s="45"/>
+      <c r="V88" s="45"/>
+      <c r="W88" s="45"/>
+      <c r="X88" s="45"/>
+      <c r="Y88" s="45"/>
+      <c r="Z88" s="45"/>
+      <c r="AA88" s="45"/>
+      <c r="AB88" s="45"/>
+      <c r="AC88" s="45"/>
+      <c r="AD88" s="45"/>
+      <c r="AE88" s="45"/>
+      <c r="AF88" s="45"/>
+      <c r="AG88" s="45"/>
+      <c r="AH88" s="45"/>
+      <c r="AI88" s="45"/>
+      <c r="AJ88" s="45"/>
+      <c r="AK88" s="45"/>
+      <c r="AL88" s="45"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20697ACE-82C7-45F0-9119-243699C7EDD6}">
   <dimension ref="A1:C88"/>
   <sheetViews>

</xml_diff>

<commit_message>
A few data modified
</commit_message>
<xml_diff>
--- a/RawData/BE_RawData_VPython.xlsx
+++ b/RawData/BE_RawData_VPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\01_MFA_GlassIndustry\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795F3120-76E9-485D-8624-B62E05E183EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D91D7C6-7079-4793-AAFF-A2A339B98735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="1170" yWindow="600" windowWidth="16665" windowHeight="15600" activeTab="4" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="19" r:id="rId1"/>
@@ -2667,7 +2667,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2716,9 +2716,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3151,140 +3148,140 @@
   <sheetFormatPr defaultColWidth="118.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81" style="33" customWidth="1"/>
+    <col min="2" max="2" width="27" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81" style="32" customWidth="1"/>
     <col min="4" max="4" width="86.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36" t="s">
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
+    <row r="7" spans="1:4" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="54" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="32" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" s="39"/>
+      <c r="D10" s="38"/>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="38"/>
+      <c r="C12" s="37"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="38" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="38"/>
-      <c r="D14" s="39"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="39"/>
+      <c r="D15" s="38"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="38"/>
-      <c r="D16" s="39"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="38"/>
     </row>
     <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="39"/>
+      <c r="D17" s="38"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="38"/>
-      <c r="D18" s="39"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="38" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="38" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="38"/>
-      <c r="D22" s="39"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="38"/>
     </row>
     <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="39"/>
+      <c r="D23" s="38"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3303,11 +3300,11 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C75" sqref="C75"/>
+      <selection pane="bottomRight" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3319,13 +3316,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="51" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3334,7 +3331,7 @@
         <v>1945</v>
       </c>
       <c r="B2" s="9"/>
-      <c r="C2" s="56">
+      <c r="C2" s="55">
         <v>0.9</v>
       </c>
     </row>
@@ -3369,7 +3366,7 @@
       <c r="B7" s="9">
         <v>206.25</v>
       </c>
-      <c r="C7" s="53">
+      <c r="C7" s="52">
         <v>0.9</v>
       </c>
     </row>
@@ -3425,7 +3422,7 @@
       <c r="A16" s="2">
         <v>1959</v>
       </c>
-      <c r="B16" s="31"/>
+      <c r="B16" s="30"/>
     </row>
     <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -3982,10 +3979,10 @@
   <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView zoomScale="72" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B76" sqref="B76"/>
+      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3995,145 +3992,146 @@
     <col min="3" max="16384" width="13.5703125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1945</v>
       </c>
-      <c r="B2" s="23"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="22"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>1946</v>
       </c>
-      <c r="B3" s="23"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="22"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>1947</v>
       </c>
-      <c r="B4" s="23"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="22"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>1948</v>
       </c>
-      <c r="B5" s="23"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="22"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>1949</v>
       </c>
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="22"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>1950</v>
       </c>
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="22"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>1951</v>
       </c>
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="22"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>1952</v>
       </c>
-      <c r="B9" s="23"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>1953</v>
       </c>
-      <c r="B10" s="23"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="22"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>1954</v>
       </c>
-      <c r="B11" s="23"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="22"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>1955</v>
       </c>
-      <c r="B12" s="23"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="22"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>1956</v>
       </c>
-      <c r="B13" s="23"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>1957</v>
       </c>
-      <c r="B14" s="23"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>1958</v>
       </c>
       <c r="B15" s="8">
         <v>4.7309999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="24"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>1959</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="22"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>1960</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="22">
         <f>14+1</f>
         <v>15</v>
       </c>
-      <c r="C17" s="17"/>
+      <c r="C17" s="24"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>1961</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="22">
         <f>4+1</f>
         <v>5</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="24"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>1962</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="22">
         <f>11+1</f>
         <v>12</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="24"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>1963</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="22">
         <f>7+1</f>
         <v>8</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="24"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
@@ -4142,7 +4140,7 @@
       <c r="B21" s="8">
         <v>22.033999999999999</v>
       </c>
-      <c r="C21" s="17"/>
+      <c r="C21" s="24"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
@@ -4151,47 +4149,47 @@
       <c r="B22" s="8">
         <v>24.206</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="C22" s="24"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>1966</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="22">
         <f>32+3</f>
         <v>35</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="24"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>1967</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="22">
         <f>26+1</f>
         <v>27</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="24"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>1968</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B25" s="22">
         <f>31+3</f>
         <v>34</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="24"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>1969</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="22">
         <f>30+6</f>
         <v>36</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="24"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
@@ -4201,117 +4199,117 @@
         <f>30+7</f>
         <v>37</v>
       </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="24"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>1971</v>
       </c>
-      <c r="B28" s="23">
+      <c r="B28" s="22">
         <f>29+9</f>
         <v>38</v>
       </c>
-      <c r="C28" s="17"/>
+      <c r="C28" s="24"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>1972</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B29" s="22">
         <f>38+7</f>
         <v>45</v>
       </c>
-      <c r="C29" s="17"/>
+      <c r="C29" s="24"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>1973</v>
       </c>
-      <c r="B30" s="23">
+      <c r="B30" s="22">
         <f>50+9</f>
         <v>59</v>
       </c>
-      <c r="C30" s="17"/>
+      <c r="C30" s="24"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>1974</v>
       </c>
-      <c r="B31" s="23">
+      <c r="B31" s="22">
         <f>51+7</f>
         <v>58</v>
       </c>
-      <c r="C31" s="17"/>
+      <c r="C31" s="24"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>1975</v>
       </c>
-      <c r="B32" s="23">
+      <c r="B32" s="22">
         <f>46+7</f>
         <v>53</v>
       </c>
-      <c r="C32" s="17"/>
+      <c r="C32" s="24"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>1976</v>
       </c>
-      <c r="B33" s="23">
+      <c r="B33" s="22">
         <f>75+10</f>
         <v>85</v>
       </c>
-      <c r="C33" s="17"/>
+      <c r="C33" s="24"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>1977</v>
       </c>
-      <c r="B34" s="23">
+      <c r="B34" s="22">
         <f>84+14</f>
         <v>98</v>
       </c>
-      <c r="C34" s="17"/>
+      <c r="C34" s="24"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>1978</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="22">
         <f>77+14</f>
         <v>91</v>
       </c>
-      <c r="C35" s="17"/>
+      <c r="C35" s="24"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
         <v>1979</v>
       </c>
-      <c r="B36" s="23">
+      <c r="B36" s="22">
         <f>94+16</f>
         <v>110</v>
       </c>
-      <c r="C36" s="17"/>
+      <c r="C36" s="24"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>1980</v>
       </c>
-      <c r="B37" s="23">
+      <c r="B37" s="22">
         <f>111+20</f>
         <v>131</v>
       </c>
-      <c r="C37" s="17"/>
+      <c r="C37" s="24"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
         <v>1981</v>
       </c>
-      <c r="B38" s="23">
+      <c r="B38" s="22">
         <f>110+18</f>
         <v>128</v>
       </c>
-      <c r="C38" s="17"/>
+      <c r="C38" s="24"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
@@ -4321,7 +4319,7 @@
         <f>154+17</f>
         <v>171</v>
       </c>
-      <c r="C39" s="17"/>
+      <c r="C39" s="24"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
@@ -4331,7 +4329,7 @@
         <f>138+17</f>
         <v>155</v>
       </c>
-      <c r="C40" s="17"/>
+      <c r="C40" s="24"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
@@ -4341,7 +4339,7 @@
         <f>118+18</f>
         <v>136</v>
       </c>
-      <c r="C41" s="17"/>
+      <c r="C41" s="24"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
@@ -4351,7 +4349,7 @@
         <f>131+20</f>
         <v>151</v>
       </c>
-      <c r="C42" s="17"/>
+      <c r="C42" s="24"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
@@ -4361,89 +4359,86 @@
         <f>136+24</f>
         <v>160</v>
       </c>
-      <c r="C43" s="17"/>
+      <c r="C43" s="24"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
         <v>1987</v>
       </c>
-      <c r="B44" s="23">
+      <c r="B44" s="22">
         <f>166+30</f>
         <v>196</v>
       </c>
-      <c r="C44" s="17"/>
+      <c r="C44" s="24"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
         <v>1988</v>
       </c>
-      <c r="B45" s="23">
+      <c r="B45" s="22">
         <f>156+44</f>
         <v>200</v>
       </c>
-      <c r="C45" s="17"/>
+      <c r="C45" s="24"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>1989</v>
       </c>
-      <c r="B46" s="23">
+      <c r="B46" s="22">
         <f>155+49</f>
         <v>204</v>
       </c>
-      <c r="C46" s="17"/>
+      <c r="C46" s="24"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
         <v>1990</v>
       </c>
-      <c r="B47" s="23">
+      <c r="B47" s="22">
         <f>142+45</f>
         <v>187</v>
       </c>
-      <c r="C47" s="17"/>
+      <c r="C47" s="24"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
         <v>1991</v>
       </c>
-      <c r="B48" s="23">
+      <c r="B48" s="22">
         <f>163+46</f>
         <v>209</v>
       </c>
-      <c r="C48" s="17"/>
+      <c r="C48" s="24"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
         <v>1992</v>
       </c>
-      <c r="B49" s="23">
+      <c r="B49" s="22">
         <f>182+48</f>
         <v>230</v>
       </c>
-      <c r="C49" s="17"/>
+      <c r="C49" s="24"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>1993</v>
       </c>
-      <c r="B50" s="23">
-        <f>124+38</f>
-        <v>162</v>
-      </c>
-      <c r="C50" s="17"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="24"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>1994</v>
       </c>
-      <c r="B51" s="23"/>
+      <c r="B51" s="22"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>1995</v>
       </c>
-      <c r="B52" s="23"/>
+      <c r="B52" s="22"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
@@ -4452,6 +4447,7 @@
       <c r="B53" s="8">
         <v>227.74783500000004</v>
       </c>
+      <c r="C53" s="24"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
@@ -4460,6 +4456,7 @@
       <c r="B54" s="8">
         <v>144.56236999999996</v>
       </c>
+      <c r="C54" s="24"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
@@ -4468,6 +4465,7 @@
       <c r="B55" s="8">
         <v>219.30247999999997</v>
       </c>
+      <c r="C55" s="24"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
@@ -4476,6 +4474,7 @@
       <c r="B56" s="8">
         <v>257.18237499999998</v>
       </c>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
@@ -4484,7 +4483,7 @@
       <c r="B57" s="8">
         <v>250.85938999999999</v>
       </c>
-      <c r="C57" s="25"/>
+      <c r="C57" s="24"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="16">
@@ -4493,7 +4492,7 @@
       <c r="B58" s="8">
         <v>238.67235000000002</v>
       </c>
-      <c r="C58" s="25"/>
+      <c r="C58" s="24"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="16">
@@ -4502,7 +4501,7 @@
       <c r="B59" s="8">
         <v>245.98853500000001</v>
       </c>
-      <c r="C59" s="25"/>
+      <c r="C59" s="24"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="16">
@@ -4511,7 +4510,7 @@
       <c r="B60" s="8">
         <v>262.16664499999996</v>
       </c>
-      <c r="C60" s="25"/>
+      <c r="C60" s="24"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="16">
@@ -4520,7 +4519,7 @@
       <c r="B61" s="8">
         <v>270.80542999999994</v>
       </c>
-      <c r="C61" s="25"/>
+      <c r="C61" s="24"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="16">
@@ -4529,7 +4528,7 @@
       <c r="B62" s="8">
         <v>272.66947499999998</v>
       </c>
-      <c r="C62" s="25"/>
+      <c r="C62" s="24"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="16">
@@ -4538,7 +4537,7 @@
       <c r="B63" s="8">
         <v>286.68788999999992</v>
       </c>
-      <c r="C63" s="25"/>
+      <c r="C63" s="24"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
@@ -4547,7 +4546,7 @@
       <c r="B64" s="8">
         <v>327.98110000000008</v>
       </c>
-      <c r="C64" s="25"/>
+      <c r="C64" s="24"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="16">
@@ -4556,7 +4555,7 @@
       <c r="B65" s="8">
         <v>298.70961000000005</v>
       </c>
-      <c r="C65" s="25"/>
+      <c r="C65" s="24"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="16">
@@ -4565,7 +4564,7 @@
       <c r="B66" s="8">
         <v>226.05818500000001</v>
       </c>
-      <c r="C66" s="25"/>
+      <c r="C66" s="24"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="16">
@@ -4574,7 +4573,7 @@
       <c r="B67" s="8">
         <v>291.62551499999995</v>
       </c>
-      <c r="C67" s="25"/>
+      <c r="C67" s="24"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="16">
@@ -4583,7 +4582,7 @@
       <c r="B68" s="8">
         <v>276.16961000000003</v>
       </c>
-      <c r="C68" s="25"/>
+      <c r="C68" s="24"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="16">
@@ -4592,7 +4591,7 @@
       <c r="B69" s="8">
         <v>238.987775</v>
       </c>
-      <c r="C69" s="25"/>
+      <c r="C69" s="24"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="16">
@@ -4601,7 +4600,7 @@
       <c r="B70" s="8">
         <v>273.47733999999997</v>
       </c>
-      <c r="C70" s="25"/>
+      <c r="C70" s="24"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="16">
@@ -4610,7 +4609,7 @@
       <c r="B71" s="8">
         <v>240.30352999999999</v>
       </c>
-      <c r="C71" s="25"/>
+      <c r="C71" s="24"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="16">
@@ -4619,7 +4618,7 @@
       <c r="B72" s="8">
         <v>224.46110999999999</v>
       </c>
-      <c r="C72" s="25"/>
+      <c r="C72" s="24"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="16">
@@ -4628,7 +4627,7 @@
       <c r="B73" s="8">
         <v>216.26886500000001</v>
       </c>
-      <c r="C73" s="25"/>
+      <c r="C73" s="24"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="16">
@@ -4637,7 +4636,7 @@
       <c r="B74" s="8">
         <v>230.95865499999996</v>
       </c>
-      <c r="C74" s="25"/>
+      <c r="C74" s="24"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="16">
@@ -4646,32 +4645,32 @@
       <c r="B75" s="8">
         <v>228.64879500000001</v>
       </c>
-      <c r="C75" s="25"/>
+      <c r="C75" s="24"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="16">
         <v>2019</v>
       </c>
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="24"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="16">
         <v>2020</v>
       </c>
-      <c r="C77" s="25"/>
+      <c r="C77" s="24"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C78" s="25"/>
+      <c r="C78" s="24"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C79" s="25"/>
+      <c r="C79" s="24"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C80" s="25"/>
+      <c r="C80" s="24"/>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81" s="25"/>
+      <c r="C81" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4686,10 +4685,10 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B76" sqref="B76"/>
+      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4700,10 +4699,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4835,7 +4834,7 @@
         <f>12*38.486</f>
         <v>461.83199999999999</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4846,7 +4845,7 @@
         <f>12*32.923</f>
         <v>395.07600000000002</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4857,7 +4856,7 @@
         <f>12*39.034</f>
         <v>468.40800000000002</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4868,7 +4867,7 @@
         <f>12*36.272</f>
         <v>435.26400000000001</v>
       </c>
-      <c r="C20" s="10"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4879,7 +4878,7 @@
         <f>12*40.991</f>
         <v>491.892</v>
       </c>
-      <c r="C21" s="10"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4890,7 +4889,7 @@
         <f>12*34.918</f>
         <v>419.01599999999996</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="10"/>
     </row>
     <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4901,7 +4900,7 @@
         <f>328+66</f>
         <v>394</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4912,7 +4911,7 @@
         <f>315+72</f>
         <v>387</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4923,7 +4922,7 @@
         <f>354+76</f>
         <v>430</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4934,7 +4933,7 @@
         <f>369+82</f>
         <v>451</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4945,7 +4944,7 @@
         <f>479+92</f>
         <v>571</v>
       </c>
-      <c r="C27" s="10"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4956,7 +4955,7 @@
         <f>425+97</f>
         <v>522</v>
       </c>
-      <c r="C28" s="10"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4967,7 +4966,7 @@
         <f>498+101</f>
         <v>599</v>
       </c>
-      <c r="C29" s="10"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4978,7 +4977,7 @@
         <f>500+102</f>
         <v>602</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4989,7 +4988,7 @@
         <f>457+90</f>
         <v>547</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="24"/>
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5000,7 +4999,7 @@
         <f>304+80</f>
         <v>384</v>
       </c>
-      <c r="C32" s="10"/>
+      <c r="C32" s="24"/>
       <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5011,7 +5010,7 @@
         <f>447+89</f>
         <v>536</v>
       </c>
-      <c r="C33" s="10"/>
+      <c r="C33" s="24"/>
       <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5022,7 +5021,7 @@
         <f>497+78</f>
         <v>575</v>
       </c>
-      <c r="C34" s="10"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5033,7 +5032,7 @@
         <f>572+89</f>
         <v>661</v>
       </c>
-      <c r="C35" s="10"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5044,7 +5043,7 @@
         <f>578+96</f>
         <v>674</v>
       </c>
-      <c r="C36" s="10"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5055,7 +5054,7 @@
         <f>576+113</f>
         <v>689</v>
       </c>
-      <c r="C37" s="10"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5066,7 +5065,7 @@
         <f>519+101</f>
         <v>620</v>
       </c>
-      <c r="C38" s="10"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5077,7 +5076,7 @@
         <f>601+108</f>
         <v>709</v>
       </c>
-      <c r="C39" s="10"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5088,7 +5087,7 @@
         <f>645+124</f>
         <v>769</v>
       </c>
-      <c r="C40" s="10"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5099,7 +5098,7 @@
         <f>718+142</f>
         <v>860</v>
       </c>
-      <c r="C41" s="10"/>
+      <c r="C41" s="24"/>
       <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5110,7 +5109,7 @@
         <f>688+153</f>
         <v>841</v>
       </c>
-      <c r="C42" s="10"/>
+      <c r="C42" s="24"/>
       <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5121,7 +5120,7 @@
         <f>726+167</f>
         <v>893</v>
       </c>
-      <c r="C43" s="10"/>
+      <c r="C43" s="24"/>
       <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5132,7 +5131,7 @@
         <f>770+194</f>
         <v>964</v>
       </c>
-      <c r="C44" s="10"/>
+      <c r="C44" s="24"/>
       <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5143,7 +5142,7 @@
         <f>757+229</f>
         <v>986</v>
       </c>
-      <c r="C45" s="10"/>
+      <c r="C45" s="24"/>
       <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5154,7 +5153,7 @@
         <f>934+252</f>
         <v>1186</v>
       </c>
-      <c r="C46" s="10"/>
+      <c r="C46" s="24"/>
       <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5165,8 +5164,8 @@
         <f>961+239</f>
         <v>1200</v>
       </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="15"/>
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
@@ -5176,7 +5175,7 @@
         <f>836+232</f>
         <v>1068</v>
       </c>
-      <c r="C48" s="10"/>
+      <c r="C48" s="24"/>
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5187,18 +5186,15 @@
         <f>846+229</f>
         <v>1075</v>
       </c>
-      <c r="C49" s="10"/>
+      <c r="C49" s="24"/>
       <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>1993</v>
       </c>
-      <c r="B50" s="4">
-        <f>928+265</f>
-        <v>1193</v>
-      </c>
-      <c r="C50" s="10"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="24"/>
       <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5206,6 +5202,7 @@
         <v>1994</v>
       </c>
       <c r="B51" s="8"/>
+      <c r="C51" s="24"/>
       <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5293,6 +5290,7 @@
       <c r="B60" s="8">
         <v>1035.6898874999999</v>
       </c>
+      <c r="C60" s="24"/>
       <c r="D60" s="10"/>
     </row>
     <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5302,7 +5300,7 @@
       <c r="B61" s="8">
         <v>1041.0621912500001</v>
       </c>
-      <c r="C61" s="29"/>
+      <c r="C61" s="24"/>
       <c r="D61" s="10"/>
     </row>
     <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5312,7 +5310,7 @@
       <c r="B62" s="8">
         <v>1017.1818999999999</v>
       </c>
-      <c r="C62" s="29"/>
+      <c r="C62" s="24"/>
       <c r="D62" s="10"/>
     </row>
     <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5323,7 +5321,7 @@
         <v>1042.5845850000003</v>
       </c>
       <c r="C63" s="24"/>
-      <c r="D63" s="29"/>
+      <c r="D63" s="28"/>
     </row>
     <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12">
@@ -5392,7 +5390,7 @@
       <c r="B70" s="8">
         <v>791.69499749999989</v>
       </c>
-      <c r="C70" s="24"/>
+      <c r="C70" s="23"/>
       <c r="D70" s="10"/>
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5402,7 +5400,7 @@
       <c r="B71" s="8">
         <v>634.72707749999995</v>
       </c>
-      <c r="C71" s="24"/>
+      <c r="C71" s="23"/>
       <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5412,7 +5410,7 @@
       <c r="B72" s="8">
         <v>643.42857000000015</v>
       </c>
-      <c r="C72" s="24"/>
+      <c r="C72" s="23"/>
       <c r="D72" s="10"/>
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5422,7 +5420,7 @@
       <c r="B73" s="8">
         <v>499.78879875000001</v>
       </c>
-      <c r="C73" s="24"/>
+      <c r="C73" s="23"/>
       <c r="D73" s="10"/>
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5432,7 +5430,7 @@
       <c r="B74" s="8">
         <v>547.19474625000009</v>
       </c>
-      <c r="C74" s="24"/>
+      <c r="C74" s="23"/>
       <c r="D74" s="10"/>
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5442,7 +5440,7 @@
       <c r="B75" s="8">
         <v>547.75624375000007</v>
       </c>
-      <c r="C75" s="24"/>
+      <c r="C75" s="23"/>
       <c r="D75" s="10"/>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5502,905 +5500,905 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7426F8F2-947A-4C47-BA81-FD7398DE30D5}">
   <dimension ref="A1:AL88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="15.140625" style="45" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="45"/>
+    <col min="1" max="1" width="8" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.140625" style="44" customWidth="1"/>
+    <col min="5" max="16384" width="10.7109375" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:5" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="40" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="43">
+      <c r="A2" s="42">
         <v>1945</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="43">
+      <c r="A3" s="42">
         <v>1946</v>
       </c>
-      <c r="B3" s="44"/>
+      <c r="B3" s="43"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="43">
+      <c r="A4" s="42">
         <v>1947</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="43">
+      <c r="A5" s="42">
         <v>1948</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="43">
+      <c r="A6" s="42">
         <v>1949</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="43">
+      <c r="A7" s="42">
         <v>1950</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="43">
         <v>30.98</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="43">
         <v>0.73</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="43">
         <v>0</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="43">
         <f>SUM(B7:D7)</f>
         <v>31.71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="43">
+      <c r="A8" s="42">
         <v>1951</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="43">
+      <c r="A9" s="42">
         <v>1952</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="43">
+      <c r="A10" s="42">
         <v>1953</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="43">
+      <c r="A11" s="42">
         <v>1954</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="43">
+      <c r="A12" s="42">
         <v>1955</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="43">
+      <c r="A13" s="42">
         <v>1956</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="43">
+      <c r="A14" s="42">
         <v>1957</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="43">
+      <c r="A15" s="42">
         <v>1958</v>
       </c>
-      <c r="B15" s="46"/>
+      <c r="B15" s="45"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="43">
+      <c r="A16" s="42">
         <v>1959</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="45"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="43">
+      <c r="A17" s="42">
         <v>1960</v>
       </c>
-      <c r="B17" s="47">
+      <c r="B17" s="46">
         <f>0.8*E17</f>
         <v>16.8</v>
       </c>
-      <c r="C17" s="47">
+      <c r="C17" s="46">
         <f>0.047*E17</f>
         <v>0.98699999999999999</v>
       </c>
-      <c r="D17" s="47">
+      <c r="D17" s="46">
         <f>0.125*E17</f>
         <v>2.625</v>
       </c>
-      <c r="E17" s="50">
+      <c r="E17" s="49">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="43">
+      <c r="A18" s="42">
         <v>1961</v>
       </c>
-      <c r="E18" s="50"/>
+      <c r="E18" s="49"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="43">
+      <c r="A19" s="42">
         <v>1962</v>
       </c>
-      <c r="E19" s="50"/>
+      <c r="E19" s="49"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="43">
+      <c r="A20" s="42">
         <v>1963</v>
       </c>
-      <c r="B20" s="46"/>
-      <c r="E20" s="50"/>
+      <c r="B20" s="45"/>
+      <c r="E20" s="49"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="43">
+      <c r="A21" s="42">
         <v>1964</v>
       </c>
-      <c r="E21" s="50"/>
+      <c r="E21" s="49"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="43">
+      <c r="A22" s="42">
         <v>1965</v>
       </c>
-      <c r="B22" s="47">
+      <c r="B22" s="46">
         <f>0.79*E22</f>
         <v>16.6295</v>
       </c>
-      <c r="C22" s="47">
+      <c r="C22" s="46">
         <f>0.055*E22</f>
         <v>1.1577500000000001</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="46">
         <f>0.12*E22</f>
         <v>2.5259999999999998</v>
       </c>
-      <c r="E22" s="50">
+      <c r="E22" s="49">
         <v>21.05</v>
       </c>
-      <c r="J22" s="51"/>
+      <c r="J22" s="50"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="43">
+      <c r="A23" s="42">
         <v>1966</v>
       </c>
-      <c r="E23" s="50"/>
+      <c r="E23" s="49"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="43">
+      <c r="A24" s="42">
         <v>1967</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="50"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="49"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="43">
+      <c r="A25" s="42">
         <v>1968</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="50"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="49"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="43">
+      <c r="A26" s="42">
         <v>1969</v>
       </c>
-      <c r="E26" s="50"/>
+      <c r="E26" s="49"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="43">
+      <c r="A27" s="42">
         <v>1970</v>
       </c>
-      <c r="B27" s="46">
+      <c r="B27" s="45">
         <f>0.79*E27</f>
         <v>15.721</v>
       </c>
-      <c r="C27" s="46">
+      <c r="C27" s="45">
         <f>0.04*E27</f>
         <v>0.79599999999999993</v>
       </c>
-      <c r="D27" s="46">
+      <c r="D27" s="45">
         <f>0.17*E27</f>
         <v>3.383</v>
       </c>
-      <c r="E27" s="50">
+      <c r="E27" s="49">
         <v>19.899999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="43">
+      <c r="A28" s="42">
         <v>1971</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="50"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="49"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="43">
+      <c r="A29" s="42">
         <v>1972</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="50"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="49"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="43">
+      <c r="A30" s="42">
         <v>1973</v>
       </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="50"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="49"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="43">
+      <c r="A31" s="42">
         <v>1974</v>
       </c>
-      <c r="E31" s="50"/>
+      <c r="E31" s="49"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="43">
+      <c r="A32" s="42">
         <v>1975</v>
       </c>
-      <c r="B32" s="46">
+      <c r="B32" s="45">
         <f>0.77*E32</f>
         <v>13.636700000000001</v>
       </c>
-      <c r="C32" s="46">
+      <c r="C32" s="45">
         <f>0.04*E32</f>
         <v>0.70840000000000003</v>
       </c>
-      <c r="D32" s="46">
+      <c r="D32" s="45">
         <f>0.18*E32</f>
         <v>3.1878000000000002</v>
       </c>
-      <c r="E32" s="50">
+      <c r="E32" s="49">
         <v>17.71</v>
       </c>
-      <c r="J32" s="51"/>
+      <c r="J32" s="50"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="43">
+      <c r="A33" s="42">
         <v>1976</v>
       </c>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="50"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="49"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="43">
+      <c r="A34" s="42">
         <v>1977</v>
       </c>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="50"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="49"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="43">
+      <c r="A35" s="42">
         <v>1978</v>
       </c>
-      <c r="B35" s="46"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="50"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="49"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="43">
+      <c r="A36" s="42">
         <v>1979</v>
       </c>
-      <c r="E36" s="50"/>
+      <c r="E36" s="49"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="43">
+      <c r="A37" s="42">
         <v>1980</v>
       </c>
-      <c r="B37" s="46">
+      <c r="B37" s="45">
         <f>0.68*E37</f>
         <v>10.376800000000001</v>
       </c>
-      <c r="C37" s="46">
+      <c r="C37" s="45">
         <f>0.04*E37</f>
         <v>0.61040000000000005</v>
       </c>
-      <c r="D37" s="46">
+      <c r="D37" s="45">
         <f>0.3*E37</f>
         <v>4.5779999999999994</v>
       </c>
-      <c r="E37" s="50">
+      <c r="E37" s="49">
         <v>15.26</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="43">
+      <c r="A38" s="42">
         <v>1981</v>
       </c>
-      <c r="E38" s="50"/>
+      <c r="E38" s="49"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="43">
+      <c r="A39" s="42">
         <v>1982</v>
       </c>
-      <c r="E39" s="50"/>
+      <c r="E39" s="49"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="43">
+      <c r="A40" s="42">
         <v>1983</v>
       </c>
-      <c r="B40" s="46"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="50"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="49"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="43">
+      <c r="A41" s="42">
         <v>1984</v>
       </c>
-      <c r="E41" s="50"/>
-      <c r="J41" s="51"/>
+      <c r="E41" s="49"/>
+      <c r="J41" s="50"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="43">
+      <c r="A42" s="42">
         <v>1985</v>
       </c>
-      <c r="B42" s="46">
+      <c r="B42" s="45">
         <f>0.65*E42</f>
         <v>8.918000000000001</v>
       </c>
-      <c r="C42" s="46">
+      <c r="C42" s="45">
         <f>0.04*E42</f>
         <v>0.54880000000000007</v>
       </c>
-      <c r="D42" s="46">
+      <c r="D42" s="45">
         <f>0.3*E42</f>
         <v>4.1159999999999997</v>
       </c>
-      <c r="E42" s="50">
+      <c r="E42" s="49">
         <v>13.72</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="43">
+      <c r="A43" s="42">
         <v>1986</v>
       </c>
-      <c r="B43" s="46"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="50"/>
+      <c r="B43" s="45"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="49"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="43">
+      <c r="A44" s="42">
         <v>1987</v>
       </c>
-      <c r="B44" s="46"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="50"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="49"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="43">
+      <c r="A45" s="42">
         <v>1988</v>
       </c>
-      <c r="B45" s="46">
+      <c r="B45" s="45">
         <f>0.65*E45</f>
         <v>8.1640000000000015</v>
       </c>
-      <c r="C45" s="46">
+      <c r="C45" s="45">
         <f>0.04*E45</f>
         <v>0.50240000000000007</v>
       </c>
-      <c r="D45" s="46">
+      <c r="D45" s="45">
         <f>0.3*E45</f>
         <v>3.7679999999999998</v>
       </c>
-      <c r="E45" s="50">
+      <c r="E45" s="49">
         <v>12.56</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="43">
+      <c r="A46" s="42">
         <v>1989</v>
       </c>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="46"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="45"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="43">
+      <c r="A47" s="42">
         <v>1990</v>
       </c>
-      <c r="B47" s="46"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="46"/>
+      <c r="B47" s="45"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="45"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="43">
+      <c r="A48" s="42">
         <v>1991</v>
       </c>
-      <c r="B48" s="46"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="46"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="45"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="43">
+      <c r="A49" s="42">
         <v>1992</v>
       </c>
-      <c r="B49" s="46"/>
-      <c r="C49" s="46"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="46"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="43">
+      <c r="A50" s="42">
         <v>1993</v>
       </c>
-      <c r="B50" s="46"/>
-      <c r="C50" s="46"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="46"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="43">
+      <c r="A51" s="42">
         <v>1994</v>
       </c>
-      <c r="B51" s="44"/>
-      <c r="C51" s="46"/>
-      <c r="D51" s="46"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="46"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="43">
+      <c r="A52" s="42">
         <v>1995</v>
       </c>
-      <c r="B52" s="46">
+      <c r="B52" s="45">
         <v>5.01</v>
       </c>
-      <c r="C52" s="46">
+      <c r="C52" s="45">
         <v>1.48</v>
       </c>
-      <c r="D52" s="46">
+      <c r="D52" s="45">
         <v>4.8</v>
       </c>
-      <c r="E52" s="46">
+      <c r="E52" s="45">
         <v>11.3</v>
       </c>
-      <c r="F52" s="46"/>
+      <c r="F52" s="45"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="43">
+      <c r="A53" s="42">
         <v>1996</v>
       </c>
-      <c r="B53" s="46"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="46"/>
-      <c r="F53" s="46"/>
+      <c r="B53" s="45"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="45"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="43">
+      <c r="A54" s="42">
         <v>1997</v>
       </c>
-      <c r="B54" s="46"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="46"/>
-      <c r="F54" s="46"/>
+      <c r="B54" s="45"/>
+      <c r="C54" s="45"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="45"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="43">
+      <c r="A55" s="42">
         <v>1998</v>
       </c>
-      <c r="B55" s="46"/>
-      <c r="C55" s="46"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="46"/>
+      <c r="B55" s="45"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="45"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="43">
+      <c r="A56" s="42">
         <v>1999</v>
       </c>
-      <c r="B56" s="46"/>
-      <c r="C56" s="46"/>
-      <c r="D56" s="46"/>
-      <c r="E56" s="46"/>
-      <c r="F56" s="46"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="45"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="43">
+      <c r="A57" s="42">
         <v>2000</v>
       </c>
-      <c r="F57" s="46"/>
+      <c r="F57" s="45"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="43">
+      <c r="A58" s="42">
         <v>2001</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="43">
+      <c r="A59" s="42">
         <v>2002</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="43">
+      <c r="A60" s="42">
         <v>2003</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="43">
+      <c r="A61" s="42">
         <v>2004</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="43">
+      <c r="A62" s="42">
         <v>2005</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="43">
+      <c r="A63" s="42">
         <v>2006</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="43">
+      <c r="A64" s="42">
         <v>2007</v>
       </c>
-      <c r="B64" s="46"/>
-      <c r="C64" s="46"/>
-      <c r="D64" s="46"/>
-      <c r="E64" s="46"/>
+      <c r="B64" s="45"/>
+      <c r="C64" s="45"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="45"/>
     </row>
     <row r="65" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A65" s="43">
+      <c r="A65" s="42">
         <v>2008</v>
       </c>
     </row>
     <row r="66" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A66" s="43">
+      <c r="A66" s="42">
         <v>2009</v>
       </c>
-      <c r="B66" s="46"/>
-      <c r="C66" s="46"/>
-      <c r="D66" s="46"/>
-      <c r="E66" s="47"/>
+      <c r="B66" s="45"/>
+      <c r="C66" s="45"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="46"/>
     </row>
     <row r="67" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A67" s="43">
+      <c r="A67" s="42">
         <v>2010</v>
       </c>
-      <c r="B67" s="46">
+      <c r="B67" s="45">
         <v>2.1</v>
       </c>
-      <c r="C67" s="46">
+      <c r="C67" s="45">
         <v>0.9</v>
       </c>
-      <c r="D67" s="46">
+      <c r="D67" s="45">
         <v>6.1</v>
       </c>
-      <c r="E67" s="44">
+      <c r="E67" s="43">
         <v>9.1</v>
       </c>
     </row>
     <row r="68" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A68" s="43">
+      <c r="A68" s="42">
         <v>2011</v>
       </c>
     </row>
     <row r="69" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A69" s="43">
+      <c r="A69" s="42">
         <v>2012</v>
       </c>
-      <c r="B69" s="46"/>
-      <c r="C69" s="46"/>
-      <c r="D69" s="46"/>
+      <c r="B69" s="45"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="45"/>
     </row>
     <row r="70" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A70" s="43">
+      <c r="A70" s="42">
         <v>2013</v>
       </c>
-      <c r="B70" s="46"/>
-      <c r="C70" s="46"/>
-      <c r="D70" s="46"/>
+      <c r="B70" s="45"/>
+      <c r="C70" s="45"/>
+      <c r="D70" s="45"/>
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A71" s="43">
+      <c r="A71" s="42">
         <v>2014</v>
       </c>
-      <c r="B71" s="46"/>
-      <c r="C71" s="46"/>
-      <c r="D71" s="46"/>
+      <c r="B71" s="45"/>
+      <c r="C71" s="45"/>
+      <c r="D71" s="45"/>
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A72" s="43">
+      <c r="A72" s="42">
         <v>2015</v>
       </c>
-      <c r="B72" s="46"/>
-      <c r="C72" s="46"/>
-      <c r="D72" s="46"/>
+      <c r="B72" s="45"/>
+      <c r="C72" s="45"/>
+      <c r="D72" s="45"/>
     </row>
     <row r="73" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A73" s="43">
+      <c r="A73" s="42">
         <v>2016</v>
       </c>
-      <c r="B73" s="46"/>
-      <c r="C73" s="46"/>
-      <c r="D73" s="46"/>
+      <c r="B73" s="45"/>
+      <c r="C73" s="45"/>
+      <c r="D73" s="45"/>
     </row>
     <row r="74" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A74" s="43">
+      <c r="A74" s="42">
         <v>2017</v>
       </c>
     </row>
     <row r="75" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A75" s="43">
+      <c r="A75" s="42">
         <v>2018</v>
       </c>
     </row>
     <row r="76" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A76" s="43">
+      <c r="A76" s="42">
         <v>2019</v>
       </c>
-      <c r="B76" s="46">
+      <c r="B76" s="45">
         <v>2.1</v>
       </c>
-      <c r="C76" s="46">
+      <c r="C76" s="45">
         <v>0.9</v>
       </c>
-      <c r="D76" s="46">
+      <c r="D76" s="45">
         <v>6.1</v>
       </c>
-      <c r="E76" s="44">
+      <c r="E76" s="43">
         <v>9.1</v>
       </c>
     </row>
     <row r="77" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A77" s="43">
+      <c r="A77" s="42">
         <v>2020</v>
       </c>
     </row>
-    <row r="78" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="48"/>
-      <c r="B78" s="45"/>
-      <c r="C78" s="45"/>
-      <c r="D78" s="45"/>
-      <c r="E78" s="45"/>
-      <c r="F78" s="45"/>
-      <c r="G78" s="45"/>
-      <c r="H78" s="45"/>
-      <c r="I78" s="45"/>
-      <c r="J78" s="45"/>
-      <c r="K78" s="45"/>
-      <c r="L78" s="45"/>
-      <c r="M78" s="45"/>
-      <c r="N78" s="45"/>
-      <c r="O78" s="45"/>
-      <c r="P78" s="45"/>
-      <c r="Q78" s="45"/>
-      <c r="R78" s="45"/>
-      <c r="S78" s="45"/>
-      <c r="T78" s="45"/>
-      <c r="U78" s="45"/>
-      <c r="V78" s="45"/>
-      <c r="W78" s="45"/>
-      <c r="X78" s="45"/>
-      <c r="Y78" s="45"/>
-      <c r="Z78" s="45"/>
-      <c r="AA78" s="45"/>
-      <c r="AB78" s="45"/>
-      <c r="AC78" s="45"/>
-      <c r="AD78" s="45"/>
-      <c r="AE78" s="45"/>
-      <c r="AF78" s="45"/>
-      <c r="AG78" s="45"/>
-      <c r="AH78" s="45"/>
-      <c r="AI78" s="45"/>
-      <c r="AJ78" s="45"/>
-      <c r="AK78" s="45"/>
-      <c r="AL78" s="45"/>
-    </row>
-    <row r="79" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="48"/>
-      <c r="B79" s="45"/>
-      <c r="C79" s="45"/>
-      <c r="D79" s="45"/>
-      <c r="E79" s="45"/>
-      <c r="F79" s="45"/>
-      <c r="G79" s="45"/>
-      <c r="H79" s="45"/>
-      <c r="I79" s="45"/>
-      <c r="J79" s="45"/>
-      <c r="K79" s="45"/>
-      <c r="L79" s="45"/>
-      <c r="M79" s="45"/>
-      <c r="N79" s="45"/>
-      <c r="O79" s="45"/>
-      <c r="P79" s="45"/>
-      <c r="Q79" s="45"/>
-      <c r="R79" s="45"/>
-      <c r="S79" s="45"/>
-      <c r="T79" s="45"/>
-      <c r="U79" s="45"/>
-      <c r="V79" s="45"/>
-      <c r="W79" s="45"/>
-      <c r="X79" s="45"/>
-      <c r="Y79" s="45"/>
-      <c r="Z79" s="45"/>
-      <c r="AA79" s="45"/>
-      <c r="AB79" s="45"/>
-      <c r="AC79" s="45"/>
-      <c r="AD79" s="45"/>
-      <c r="AE79" s="45"/>
-      <c r="AF79" s="45"/>
-      <c r="AG79" s="45"/>
-      <c r="AH79" s="45"/>
-      <c r="AI79" s="45"/>
-      <c r="AJ79" s="45"/>
-      <c r="AK79" s="45"/>
-      <c r="AL79" s="45"/>
-    </row>
-    <row r="80" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="48"/>
-      <c r="B80" s="45"/>
-      <c r="C80" s="45"/>
-      <c r="D80" s="45"/>
-      <c r="E80" s="45"/>
-      <c r="F80" s="45"/>
-      <c r="G80" s="45"/>
-      <c r="H80" s="45"/>
-      <c r="I80" s="45"/>
-      <c r="J80" s="45"/>
-      <c r="K80" s="45"/>
-      <c r="L80" s="45"/>
-      <c r="M80" s="45"/>
-      <c r="N80" s="45"/>
-      <c r="O80" s="45"/>
-      <c r="P80" s="45"/>
-      <c r="Q80" s="45"/>
-      <c r="R80" s="45"/>
-      <c r="S80" s="45"/>
-      <c r="T80" s="45"/>
-      <c r="U80" s="45"/>
-      <c r="V80" s="45"/>
-      <c r="W80" s="45"/>
-      <c r="X80" s="45"/>
-      <c r="Y80" s="45"/>
-      <c r="Z80" s="45"/>
-      <c r="AA80" s="45"/>
-      <c r="AB80" s="45"/>
-      <c r="AC80" s="45"/>
-      <c r="AD80" s="45"/>
-      <c r="AE80" s="45"/>
-      <c r="AF80" s="45"/>
-      <c r="AG80" s="45"/>
-      <c r="AH80" s="45"/>
-      <c r="AI80" s="45"/>
-      <c r="AJ80" s="45"/>
-      <c r="AK80" s="45"/>
-      <c r="AL80" s="45"/>
-    </row>
-    <row r="87" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="48"/>
-      <c r="B87" s="45"/>
-      <c r="C87" s="45"/>
-      <c r="D87" s="45"/>
-      <c r="E87" s="45"/>
-      <c r="F87" s="45"/>
-      <c r="G87" s="45"/>
-      <c r="H87" s="45"/>
-      <c r="I87" s="45"/>
-      <c r="J87" s="45"/>
-      <c r="K87" s="45"/>
-      <c r="L87" s="45"/>
-      <c r="M87" s="45"/>
-      <c r="N87" s="45"/>
-      <c r="O87" s="45"/>
-      <c r="P87" s="45"/>
-      <c r="Q87" s="45"/>
-      <c r="R87" s="45"/>
-      <c r="S87" s="45"/>
-      <c r="T87" s="45"/>
-      <c r="U87" s="45"/>
-      <c r="V87" s="45"/>
-      <c r="W87" s="45"/>
-      <c r="X87" s="45"/>
-      <c r="Y87" s="45"/>
-      <c r="Z87" s="45"/>
-      <c r="AA87" s="45"/>
-      <c r="AB87" s="45"/>
-      <c r="AC87" s="45"/>
-      <c r="AD87" s="45"/>
-      <c r="AE87" s="45"/>
-      <c r="AF87" s="45"/>
-      <c r="AG87" s="45"/>
-      <c r="AH87" s="45"/>
-      <c r="AI87" s="45"/>
-      <c r="AJ87" s="45"/>
-      <c r="AK87" s="45"/>
-      <c r="AL87" s="45"/>
-    </row>
-    <row r="88" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="48"/>
-      <c r="B88" s="45"/>
-      <c r="C88" s="45"/>
-      <c r="D88" s="45"/>
-      <c r="E88" s="45"/>
-      <c r="F88" s="45"/>
-      <c r="G88" s="45"/>
-      <c r="H88" s="45"/>
-      <c r="I88" s="45"/>
-      <c r="J88" s="45"/>
-      <c r="K88" s="45"/>
-      <c r="L88" s="45"/>
-      <c r="M88" s="45"/>
-      <c r="N88" s="45"/>
-      <c r="O88" s="45"/>
-      <c r="P88" s="45"/>
-      <c r="Q88" s="45"/>
-      <c r="R88" s="45"/>
-      <c r="S88" s="45"/>
-      <c r="T88" s="45"/>
-      <c r="U88" s="45"/>
-      <c r="V88" s="45"/>
-      <c r="W88" s="45"/>
-      <c r="X88" s="45"/>
-      <c r="Y88" s="45"/>
-      <c r="Z88" s="45"/>
-      <c r="AA88" s="45"/>
-      <c r="AB88" s="45"/>
-      <c r="AC88" s="45"/>
-      <c r="AD88" s="45"/>
-      <c r="AE88" s="45"/>
-      <c r="AF88" s="45"/>
-      <c r="AG88" s="45"/>
-      <c r="AH88" s="45"/>
-      <c r="AI88" s="45"/>
-      <c r="AJ88" s="45"/>
-      <c r="AK88" s="45"/>
-      <c r="AL88" s="45"/>
+    <row r="78" spans="1:38" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="47"/>
+      <c r="B78" s="44"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="44"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="44"/>
+      <c r="G78" s="44"/>
+      <c r="H78" s="44"/>
+      <c r="I78" s="44"/>
+      <c r="J78" s="44"/>
+      <c r="K78" s="44"/>
+      <c r="L78" s="44"/>
+      <c r="M78" s="44"/>
+      <c r="N78" s="44"/>
+      <c r="O78" s="44"/>
+      <c r="P78" s="44"/>
+      <c r="Q78" s="44"/>
+      <c r="R78" s="44"/>
+      <c r="S78" s="44"/>
+      <c r="T78" s="44"/>
+      <c r="U78" s="44"/>
+      <c r="V78" s="44"/>
+      <c r="W78" s="44"/>
+      <c r="X78" s="44"/>
+      <c r="Y78" s="44"/>
+      <c r="Z78" s="44"/>
+      <c r="AA78" s="44"/>
+      <c r="AB78" s="44"/>
+      <c r="AC78" s="44"/>
+      <c r="AD78" s="44"/>
+      <c r="AE78" s="44"/>
+      <c r="AF78" s="44"/>
+      <c r="AG78" s="44"/>
+      <c r="AH78" s="44"/>
+      <c r="AI78" s="44"/>
+      <c r="AJ78" s="44"/>
+      <c r="AK78" s="44"/>
+      <c r="AL78" s="44"/>
+    </row>
+    <row r="79" spans="1:38" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="47"/>
+      <c r="B79" s="44"/>
+      <c r="C79" s="44"/>
+      <c r="D79" s="44"/>
+      <c r="E79" s="44"/>
+      <c r="F79" s="44"/>
+      <c r="G79" s="44"/>
+      <c r="H79" s="44"/>
+      <c r="I79" s="44"/>
+      <c r="J79" s="44"/>
+      <c r="K79" s="44"/>
+      <c r="L79" s="44"/>
+      <c r="M79" s="44"/>
+      <c r="N79" s="44"/>
+      <c r="O79" s="44"/>
+      <c r="P79" s="44"/>
+      <c r="Q79" s="44"/>
+      <c r="R79" s="44"/>
+      <c r="S79" s="44"/>
+      <c r="T79" s="44"/>
+      <c r="U79" s="44"/>
+      <c r="V79" s="44"/>
+      <c r="W79" s="44"/>
+      <c r="X79" s="44"/>
+      <c r="Y79" s="44"/>
+      <c r="Z79" s="44"/>
+      <c r="AA79" s="44"/>
+      <c r="AB79" s="44"/>
+      <c r="AC79" s="44"/>
+      <c r="AD79" s="44"/>
+      <c r="AE79" s="44"/>
+      <c r="AF79" s="44"/>
+      <c r="AG79" s="44"/>
+      <c r="AH79" s="44"/>
+      <c r="AI79" s="44"/>
+      <c r="AJ79" s="44"/>
+      <c r="AK79" s="44"/>
+      <c r="AL79" s="44"/>
+    </row>
+    <row r="80" spans="1:38" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="47"/>
+      <c r="B80" s="44"/>
+      <c r="C80" s="44"/>
+      <c r="D80" s="44"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="44"/>
+      <c r="G80" s="44"/>
+      <c r="H80" s="44"/>
+      <c r="I80" s="44"/>
+      <c r="J80" s="44"/>
+      <c r="K80" s="44"/>
+      <c r="L80" s="44"/>
+      <c r="M80" s="44"/>
+      <c r="N80" s="44"/>
+      <c r="O80" s="44"/>
+      <c r="P80" s="44"/>
+      <c r="Q80" s="44"/>
+      <c r="R80" s="44"/>
+      <c r="S80" s="44"/>
+      <c r="T80" s="44"/>
+      <c r="U80" s="44"/>
+      <c r="V80" s="44"/>
+      <c r="W80" s="44"/>
+      <c r="X80" s="44"/>
+      <c r="Y80" s="44"/>
+      <c r="Z80" s="44"/>
+      <c r="AA80" s="44"/>
+      <c r="AB80" s="44"/>
+      <c r="AC80" s="44"/>
+      <c r="AD80" s="44"/>
+      <c r="AE80" s="44"/>
+      <c r="AF80" s="44"/>
+      <c r="AG80" s="44"/>
+      <c r="AH80" s="44"/>
+      <c r="AI80" s="44"/>
+      <c r="AJ80" s="44"/>
+      <c r="AK80" s="44"/>
+      <c r="AL80" s="44"/>
+    </row>
+    <row r="87" spans="1:38" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="47"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="44"/>
+      <c r="E87" s="44"/>
+      <c r="F87" s="44"/>
+      <c r="G87" s="44"/>
+      <c r="H87" s="44"/>
+      <c r="I87" s="44"/>
+      <c r="J87" s="44"/>
+      <c r="K87" s="44"/>
+      <c r="L87" s="44"/>
+      <c r="M87" s="44"/>
+      <c r="N87" s="44"/>
+      <c r="O87" s="44"/>
+      <c r="P87" s="44"/>
+      <c r="Q87" s="44"/>
+      <c r="R87" s="44"/>
+      <c r="S87" s="44"/>
+      <c r="T87" s="44"/>
+      <c r="U87" s="44"/>
+      <c r="V87" s="44"/>
+      <c r="W87" s="44"/>
+      <c r="X87" s="44"/>
+      <c r="Y87" s="44"/>
+      <c r="Z87" s="44"/>
+      <c r="AA87" s="44"/>
+      <c r="AB87" s="44"/>
+      <c r="AC87" s="44"/>
+      <c r="AD87" s="44"/>
+      <c r="AE87" s="44"/>
+      <c r="AF87" s="44"/>
+      <c r="AG87" s="44"/>
+      <c r="AH87" s="44"/>
+      <c r="AI87" s="44"/>
+      <c r="AJ87" s="44"/>
+      <c r="AK87" s="44"/>
+      <c r="AL87" s="44"/>
+    </row>
+    <row r="88" spans="1:38" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="47"/>
+      <c r="B88" s="44"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="44"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="44"/>
+      <c r="H88" s="44"/>
+      <c r="I88" s="44"/>
+      <c r="J88" s="44"/>
+      <c r="K88" s="44"/>
+      <c r="L88" s="44"/>
+      <c r="M88" s="44"/>
+      <c r="N88" s="44"/>
+      <c r="O88" s="44"/>
+      <c r="P88" s="44"/>
+      <c r="Q88" s="44"/>
+      <c r="R88" s="44"/>
+      <c r="S88" s="44"/>
+      <c r="T88" s="44"/>
+      <c r="U88" s="44"/>
+      <c r="V88" s="44"/>
+      <c r="W88" s="44"/>
+      <c r="X88" s="44"/>
+      <c r="Y88" s="44"/>
+      <c r="Z88" s="44"/>
+      <c r="AA88" s="44"/>
+      <c r="AB88" s="44"/>
+      <c r="AC88" s="44"/>
+      <c r="AD88" s="44"/>
+      <c r="AE88" s="44"/>
+      <c r="AF88" s="44"/>
+      <c r="AG88" s="44"/>
+      <c r="AH88" s="44"/>
+      <c r="AI88" s="44"/>
+      <c r="AJ88" s="44"/>
+      <c r="AK88" s="44"/>
+      <c r="AL88" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6424,10 +6422,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>2</v>
       </c>
     </row>
@@ -6448,7 +6446,7 @@
       <c r="B4" s="8">
         <v>8512</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="25"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
@@ -6479,8 +6477,8 @@
       <c r="A10" s="12">
         <v>1953</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
@@ -6991,13 +6989,13 @@
       <c r="B76" s="8">
         <v>11481</v>
       </c>
-      <c r="C76" s="28"/>
+      <c r="C76" s="27"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
         <v>2020</v>
       </c>
-      <c r="B77" s="27">
+      <c r="B77" s="26">
         <v>11493</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revised version for publication
</commit_message>
<xml_diff>
--- a/RawData/BE_RawData_VPython.xlsx
+++ b/RawData/BE_RawData_VPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\01_MFA_GlassIndustry\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D91D7C6-7079-4793-AAFF-A2A339B98735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF3AEE7-CEC0-473C-BA3E-0E22B6E30022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="600" windowWidth="16665" windowHeight="15600" activeTab="4" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="19" r:id="rId1"/>
@@ -2667,7 +2667,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2770,7 +2770,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3141,16 +3140,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025F8ED2-37F9-40BE-8E6A-7FBA957A3175}">
   <dimension ref="A2:D23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="118.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="27" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81" style="32" customWidth="1"/>
-    <col min="4" max="4" width="86.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.140625" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3164,7 +3161,7 @@
       <c r="C3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="33"/>
+      <c r="D3" s="34"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="36" t="s">
@@ -3178,10 +3175,10 @@
       <c r="B7" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="53" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3194,7 +3191,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" s="38"/>
+      <c r="D10" s="53"/>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="36" t="s">
@@ -3214,13 +3211,13 @@
       <c r="C13" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="53" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
+      <c r="D14" s="53"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="36" t="s">
@@ -3229,11 +3226,11 @@
       <c r="C15" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="38"/>
+      <c r="D15" s="53"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" s="37"/>
-      <c r="D16" s="38"/>
+      <c r="D16" s="53"/>
     </row>
     <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="36" t="s">
@@ -3242,11 +3239,11 @@
       <c r="C17" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="38"/>
+      <c r="D17" s="53"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
+      <c r="D18" s="53"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="36" t="s">
@@ -3255,7 +3252,7 @@
       <c r="C19" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="53" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3266,13 +3263,13 @@
       <c r="C21" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="53" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C22" s="37"/>
-      <c r="D22" s="38"/>
+      <c r="D22" s="53"/>
     </row>
     <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="36" t="s">
@@ -3281,7 +3278,7 @@
       <c r="C23" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="38"/>
+      <c r="D23" s="53"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3322,7 +3319,7 @@
       <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="50" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3331,7 +3328,7 @@
         <v>1945</v>
       </c>
       <c r="B2" s="9"/>
-      <c r="C2" s="55">
+      <c r="C2" s="54">
         <v>0.9</v>
       </c>
     </row>
@@ -3366,7 +3363,7 @@
       <c r="B7" s="9">
         <v>206.25</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="51">
         <v>0.9</v>
       </c>
     </row>
@@ -5500,905 +5497,905 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7426F8F2-947A-4C47-BA81-FD7398DE30D5}">
   <dimension ref="A1:AL88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="15.140625" style="44" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="44"/>
+    <col min="1" max="1" width="8" style="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.140625" style="43" customWidth="1"/>
+    <col min="5" max="16384" width="10.7109375" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:5" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="42">
+      <c r="A2" s="41">
         <v>1945</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="42">
+      <c r="A3" s="41">
         <v>1946</v>
       </c>
-      <c r="B3" s="43"/>
+      <c r="B3" s="42"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="42">
+      <c r="A4" s="41">
         <v>1947</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="42">
+      <c r="A5" s="41">
         <v>1948</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="42">
+      <c r="A6" s="41">
         <v>1949</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="42">
+      <c r="A7" s="41">
         <v>1950</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="42">
         <v>30.98</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="42">
         <v>0.73</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="42">
         <v>0</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="42">
         <f>SUM(B7:D7)</f>
         <v>31.71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="42">
+      <c r="A8" s="41">
         <v>1951</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="42">
+      <c r="A9" s="41">
         <v>1952</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="42">
+      <c r="A10" s="41">
         <v>1953</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="42">
+      <c r="A11" s="41">
         <v>1954</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="42">
+      <c r="A12" s="41">
         <v>1955</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="42">
+      <c r="A13" s="41">
         <v>1956</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="42">
+      <c r="A14" s="41">
         <v>1957</v>
       </c>
+      <c r="D14" s="44"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="42">
+      <c r="A15" s="41">
         <v>1958</v>
       </c>
-      <c r="B15" s="45"/>
+      <c r="B15" s="44"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="42">
+      <c r="A16" s="41">
         <v>1959</v>
       </c>
-      <c r="B16" s="45"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="42">
+      <c r="A17" s="41">
         <v>1960</v>
       </c>
-      <c r="B17" s="46">
-        <f>0.8*E17</f>
-        <v>16.8</v>
-      </c>
-      <c r="C17" s="46">
-        <f>0.047*E17</f>
-        <v>0.98699999999999999</v>
-      </c>
-      <c r="D17" s="46">
-        <f>0.125*E17</f>
-        <v>2.625</v>
-      </c>
-      <c r="E17" s="49">
+      <c r="B17" s="45">
+        <f>0.9*E17</f>
+        <v>18.900000000000002</v>
+      </c>
+      <c r="C17" s="45">
+        <f>0.04*E17</f>
+        <v>0.84</v>
+      </c>
+      <c r="D17" s="45">
+        <f>0.06*E17</f>
+        <v>1.26</v>
+      </c>
+      <c r="E17" s="48">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="42">
+      <c r="A18" s="41">
         <v>1961</v>
       </c>
-      <c r="E18" s="49"/>
+      <c r="E18" s="48"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="42">
+      <c r="A19" s="41">
         <v>1962</v>
       </c>
-      <c r="E19" s="49"/>
+      <c r="E19" s="48"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="42">
+      <c r="A20" s="41">
         <v>1963</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="E20" s="49"/>
+      <c r="B20" s="44"/>
+      <c r="E20" s="48"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="42">
+      <c r="A21" s="41">
         <v>1964</v>
       </c>
-      <c r="E21" s="49"/>
+      <c r="E21" s="48"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="42">
+      <c r="A22" s="41">
         <v>1965</v>
       </c>
-      <c r="B22" s="46">
+      <c r="B22" s="45">
         <f>0.79*E22</f>
         <v>16.6295</v>
       </c>
-      <c r="C22" s="46">
+      <c r="C22" s="45">
         <f>0.055*E22</f>
         <v>1.1577500000000001</v>
       </c>
-      <c r="D22" s="46">
+      <c r="D22" s="45">
         <f>0.12*E22</f>
         <v>2.5259999999999998</v>
       </c>
-      <c r="E22" s="49">
+      <c r="E22" s="48">
         <v>21.05</v>
       </c>
-      <c r="J22" s="50"/>
+      <c r="J22" s="49"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="42">
+      <c r="A23" s="41">
         <v>1966</v>
       </c>
-      <c r="E23" s="49"/>
+      <c r="E23" s="48"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="42">
+      <c r="A24" s="41">
         <v>1967</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="49"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="48"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="42">
+      <c r="A25" s="41">
         <v>1968</v>
       </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="49"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="48"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="42">
+      <c r="A26" s="41">
         <v>1969</v>
       </c>
-      <c r="E26" s="49"/>
+      <c r="E26" s="48"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="42">
+      <c r="A27" s="41">
         <v>1970</v>
       </c>
-      <c r="B27" s="45">
+      <c r="B27" s="44">
         <f>0.79*E27</f>
         <v>15.721</v>
       </c>
-      <c r="C27" s="45">
+      <c r="C27" s="44">
         <f>0.04*E27</f>
         <v>0.79599999999999993</v>
       </c>
-      <c r="D27" s="45">
+      <c r="D27" s="44">
         <f>0.17*E27</f>
         <v>3.383</v>
       </c>
-      <c r="E27" s="49">
+      <c r="E27" s="48">
         <v>19.899999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="42">
+      <c r="A28" s="41">
         <v>1971</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="49"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="48"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="42">
+      <c r="A29" s="41">
         <v>1972</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="49"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="48"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="42">
+      <c r="A30" s="41">
         <v>1973</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="49"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="48"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="42">
+      <c r="A31" s="41">
         <v>1974</v>
       </c>
-      <c r="E31" s="49"/>
+      <c r="E31" s="48"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="42">
+      <c r="A32" s="41">
         <v>1975</v>
       </c>
-      <c r="B32" s="45">
+      <c r="B32" s="44">
         <f>0.77*E32</f>
         <v>13.636700000000001</v>
       </c>
-      <c r="C32" s="45">
+      <c r="C32" s="44">
         <f>0.04*E32</f>
         <v>0.70840000000000003</v>
       </c>
-      <c r="D32" s="45">
+      <c r="D32" s="44">
         <f>0.18*E32</f>
         <v>3.1878000000000002</v>
       </c>
-      <c r="E32" s="49">
+      <c r="E32" s="48">
         <v>17.71</v>
       </c>
-      <c r="J32" s="50"/>
+      <c r="J32" s="49"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="42">
+      <c r="A33" s="41">
         <v>1976</v>
       </c>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="49"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="48"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="42">
+      <c r="A34" s="41">
         <v>1977</v>
       </c>
-      <c r="B34" s="45"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="49"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="48"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="42">
+      <c r="A35" s="41">
         <v>1978</v>
       </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="49"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="48"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="42">
+      <c r="A36" s="41">
         <v>1979</v>
       </c>
-      <c r="E36" s="49"/>
+      <c r="E36" s="48"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="42">
+      <c r="A37" s="41">
         <v>1980</v>
       </c>
-      <c r="B37" s="45">
+      <c r="B37" s="44">
         <f>0.68*E37</f>
         <v>10.376800000000001</v>
       </c>
-      <c r="C37" s="45">
+      <c r="C37" s="44">
         <f>0.04*E37</f>
         <v>0.61040000000000005</v>
       </c>
-      <c r="D37" s="45">
+      <c r="D37" s="44">
         <f>0.3*E37</f>
         <v>4.5779999999999994</v>
       </c>
-      <c r="E37" s="49">
+      <c r="E37" s="48">
         <v>15.26</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="42">
+      <c r="A38" s="41">
         <v>1981</v>
       </c>
-      <c r="E38" s="49"/>
+      <c r="E38" s="48"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="42">
+      <c r="A39" s="41">
         <v>1982</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="48"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="42">
+      <c r="A40" s="41">
         <v>1983</v>
       </c>
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="49"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="48"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="42">
+      <c r="A41" s="41">
         <v>1984</v>
       </c>
-      <c r="E41" s="49"/>
-      <c r="J41" s="50"/>
+      <c r="E41" s="48"/>
+      <c r="J41" s="49"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="42">
+      <c r="A42" s="41">
         <v>1985</v>
       </c>
-      <c r="B42" s="45">
+      <c r="B42" s="44">
         <f>0.65*E42</f>
         <v>8.918000000000001</v>
       </c>
-      <c r="C42" s="45">
+      <c r="C42" s="44">
         <f>0.04*E42</f>
         <v>0.54880000000000007</v>
       </c>
-      <c r="D42" s="45">
+      <c r="D42" s="44">
         <f>0.3*E42</f>
         <v>4.1159999999999997</v>
       </c>
-      <c r="E42" s="49">
+      <c r="E42" s="48">
         <v>13.72</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="42">
+      <c r="A43" s="41">
         <v>1986</v>
       </c>
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="49"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="48"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="42">
+      <c r="A44" s="41">
         <v>1987</v>
       </c>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="49"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="48"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="42">
+      <c r="A45" s="41">
         <v>1988</v>
       </c>
-      <c r="B45" s="45">
+      <c r="B45" s="44">
         <f>0.65*E45</f>
         <v>8.1640000000000015</v>
       </c>
-      <c r="C45" s="45">
+      <c r="C45" s="44">
         <f>0.04*E45</f>
         <v>0.50240000000000007</v>
       </c>
-      <c r="D45" s="45">
+      <c r="D45" s="44">
         <f>0.3*E45</f>
         <v>3.7679999999999998</v>
       </c>
-      <c r="E45" s="49">
+      <c r="E45" s="48">
         <v>12.56</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="42">
+      <c r="A46" s="41">
         <v>1989</v>
       </c>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="45"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="44"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="42">
+      <c r="A47" s="41">
         <v>1990</v>
       </c>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="45"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="44"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="42">
+      <c r="A48" s="41">
         <v>1991</v>
       </c>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="45"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="44"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="42">
+      <c r="A49" s="41">
         <v>1992</v>
       </c>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="42">
+      <c r="A50" s="41">
         <v>1993</v>
       </c>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="42">
+      <c r="A51" s="41">
         <v>1994</v>
       </c>
-      <c r="B51" s="43"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
+      <c r="B51" s="42"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="42">
+      <c r="A52" s="41">
         <v>1995</v>
       </c>
-      <c r="B52" s="45">
+      <c r="B52" s="44">
         <v>5.01</v>
       </c>
-      <c r="C52" s="45">
+      <c r="C52" s="44">
         <v>1.48</v>
       </c>
-      <c r="D52" s="45">
+      <c r="D52" s="44">
         <v>4.8</v>
       </c>
-      <c r="E52" s="45">
+      <c r="E52" s="44">
         <v>11.3</v>
       </c>
-      <c r="F52" s="45"/>
+      <c r="F52" s="44"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="42">
+      <c r="A53" s="41">
         <v>1996</v>
       </c>
-      <c r="B53" s="45"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="45"/>
-      <c r="F53" s="45"/>
+      <c r="B53" s="44"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="42">
+      <c r="A54" s="41">
         <v>1997</v>
       </c>
-      <c r="B54" s="45"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="45"/>
-      <c r="F54" s="45"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="42">
+      <c r="A55" s="41">
         <v>1998</v>
       </c>
-      <c r="B55" s="45"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="44"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="42">
+      <c r="A56" s="41">
         <v>1999</v>
       </c>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="42">
+      <c r="A57" s="41">
         <v>2000</v>
       </c>
-      <c r="F57" s="45"/>
+      <c r="F57" s="44"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="42">
+      <c r="A58" s="41">
         <v>2001</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="42">
+      <c r="A59" s="41">
         <v>2002</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="42">
+      <c r="A60" s="41">
         <v>2003</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="42">
+      <c r="A61" s="41">
         <v>2004</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="42">
+      <c r="A62" s="41">
         <v>2005</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="42">
+      <c r="A63" s="41">
         <v>2006</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="42">
+      <c r="A64" s="41">
         <v>2007</v>
       </c>
-      <c r="B64" s="45"/>
-      <c r="C64" s="45"/>
-      <c r="D64" s="45"/>
-      <c r="E64" s="45"/>
+      <c r="B64" s="44"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
     </row>
     <row r="65" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A65" s="42">
+      <c r="A65" s="41">
         <v>2008</v>
       </c>
     </row>
     <row r="66" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A66" s="42">
+      <c r="A66" s="41">
         <v>2009</v>
       </c>
-      <c r="B66" s="45"/>
-      <c r="C66" s="45"/>
-      <c r="D66" s="45"/>
-      <c r="E66" s="46"/>
+      <c r="B66" s="44"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="45"/>
     </row>
     <row r="67" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A67" s="42">
+      <c r="A67" s="41">
         <v>2010</v>
       </c>
-      <c r="B67" s="45">
+      <c r="B67" s="44">
         <v>2.1</v>
       </c>
-      <c r="C67" s="45">
+      <c r="C67" s="44">
         <v>0.9</v>
       </c>
-      <c r="D67" s="45">
+      <c r="D67" s="44">
         <v>6.1</v>
       </c>
-      <c r="E67" s="43">
+      <c r="E67" s="42">
         <v>9.1</v>
       </c>
     </row>
     <row r="68" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A68" s="42">
+      <c r="A68" s="41">
         <v>2011</v>
       </c>
     </row>
     <row r="69" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A69" s="42">
+      <c r="A69" s="41">
         <v>2012</v>
       </c>
-      <c r="B69" s="45"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="45"/>
+      <c r="B69" s="44"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="44"/>
     </row>
     <row r="70" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A70" s="42">
+      <c r="A70" s="41">
         <v>2013</v>
       </c>
-      <c r="B70" s="45"/>
-      <c r="C70" s="45"/>
-      <c r="D70" s="45"/>
+      <c r="B70" s="44"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="44"/>
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A71" s="42">
+      <c r="A71" s="41">
         <v>2014</v>
       </c>
-      <c r="B71" s="45"/>
-      <c r="C71" s="45"/>
-      <c r="D71" s="45"/>
+      <c r="B71" s="44"/>
+      <c r="C71" s="44"/>
+      <c r="D71" s="44"/>
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A72" s="42">
+      <c r="A72" s="41">
         <v>2015</v>
       </c>
-      <c r="B72" s="45"/>
-      <c r="C72" s="45"/>
-      <c r="D72" s="45"/>
+      <c r="B72" s="44"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="44"/>
     </row>
     <row r="73" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A73" s="42">
+      <c r="A73" s="41">
         <v>2016</v>
       </c>
-      <c r="B73" s="45"/>
-      <c r="C73" s="45"/>
-      <c r="D73" s="45"/>
+      <c r="B73" s="44"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="44"/>
     </row>
     <row r="74" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A74" s="42">
+      <c r="A74" s="41">
         <v>2017</v>
       </c>
     </row>
     <row r="75" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A75" s="42">
+      <c r="A75" s="41">
         <v>2018</v>
       </c>
     </row>
     <row r="76" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A76" s="42">
+      <c r="A76" s="41">
         <v>2019</v>
       </c>
-      <c r="B76" s="45">
+      <c r="B76" s="44">
         <v>2.1</v>
       </c>
-      <c r="C76" s="45">
+      <c r="C76" s="44">
         <v>0.9</v>
       </c>
-      <c r="D76" s="45">
+      <c r="D76" s="44">
         <v>6.1</v>
       </c>
-      <c r="E76" s="43">
+      <c r="E76" s="42">
         <v>9.1</v>
       </c>
     </row>
     <row r="77" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A77" s="42">
+      <c r="A77" s="41">
         <v>2020</v>
       </c>
     </row>
-    <row r="78" spans="1:38" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="47"/>
-      <c r="B78" s="44"/>
-      <c r="C78" s="44"/>
-      <c r="D78" s="44"/>
-      <c r="E78" s="44"/>
-      <c r="F78" s="44"/>
-      <c r="G78" s="44"/>
-      <c r="H78" s="44"/>
-      <c r="I78" s="44"/>
-      <c r="J78" s="44"/>
-      <c r="K78" s="44"/>
-      <c r="L78" s="44"/>
-      <c r="M78" s="44"/>
-      <c r="N78" s="44"/>
-      <c r="O78" s="44"/>
-      <c r="P78" s="44"/>
-      <c r="Q78" s="44"/>
-      <c r="R78" s="44"/>
-      <c r="S78" s="44"/>
-      <c r="T78" s="44"/>
-      <c r="U78" s="44"/>
-      <c r="V78" s="44"/>
-      <c r="W78" s="44"/>
-      <c r="X78" s="44"/>
-      <c r="Y78" s="44"/>
-      <c r="Z78" s="44"/>
-      <c r="AA78" s="44"/>
-      <c r="AB78" s="44"/>
-      <c r="AC78" s="44"/>
-      <c r="AD78" s="44"/>
-      <c r="AE78" s="44"/>
-      <c r="AF78" s="44"/>
-      <c r="AG78" s="44"/>
-      <c r="AH78" s="44"/>
-      <c r="AI78" s="44"/>
-      <c r="AJ78" s="44"/>
-      <c r="AK78" s="44"/>
-      <c r="AL78" s="44"/>
-    </row>
-    <row r="79" spans="1:38" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="47"/>
-      <c r="B79" s="44"/>
-      <c r="C79" s="44"/>
-      <c r="D79" s="44"/>
-      <c r="E79" s="44"/>
-      <c r="F79" s="44"/>
-      <c r="G79" s="44"/>
-      <c r="H79" s="44"/>
-      <c r="I79" s="44"/>
-      <c r="J79" s="44"/>
-      <c r="K79" s="44"/>
-      <c r="L79" s="44"/>
-      <c r="M79" s="44"/>
-      <c r="N79" s="44"/>
-      <c r="O79" s="44"/>
-      <c r="P79" s="44"/>
-      <c r="Q79" s="44"/>
-      <c r="R79" s="44"/>
-      <c r="S79" s="44"/>
-      <c r="T79" s="44"/>
-      <c r="U79" s="44"/>
-      <c r="V79" s="44"/>
-      <c r="W79" s="44"/>
-      <c r="X79" s="44"/>
-      <c r="Y79" s="44"/>
-      <c r="Z79" s="44"/>
-      <c r="AA79" s="44"/>
-      <c r="AB79" s="44"/>
-      <c r="AC79" s="44"/>
-      <c r="AD79" s="44"/>
-      <c r="AE79" s="44"/>
-      <c r="AF79" s="44"/>
-      <c r="AG79" s="44"/>
-      <c r="AH79" s="44"/>
-      <c r="AI79" s="44"/>
-      <c r="AJ79" s="44"/>
-      <c r="AK79" s="44"/>
-      <c r="AL79" s="44"/>
-    </row>
-    <row r="80" spans="1:38" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="47"/>
-      <c r="B80" s="44"/>
-      <c r="C80" s="44"/>
-      <c r="D80" s="44"/>
-      <c r="E80" s="44"/>
-      <c r="F80" s="44"/>
-      <c r="G80" s="44"/>
-      <c r="H80" s="44"/>
-      <c r="I80" s="44"/>
-      <c r="J80" s="44"/>
-      <c r="K80" s="44"/>
-      <c r="L80" s="44"/>
-      <c r="M80" s="44"/>
-      <c r="N80" s="44"/>
-      <c r="O80" s="44"/>
-      <c r="P80" s="44"/>
-      <c r="Q80" s="44"/>
-      <c r="R80" s="44"/>
-      <c r="S80" s="44"/>
-      <c r="T80" s="44"/>
-      <c r="U80" s="44"/>
-      <c r="V80" s="44"/>
-      <c r="W80" s="44"/>
-      <c r="X80" s="44"/>
-      <c r="Y80" s="44"/>
-      <c r="Z80" s="44"/>
-      <c r="AA80" s="44"/>
-      <c r="AB80" s="44"/>
-      <c r="AC80" s="44"/>
-      <c r="AD80" s="44"/>
-      <c r="AE80" s="44"/>
-      <c r="AF80" s="44"/>
-      <c r="AG80" s="44"/>
-      <c r="AH80" s="44"/>
-      <c r="AI80" s="44"/>
-      <c r="AJ80" s="44"/>
-      <c r="AK80" s="44"/>
-      <c r="AL80" s="44"/>
-    </row>
-    <row r="87" spans="1:38" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="47"/>
-      <c r="B87" s="44"/>
-      <c r="C87" s="44"/>
-      <c r="D87" s="44"/>
-      <c r="E87" s="44"/>
-      <c r="F87" s="44"/>
-      <c r="G87" s="44"/>
-      <c r="H87" s="44"/>
-      <c r="I87" s="44"/>
-      <c r="J87" s="44"/>
-      <c r="K87" s="44"/>
-      <c r="L87" s="44"/>
-      <c r="M87" s="44"/>
-      <c r="N87" s="44"/>
-      <c r="O87" s="44"/>
-      <c r="P87" s="44"/>
-      <c r="Q87" s="44"/>
-      <c r="R87" s="44"/>
-      <c r="S87" s="44"/>
-      <c r="T87" s="44"/>
-      <c r="U87" s="44"/>
-      <c r="V87" s="44"/>
-      <c r="W87" s="44"/>
-      <c r="X87" s="44"/>
-      <c r="Y87" s="44"/>
-      <c r="Z87" s="44"/>
-      <c r="AA87" s="44"/>
-      <c r="AB87" s="44"/>
-      <c r="AC87" s="44"/>
-      <c r="AD87" s="44"/>
-      <c r="AE87" s="44"/>
-      <c r="AF87" s="44"/>
-      <c r="AG87" s="44"/>
-      <c r="AH87" s="44"/>
-      <c r="AI87" s="44"/>
-      <c r="AJ87" s="44"/>
-      <c r="AK87" s="44"/>
-      <c r="AL87" s="44"/>
-    </row>
-    <row r="88" spans="1:38" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="47"/>
-      <c r="B88" s="44"/>
-      <c r="C88" s="44"/>
-      <c r="D88" s="44"/>
-      <c r="E88" s="44"/>
-      <c r="F88" s="44"/>
-      <c r="G88" s="44"/>
-      <c r="H88" s="44"/>
-      <c r="I88" s="44"/>
-      <c r="J88" s="44"/>
-      <c r="K88" s="44"/>
-      <c r="L88" s="44"/>
-      <c r="M88" s="44"/>
-      <c r="N88" s="44"/>
-      <c r="O88" s="44"/>
-      <c r="P88" s="44"/>
-      <c r="Q88" s="44"/>
-      <c r="R88" s="44"/>
-      <c r="S88" s="44"/>
-      <c r="T88" s="44"/>
-      <c r="U88" s="44"/>
-      <c r="V88" s="44"/>
-      <c r="W88" s="44"/>
-      <c r="X88" s="44"/>
-      <c r="Y88" s="44"/>
-      <c r="Z88" s="44"/>
-      <c r="AA88" s="44"/>
-      <c r="AB88" s="44"/>
-      <c r="AC88" s="44"/>
-      <c r="AD88" s="44"/>
-      <c r="AE88" s="44"/>
-      <c r="AF88" s="44"/>
-      <c r="AG88" s="44"/>
-      <c r="AH88" s="44"/>
-      <c r="AI88" s="44"/>
-      <c r="AJ88" s="44"/>
-      <c r="AK88" s="44"/>
-      <c r="AL88" s="44"/>
+    <row r="78" spans="1:38" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="46"/>
+      <c r="B78" s="43"/>
+      <c r="C78" s="43"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="43"/>
+      <c r="H78" s="43"/>
+      <c r="I78" s="43"/>
+      <c r="J78" s="43"/>
+      <c r="K78" s="43"/>
+      <c r="L78" s="43"/>
+      <c r="M78" s="43"/>
+      <c r="N78" s="43"/>
+      <c r="O78" s="43"/>
+      <c r="P78" s="43"/>
+      <c r="Q78" s="43"/>
+      <c r="R78" s="43"/>
+      <c r="S78" s="43"/>
+      <c r="T78" s="43"/>
+      <c r="U78" s="43"/>
+      <c r="V78" s="43"/>
+      <c r="W78" s="43"/>
+      <c r="X78" s="43"/>
+      <c r="Y78" s="43"/>
+      <c r="Z78" s="43"/>
+      <c r="AA78" s="43"/>
+      <c r="AB78" s="43"/>
+      <c r="AC78" s="43"/>
+      <c r="AD78" s="43"/>
+      <c r="AE78" s="43"/>
+      <c r="AF78" s="43"/>
+      <c r="AG78" s="43"/>
+      <c r="AH78" s="43"/>
+      <c r="AI78" s="43"/>
+      <c r="AJ78" s="43"/>
+      <c r="AK78" s="43"/>
+      <c r="AL78" s="43"/>
+    </row>
+    <row r="79" spans="1:38" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="46"/>
+      <c r="B79" s="43"/>
+      <c r="C79" s="43"/>
+      <c r="D79" s="43"/>
+      <c r="E79" s="43"/>
+      <c r="F79" s="43"/>
+      <c r="G79" s="43"/>
+      <c r="H79" s="43"/>
+      <c r="I79" s="43"/>
+      <c r="J79" s="43"/>
+      <c r="K79" s="43"/>
+      <c r="L79" s="43"/>
+      <c r="M79" s="43"/>
+      <c r="N79" s="43"/>
+      <c r="O79" s="43"/>
+      <c r="P79" s="43"/>
+      <c r="Q79" s="43"/>
+      <c r="R79" s="43"/>
+      <c r="S79" s="43"/>
+      <c r="T79" s="43"/>
+      <c r="U79" s="43"/>
+      <c r="V79" s="43"/>
+      <c r="W79" s="43"/>
+      <c r="X79" s="43"/>
+      <c r="Y79" s="43"/>
+      <c r="Z79" s="43"/>
+      <c r="AA79" s="43"/>
+      <c r="AB79" s="43"/>
+      <c r="AC79" s="43"/>
+      <c r="AD79" s="43"/>
+      <c r="AE79" s="43"/>
+      <c r="AF79" s="43"/>
+      <c r="AG79" s="43"/>
+      <c r="AH79" s="43"/>
+      <c r="AI79" s="43"/>
+      <c r="AJ79" s="43"/>
+      <c r="AK79" s="43"/>
+      <c r="AL79" s="43"/>
+    </row>
+    <row r="80" spans="1:38" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="46"/>
+      <c r="B80" s="43"/>
+      <c r="C80" s="43"/>
+      <c r="D80" s="43"/>
+      <c r="E80" s="43"/>
+      <c r="F80" s="43"/>
+      <c r="G80" s="43"/>
+      <c r="H80" s="43"/>
+      <c r="I80" s="43"/>
+      <c r="J80" s="43"/>
+      <c r="K80" s="43"/>
+      <c r="L80" s="43"/>
+      <c r="M80" s="43"/>
+      <c r="N80" s="43"/>
+      <c r="O80" s="43"/>
+      <c r="P80" s="43"/>
+      <c r="Q80" s="43"/>
+      <c r="R80" s="43"/>
+      <c r="S80" s="43"/>
+      <c r="T80" s="43"/>
+      <c r="U80" s="43"/>
+      <c r="V80" s="43"/>
+      <c r="W80" s="43"/>
+      <c r="X80" s="43"/>
+      <c r="Y80" s="43"/>
+      <c r="Z80" s="43"/>
+      <c r="AA80" s="43"/>
+      <c r="AB80" s="43"/>
+      <c r="AC80" s="43"/>
+      <c r="AD80" s="43"/>
+      <c r="AE80" s="43"/>
+      <c r="AF80" s="43"/>
+      <c r="AG80" s="43"/>
+      <c r="AH80" s="43"/>
+      <c r="AI80" s="43"/>
+      <c r="AJ80" s="43"/>
+      <c r="AK80" s="43"/>
+      <c r="AL80" s="43"/>
+    </row>
+    <row r="87" spans="1:38" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="46"/>
+      <c r="B87" s="43"/>
+      <c r="C87" s="43"/>
+      <c r="D87" s="43"/>
+      <c r="E87" s="43"/>
+      <c r="F87" s="43"/>
+      <c r="G87" s="43"/>
+      <c r="H87" s="43"/>
+      <c r="I87" s="43"/>
+      <c r="J87" s="43"/>
+      <c r="K87" s="43"/>
+      <c r="L87" s="43"/>
+      <c r="M87" s="43"/>
+      <c r="N87" s="43"/>
+      <c r="O87" s="43"/>
+      <c r="P87" s="43"/>
+      <c r="Q87" s="43"/>
+      <c r="R87" s="43"/>
+      <c r="S87" s="43"/>
+      <c r="T87" s="43"/>
+      <c r="U87" s="43"/>
+      <c r="V87" s="43"/>
+      <c r="W87" s="43"/>
+      <c r="X87" s="43"/>
+      <c r="Y87" s="43"/>
+      <c r="Z87" s="43"/>
+      <c r="AA87" s="43"/>
+      <c r="AB87" s="43"/>
+      <c r="AC87" s="43"/>
+      <c r="AD87" s="43"/>
+      <c r="AE87" s="43"/>
+      <c r="AF87" s="43"/>
+      <c r="AG87" s="43"/>
+      <c r="AH87" s="43"/>
+      <c r="AI87" s="43"/>
+      <c r="AJ87" s="43"/>
+      <c r="AK87" s="43"/>
+      <c r="AL87" s="43"/>
+    </row>
+    <row r="88" spans="1:38" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="46"/>
+      <c r="B88" s="43"/>
+      <c r="C88" s="43"/>
+      <c r="D88" s="43"/>
+      <c r="E88" s="43"/>
+      <c r="F88" s="43"/>
+      <c r="G88" s="43"/>
+      <c r="H88" s="43"/>
+      <c r="I88" s="43"/>
+      <c r="J88" s="43"/>
+      <c r="K88" s="43"/>
+      <c r="L88" s="43"/>
+      <c r="M88" s="43"/>
+      <c r="N88" s="43"/>
+      <c r="O88" s="43"/>
+      <c r="P88" s="43"/>
+      <c r="Q88" s="43"/>
+      <c r="R88" s="43"/>
+      <c r="S88" s="43"/>
+      <c r="T88" s="43"/>
+      <c r="U88" s="43"/>
+      <c r="V88" s="43"/>
+      <c r="W88" s="43"/>
+      <c r="X88" s="43"/>
+      <c r="Y88" s="43"/>
+      <c r="Z88" s="43"/>
+      <c r="AA88" s="43"/>
+      <c r="AB88" s="43"/>
+      <c r="AC88" s="43"/>
+      <c r="AD88" s="43"/>
+      <c r="AE88" s="43"/>
+      <c r="AF88" s="43"/>
+      <c r="AG88" s="43"/>
+      <c r="AH88" s="43"/>
+      <c r="AI88" s="43"/>
+      <c r="AJ88" s="43"/>
+      <c r="AK88" s="43"/>
+      <c r="AL88" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>